<commit_message>
Commit on 23.01.2019. Added new questions and answers in the .xslx file. Currently at 34th question.
</commit_message>
<xml_diff>
--- a/Exam Preparation/resources/70-480 Practice Exam Answers and Explanations.xlsx
+++ b/Exam Preparation/resources/70-480 Practice Exam Answers and Explanations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22264" windowHeight="12647"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="115">
   <si>
     <t>Question</t>
   </si>
@@ -156,12 +156,312 @@
   <si>
     <t>My answer is correct.Answer explanation:DOM event objects have a returnValue property that you can set to control the default behavior of an element when the event is raised.Whan you set this property to true you indicate that the default behavior of an element should occur.When you set this property to false you indicate that the default behavior should not occur.</t>
   </si>
+  <si>
+    <t>11.A Web page allows users to enter JSON encoded data into an input field named data.You need to validate data to ensure that it is JSON encoded.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+try {
+    JSON.parse(document.getElementById('data').value);
+}
+catch (e) {
+    window.alert('Invalid JSON data');
+}</t>
+  </si>
+  <si>
+    <t>try{
+    JSON.stringify(document.getElementById('data').value);
+}
+catch (e) {
+    window.alert('Invalid JSON data');
+}</t>
+  </si>
+  <si>
+    <t>My answer is incorrect.Answer explanation: This code calls the parse function of the JSON object, passing to it the value of the input field.The parse function attemps to convert string data to a JSON-encoded object.If conversion fails an error is thrown;</t>
+  </si>
+  <si>
+    <t>12.You are developing a web page for a publishing company.The page allows users to comment on published articles.The web page stores a user's login credentials in a cookie.A security expert informs you that the page allows code injection.When you and other users visit the page an alert message is displayed showing the user's login credentials.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modify  the Show function as follows:                                                                                                                                                                         function Show(comment) {
+    comment = comment.replace("&lt;", "&amp;lt;").replace("&gt;","&amp;gt;");
+    var div = document.createElement('div');
+    div.innerHTML = comment;
+    comment.appendChild(div);
+}                                                                               </t>
+  </si>
+  <si>
+    <t>My answer is correct. Answer explanation: This code repalces the left and right angle brackets (&lt; &gt;) with their HTML encoded equivalents.This prevents the rendering or processing of any HTML markup a user may enter. Altough the security expert in this scenario shows how to simply display an alert message a more complex example involves generating a form element that posts the contents of the cookie to an attacker's website.</t>
+  </si>
+  <si>
+    <t>13.You are developing a web page that allows users to choose toppings for a pizza.The user must select at least one topping.If not you want to display the message "Please select a topping" to the user and prevent the form from being submitted.If the user selects at least one topping the form should be submitted.</t>
+  </si>
+  <si>
+    <t>You should use the following code segment:                                                                                                                                                                              $('#submitButton').click(function () {
+   var isChecked = false;
+   $('input:checkbox').forEach(function (index, value) {
+      if (value.checked) {
+          isChecked = true;
+      } 
+      if(!isChecked) {
+          alert('Please select a topping.');
+      }
+   });
+});</t>
+  </si>
+  <si>
+    <t>My answer is correct.Answer explanation: This code first sets a local variable named isChecked to false.This variable is used to determine whether or not to display the message.The code then iterates through all input elements whose type arribute is set to checkbox as indicated by input:checkbox jQuery selector.If the checked property of anycheckbox is true the code sets the isChecked property to true.</t>
+  </si>
+  <si>
+    <t>14.The validateUserName function accepts a string value.You need to use the following regular expression to ensure that the user name is valid: ^[a-zA-Zo-9_-]{8,16}$ You need to write JavaScript code to determine wheter the userName value is valid.</t>
+  </si>
+  <si>
+    <t>var regex = /[^a-zA-Z0-9_-]{8,16}$/;
+regex.test(userName);</t>
+  </si>
+  <si>
+    <t>var regex = /[^a-zA-Z0-9_-]{8,16}$/;
+userName.test(regex);</t>
+  </si>
+  <si>
+    <t>My answer is incorrect. Answer explanation: This code initializes a RegExp object named regex with a regular expression. When you assign a regular expression this way you should enclose the expression within / / symbols. Next it calls the test function of the RegExp object to determine whether the userName variable contains the pattern specified by the regular expression.</t>
+  </si>
+  <si>
+    <t>15.You want to generate an error that could be handled by a try-catch block in JavaScript.</t>
+  </si>
+  <si>
+    <t>throw</t>
+  </si>
+  <si>
+    <t>try</t>
+  </si>
+  <si>
+    <t>My answeri is incorrect.Answer explanation: You should use "throw" to generate an error that could be handled by a try-catch block.</t>
+  </si>
+  <si>
+    <t>16.You want to invoke a function in JavaScript.The function generates an error in certain conditions.You want to invoke the function safely.An alert box must be be displayed if and only if an error is generated by the function.A block of clean-up code should be executed whether or not there is an error.However the clean-up process should not happen before the alert box is displayed when an error occurs.</t>
+  </si>
+  <si>
+    <t>try{
+    couldFail();
+}
+catch (e) {
+    alert('Error!');
+}
+finally {
+    // clean up
+}</t>
+  </si>
+  <si>
+    <t>My answer is correct. Answer explanations:The standard error handling in JavaScript is a try…catch…finally block.Statements where an error can occur should be placed in the try block. The catch block will be executed if an error occurs.The finally block will be executed unconditionally after all error processing has been completed.</t>
+  </si>
+  <si>
+    <t>17.You need to ensure that the CalculateDefaultShipping function is called only if the LogError function is called.</t>
+  </si>
+  <si>
+    <t>Add this code between lines 20 and 21: throw e;</t>
+  </si>
+  <si>
+    <t>Add this code between lines 20 and 21:                                                                                                                                    finally{ CalculateDefaultShipping(); }</t>
+  </si>
+  <si>
+    <t>My answer is incorrect.Answer explanation: The throw statement allows you to re-throw an error that is caught,By default when an error is handled in a catch block it is not propagated up the call stack.By re-throwing the error you allow the catch block higher in the call stack to handle the error.In this scenario the catch block in the call stack executes the CalculateDefaultShipping function.</t>
+  </si>
+  <si>
+    <t>18.You need to determine which function or functions threw an error.</t>
+  </si>
+  <si>
+    <t>1.CalculateShipping 2.LogError</t>
+  </si>
+  <si>
+    <t>1.CalculateShipping 2.Cleanup</t>
+  </si>
+  <si>
+    <t>My answer is incorrect. Answer explanation: You should conclude that the LogError and CalculateShipping functions threw an error.In this scenario the inner try block successfully writes "Packages created".But it fails to write "Shipping calculated".This means that the CalculateShipping function threw an error.Execution then proceeds to the catch block associated with that try block.The catch block should write "Error calculating shipping costs".However it fails to do so.This means that the LogError function also threw an error.Execution then proceeds to the outer catch block which also throws an error.</t>
+  </si>
+  <si>
+    <t>19.You need to write a function.The purpose of the function is to divide two numbers.If the number passed as the second parameter is zero you must raise an error so that code in a catch block executes.</t>
+  </si>
+  <si>
+    <t>throw "divisor cannot be zero.";</t>
+  </si>
+  <si>
+    <t>My answer is correct. Answer explanation: This code throws an error.If the Divide function is called from a try block the corresponding catch block gets executed when the throw statement is executed.</t>
+  </si>
+  <si>
+    <t>20.The webpage contains multiple anchor links.Some of these links are targeting URLs using the HTTPS protocol.You want to highlight these links with a different color.</t>
+  </si>
+  <si>
+    <t>a[href^="https://"]</t>
+  </si>
+  <si>
+    <t>My anwer is correct. Answer explanation: This code is the most appropriate selector because it matches all anchor links with an href value that begins with "https://".</t>
+  </si>
+  <si>
+    <t>21.The webpage contains hundreds of paragraphs.Each paragraph is wrapped with a &lt;p&gt; element. You want to highlight paragraphs that have a matching text "keyword" using jQuery.</t>
+  </si>
+  <si>
+    <t>$(":contains('keyword')")</t>
+  </si>
+  <si>
+    <t>$("p[text='keyword']")</t>
+  </si>
+  <si>
+    <t>My answer is incorrect. Answer explanation: To match all &lt;p&gt; elements that contain the text "keyword" using jQuery you should use the "p:contains('keyword')" selector.</t>
+  </si>
+  <si>
+    <t>22.You are using CSS3 and jQuery to dynamically style a web page.You want to find every paragraph element that is the third paragraph of its parent element and set its background color to green.</t>
+  </si>
+  <si>
+    <t>$("p:nth-of-type(3)").css("background-color", "green");</t>
+  </si>
+  <si>
+    <t xml:space="preserve">My answer is correct.Answer explanation: This code uses the nth-of-type selector to find the third paragraph element.The index is one-based.It then calls the css function to set the background-color property to green. </t>
+  </si>
+  <si>
+    <t>23.When the mouse pointer enters an input element the background color of the row must run green.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$("table td input").focus(function() { $(this).parent().parent().css("background-color", "green"); }); </t>
+  </si>
+  <si>
+    <t xml:space="preserve">$("td &gt; input").focus(function() { $('input').parent().parent().css("background-color", "green"); });   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> My answer is incorrect. Answer explanation: This code first finds all input elements that are descendants of td elements, which are in turn descendants of table elements.It calls the focus function to attach the onfocus event of the input elements to an anonymous function that represents an event handler.The anonymous function uses the "this" keyword to obtain a reference to the current object which is the input element that has focus.It then calls the parent function twice to obtain a reference to the tr element that represents the current row.Finally it calls the css function to set the background color of the row to green.</t>
+  </si>
+  <si>
+    <t>24.You want to set the background color of all button controls to blue regardless of the syntax that is used.</t>
+  </si>
+  <si>
+    <t>$(":button").css("background-color", "blue");</t>
+  </si>
+  <si>
+    <t>My answer is correct. Answer explanation: This code uses the $(":button") syntax to find all elements of type button.This includes &lt;input type="button"/&gt; elements and &lt;button&gt; elements.It then calls the css function to set the background color of the buttons to blue.</t>
+  </si>
+  <si>
+    <t>25.You are using CSS3 and jQuery to  dynamically style a web page.You want to find every section element that is the fourth section element of its parent element and set its background color to lightgrey.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$("section:nth-of-type(4)").css("background-color", "lightgrey"); </t>
+  </si>
+  <si>
+    <t>My answer is correct.Answer explanation: This code uses the nth-of-type selector to find the fourth section element of each parent element.The index is one-based.It then calls the css function to set the background-color property to lightgreay.</t>
+  </si>
+  <si>
+    <t>26.A web site has mixed use of button control syntax.Some pages use &lt;input type="button" /&gt; and other pages use &lt;button /&gt;.All button controls must have a solid one-pixel red border.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$(":button").css("border", "solid 1px red"); </t>
+  </si>
+  <si>
+    <t>27.You have a canvas in an HTML5 webpage.You want to programmatically change the background color of the canvas to orange.</t>
+  </si>
+  <si>
+    <t>var canvas = document.getElementById("myCanvas");
+var ctx = canvas.getContext("2d");
+ctx.fillStyle = "orange";
+ctx.fillRect(0, 0, 200, 200);</t>
+  </si>
+  <si>
+    <t>My answer is correct.Answer explanations: To manipulate an HTML5 canvas you must first get its 2D context. Var ctx = canvas.getContext("2d"); To fill the background of a canvas with an orange color you should specify the fillStyle  property of the context.The fillStyle property could be a CSS color value a gradient or a pattern. ctx.fillStyle = "orange"; The canvas is a 200x200 rectangle.To change its background you can use the fillRect(x, y, width, height ); method to fill the entire rectangle from the top-left corner.The coordinate of the top-left is (0, 0); ctx.fillRect.</t>
+  </si>
+  <si>
+    <t>28.You need to write JavaScript code that plays the video file specified in the text box when the play button is clicked</t>
+  </si>
+  <si>
+    <t>var player = document.getElementById("player");
+var videoFileInput = document.getElementById("videoFile");
+if (videoFileInput.value) {
+    player.src = videoFileInput.value;
+    player.play();
+}</t>
+  </si>
+  <si>
+    <t>My answer is correct. Answer explanation: This code first retrieves a reference to the video object and the input object that represents the text box.It sets the the src attribute of the video object to the value of the input element.The src attribute specifies the URL of the video to be played.It then calls the play function of the video object.The play function plays the video.</t>
+  </si>
+  <si>
+    <t>29.You need to draw a red-filled rectangle of the entire left half of the canvas.</t>
+  </si>
+  <si>
+    <t>var canvas = document.getElementById("myCanvas");
+var context = canvas.getContext("2d");
+context.fillStyle = "#FF0000";
+context.fillRect(0, 0, 100, 200);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">My answer is correct.Answer explanation: This code first retrieves an instance to the canvas element.Next it calls the getContext function to return a two-dimensional drawing context.It sets the fillStyle property of the context to red.Finally it calls the fillRect function to fill a rectangle at the coordinates 0, 0, 100, 200 which represent the left coordinate, top coordinate, width and height of the rectangle respectively. </t>
+  </si>
+  <si>
+    <t>30.You need to implement the ToggleMute function to accomplish your goal.</t>
+  </si>
+  <si>
+    <t>var audio = document.getElementById("myAudio");
+var checkbox = document.getElementById("muteCheckBox");
+audio.muted = checkbox.checked;</t>
+  </si>
+  <si>
+    <t>My answer is correct.Answer explanation:This code first retrieves instances of the audio object and the input object that represents the checkbox.It then sets the muted property of the audio object to the value of the checked property of the input object.This mutes the audio when the checkbox is checked and it unmutes the object when the checkbox is unchecked.</t>
+  </si>
+  <si>
+    <t>31.When a user clicks the Add Family Member button you want to dynamically add a new input element to the section.Each newly added element must use the same style as the existing input elements.</t>
+  </si>
+  <si>
+    <t>var input = document.createElement("input");
+input.style.display = "block";
+input.setAttribute("type", "text");
+var section = document.getElementById("memberSection");
+section.appendChild(input);</t>
+  </si>
+  <si>
+    <t>My answer is correct.Answer explanation: This code first creates an input object by calling the createElement function of the document object.The parameter to this function specifies the type of element the created object represents.In this scenario it is a input element.Next it accesses the style property of the input object to retrieve a reference to a style object.It then sets the display property of the style object to block allowing the input object to use the same style as the existing input elements.It calls the setAttribute function of the input object to set the type attribute to text matching the existing input elements.Next it retrieves an instance of the section object that contains the current input elements.It calls the appendChild function of the section object to add the input element as child of the section element.</t>
+  </si>
+  <si>
+    <t>32.You need to add code at line 4 to play the audio file specified in the text box when the play button is cliked.The audio file must play only once.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">player.src = audioFileInput.value;
+player.play();
+</t>
+  </si>
+  <si>
+    <t>My answer is correct.Answer explanation: This code retrieves references to the audio and the text box.If the text box has a value it sets the src attribute of the audio element to the value of the text box.It then calls the play function of the audio element to play the sound.</t>
+  </si>
+  <si>
+    <t>33.Which button style matches the applied style:                                                                                                                               
+div.button {
+    background-color: rgb(41, 140, 218);
+    border-radius: 0 10px;
+    color: #FFFFFF;
+    display: table-cell;
+    font-weight: bold;
+    height: 40px;
+    text-align: center;
+    vertical-align: middle;
+    width: 90px;
+}</t>
+  </si>
+  <si>
+    <t>Style 2</t>
+  </si>
+  <si>
+    <t>My answer is correct.Answer explanation: The value specified for border-radius is 0 10px which meanst the both top-left and bottom-right corners are not rounded and top-right and bottom-left corners are rounded with a radius of 10px.Therefore Style 2 is correct.</t>
+  </si>
+  <si>
+    <t>34.What are the positions of the padding, border and margin in the CSS box model?</t>
+  </si>
+  <si>
+    <t>The correct order is 1.Margin 2.Border 3.Padding</t>
+  </si>
+  <si>
+    <t>My answer is correct.Answer explanation: According to the CSS box model each box has a content area and optional surrounding margin, border and padding areas.The content area is the innermost followed by padding border and margin areas.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,20 +470,62 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="16"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color theme="0"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color theme="0"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -195,23 +537,55 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Accent1" xfId="1" builtinId="29"/>
+    <cellStyle name="Accent2" xfId="2" builtinId="33"/>
+    <cellStyle name="Accent4" xfId="3" builtinId="41"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFCC3300"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -488,336 +862,601 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D352"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="100.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="95.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="89.88671875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="125.109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="147.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="151" style="5" customWidth="1"/>
+    <col min="3" max="3" width="149.85546875" style="7" customWidth="1"/>
+    <col min="4" max="4" width="147" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21.3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="227.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="227.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="273.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="273.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="273.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="273.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="273.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="273.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="273.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="273.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="273.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="273.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="273.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="9" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:4" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:4" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="17" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="18" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="19" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="20" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="21" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="22" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="23" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="24" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="25" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="26" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="27" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="28" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="32" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="33" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="34" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="35" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="36" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="37" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="38" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="39" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="40" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="41" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="42" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="43" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="44" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="45" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="46" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="47" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="48" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="49" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="50" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="51" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="52" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="53" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="54" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="55" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="56" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="57" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="58" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="59" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="60" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="61" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="62" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="63" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="64" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="65" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="66" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="67" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="68" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="69" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="70" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="71" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="72" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="73" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="74" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="75" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="76" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="77" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="78" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="79" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="80" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="81" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="82" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="83" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="84" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="85" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="86" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="87" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="88" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="89" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="90" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="91" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="92" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="93" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="94" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="95" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="96" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="97" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="98" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="99" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="100" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="101" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="102" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="103" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="104" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="105" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="106" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="107" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="108" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="109" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="110" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="111" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="112" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="113" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="114" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="115" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="116" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="117" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="118" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="119" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="120" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="121" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="122" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="123" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="124" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="125" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="126" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="127" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="128" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="129" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="130" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="131" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="132" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="133" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="134" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="135" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="136" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="137" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="138" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="139" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="140" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="141" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="142" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="143" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="144" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="145" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="146" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="147" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="148" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="149" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="150" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="151" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="152" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="153" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="154" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="155" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="156" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="157" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="158" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="159" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="160" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="161" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="162" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="163" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="164" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="165" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="166" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="167" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="168" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="169" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="170" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="171" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="172" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="173" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="174" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="175" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="176" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="177" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="178" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="179" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="180" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="181" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="182" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="183" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="184" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="185" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="186" ht="273.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="351" ht="218.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="352" ht="409.6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="373.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="101" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="102" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="103" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="104" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="105" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="106" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="107" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="108" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="109" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="110" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="111" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="112" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="113" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="114" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="115" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="116" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="117" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="118" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="119" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="120" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="121" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="124" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="125" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="126" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="127" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="128" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="129" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="130" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="131" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="132" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="133" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="134" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="135" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="136" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="137" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="138" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="139" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="140" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="141" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="142" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="143" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="144" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="145" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="146" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="147" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="148" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="149" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="150" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="151" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="152" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="153" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="154" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="155" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="156" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="157" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="158" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="159" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="160" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="161" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="162" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="163" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="164" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="165" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="166" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="167" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="168" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="169" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="170" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="171" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="172" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="173" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="174" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="175" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="176" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="177" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="178" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="179" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="180" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="181" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="182" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="183" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="184" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="185" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="186" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="187" ht="276" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="188" ht="276" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="189" ht="276" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="190" ht="276" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="191" ht="276" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="192" ht="276" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="250" ht="240" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="351" ht="218.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="352" ht="409.6" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Commit on 23.01.2019. Applied the biggest height for an element in the rows.
</commit_message>
<xml_diff>
--- a/Exam Preparation/resources/70-480 Practice Exam Answers and Explanations.xlsx
+++ b/Exam Preparation/resources/70-480 Practice Exam Answers and Explanations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22264" windowHeight="12647"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -461,7 +461,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -494,6 +494,13 @@
     <font>
       <b/>
       <sz val="24"/>
+      <color theme="0"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="22"/>
       <color theme="0"/>
       <name val="Calibri Light"/>
       <family val="2"/>
@@ -544,7 +551,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -569,6 +576,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -862,19 +881,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D352"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="23.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="147.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="147.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="151" style="5" customWidth="1"/>
-    <col min="3" max="3" width="149.85546875" style="7" customWidth="1"/>
+    <col min="3" max="3" width="149.88671875" style="7" customWidth="1"/>
     <col min="4" max="4" width="147" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="3" customFormat="1" ht="30.7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -888,575 +907,1746 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="227.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="B2" s="11"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="13"/>
+    </row>
+    <row r="3" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="C3" s="12"/>
+      <c r="D3" s="13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="C4" s="12"/>
+      <c r="D4" s="13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="C5" s="12"/>
+      <c r="D5" s="13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="B6" s="11"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="13"/>
+    </row>
+    <row r="7" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="C7" s="12"/>
+      <c r="D7" s="13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="C8" s="12"/>
+      <c r="D8" s="13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="C9" s="12"/>
+      <c r="D9" s="13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="13" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="13" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="C13" s="12"/>
+      <c r="D13" s="13" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="13" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="C15" s="12"/>
+      <c r="D15" s="13" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="C16" s="12"/>
+      <c r="D16" s="13" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="13" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="13" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="C19" s="12"/>
+      <c r="D19" s="13" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="13" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="13" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="C22" s="12"/>
+      <c r="D22" s="13" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+    <row r="23" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="C23" s="12"/>
+      <c r="D23" s="13" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+    <row r="24" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="D24" s="9" t="s">
+      <c r="D24" s="13" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+    <row r="25" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="C25" s="12"/>
+      <c r="D25" s="13" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+    <row r="26" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C26" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="D26" s="9" t="s">
+      <c r="D26" s="13" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+    <row r="27" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="D27" s="9" t="s">
+      <c r="C27" s="12"/>
+      <c r="D27" s="13" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+    <row r="28" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="D28" s="9" t="s">
+      <c r="C28" s="12"/>
+      <c r="D28" s="13" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+    <row r="29" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="11" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+      <c r="C29" s="12"/>
+      <c r="D29" s="13"/>
+    </row>
+    <row r="30" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="D30" s="9" t="s">
+      <c r="C30" s="12"/>
+      <c r="D30" s="13" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+    <row r="31" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="D31" s="9" t="s">
+      <c r="C31" s="12"/>
+      <c r="D31" s="13" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+    <row r="32" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="D32" s="9" t="s">
+      <c r="C32" s="12"/>
+      <c r="D32" s="13" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+    <row r="33" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="D33" s="9" t="s">
+      <c r="C33" s="12"/>
+      <c r="D33" s="13" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+    <row r="34" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="D34" s="9" t="s">
+      <c r="C34" s="12"/>
+      <c r="D34" s="13" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+    <row r="35" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="D35" s="9" t="s">
+      <c r="C35" s="12"/>
+      <c r="D35" s="13" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="373.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+    <row r="36" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="D36" s="9" t="s">
+      <c r="C36" s="12"/>
+      <c r="D36" s="13" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+    <row r="37" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="D37" s="9" t="s">
+      <c r="C37" s="12"/>
+      <c r="D37" s="13" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:4" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="65" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="66" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="67" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="68" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="69" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="70" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="71" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="72" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="73" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="74" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="75" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="76" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="77" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="78" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="79" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="80" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="81" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="82" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="83" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="84" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="85" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="86" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="87" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="88" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="89" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="90" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="91" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="92" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="93" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="94" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="95" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="96" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="97" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="98" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="99" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="100" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="101" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="102" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="103" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="104" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="105" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="106" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="107" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="108" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="109" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="110" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="111" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="112" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="113" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="114" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="115" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="116" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="117" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="118" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="119" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="120" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="121" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="122" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="123" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="124" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="125" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="126" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="127" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="128" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="129" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="130" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="131" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="132" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="133" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="134" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="135" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="136" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="137" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="138" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="139" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="140" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="141" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="142" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="143" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="144" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="145" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="146" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="147" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="148" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="149" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="150" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="151" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="152" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="153" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="154" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="155" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="156" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="157" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="158" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="159" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="160" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="161" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="162" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="163" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="164" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="165" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="166" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="167" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="168" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="169" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="170" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="171" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="172" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="173" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="174" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="175" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="176" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="177" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="178" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="179" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="180" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="181" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="182" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="183" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="184" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="185" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="186" ht="273.39999999999998" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="187" ht="276" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="188" ht="276" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="189" ht="276" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="190" ht="276" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="191" ht="276" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="192" ht="276" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="250" ht="240" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="351" ht="218.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="352" ht="409.6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="10"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="13"/>
+    </row>
+    <row r="39" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="10"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="13"/>
+    </row>
+    <row r="40" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="10"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="13"/>
+    </row>
+    <row r="41" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="10"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="13"/>
+    </row>
+    <row r="42" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="10"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="13"/>
+    </row>
+    <row r="43" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="10"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="13"/>
+    </row>
+    <row r="44" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="10"/>
+      <c r="B44" s="11"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="13"/>
+    </row>
+    <row r="45" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="10"/>
+      <c r="B45" s="11"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="13"/>
+    </row>
+    <row r="46" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="10"/>
+      <c r="B46" s="11"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="13"/>
+    </row>
+    <row r="47" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="10"/>
+      <c r="B47" s="11"/>
+      <c r="C47" s="12"/>
+      <c r="D47" s="13"/>
+    </row>
+    <row r="48" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="10"/>
+      <c r="B48" s="11"/>
+      <c r="C48" s="12"/>
+      <c r="D48" s="13"/>
+    </row>
+    <row r="49" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="10"/>
+      <c r="B49" s="11"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="13"/>
+    </row>
+    <row r="50" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="10"/>
+      <c r="B50" s="11"/>
+      <c r="C50" s="12"/>
+      <c r="D50" s="13"/>
+    </row>
+    <row r="51" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="10"/>
+      <c r="B51" s="11"/>
+      <c r="C51" s="12"/>
+      <c r="D51" s="13"/>
+    </row>
+    <row r="52" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="10"/>
+      <c r="B52" s="11"/>
+      <c r="C52" s="12"/>
+      <c r="D52" s="13"/>
+    </row>
+    <row r="53" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="10"/>
+      <c r="B53" s="11"/>
+      <c r="C53" s="12"/>
+      <c r="D53" s="13"/>
+    </row>
+    <row r="54" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="10"/>
+      <c r="B54" s="11"/>
+      <c r="C54" s="12"/>
+      <c r="D54" s="13"/>
+    </row>
+    <row r="55" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="10"/>
+      <c r="B55" s="11"/>
+      <c r="C55" s="12"/>
+      <c r="D55" s="13"/>
+    </row>
+    <row r="56" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="10"/>
+      <c r="B56" s="11"/>
+      <c r="C56" s="12"/>
+      <c r="D56" s="13"/>
+    </row>
+    <row r="57" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="10"/>
+      <c r="B57" s="11"/>
+      <c r="C57" s="12"/>
+      <c r="D57" s="13"/>
+    </row>
+    <row r="58" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="10"/>
+      <c r="B58" s="11"/>
+      <c r="C58" s="12"/>
+      <c r="D58" s="13"/>
+    </row>
+    <row r="59" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="10"/>
+      <c r="B59" s="11"/>
+      <c r="C59" s="12"/>
+      <c r="D59" s="13"/>
+    </row>
+    <row r="60" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="10"/>
+      <c r="B60" s="11"/>
+      <c r="C60" s="12"/>
+      <c r="D60" s="13"/>
+    </row>
+    <row r="61" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="10"/>
+      <c r="B61" s="11"/>
+      <c r="C61" s="12"/>
+      <c r="D61" s="13"/>
+    </row>
+    <row r="62" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="10"/>
+      <c r="B62" s="11"/>
+      <c r="C62" s="12"/>
+      <c r="D62" s="13"/>
+    </row>
+    <row r="63" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="10"/>
+      <c r="B63" s="11"/>
+      <c r="C63" s="12"/>
+      <c r="D63" s="13"/>
+    </row>
+    <row r="64" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="10"/>
+      <c r="B64" s="11"/>
+      <c r="C64" s="12"/>
+      <c r="D64" s="13"/>
+    </row>
+    <row r="65" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="10"/>
+      <c r="B65" s="11"/>
+      <c r="C65" s="12"/>
+      <c r="D65" s="13"/>
+    </row>
+    <row r="66" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="10"/>
+      <c r="B66" s="11"/>
+      <c r="C66" s="12"/>
+      <c r="D66" s="13"/>
+    </row>
+    <row r="67" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="10"/>
+      <c r="B67" s="11"/>
+      <c r="C67" s="12"/>
+      <c r="D67" s="13"/>
+    </row>
+    <row r="68" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="10"/>
+      <c r="B68" s="11"/>
+      <c r="C68" s="12"/>
+      <c r="D68" s="13"/>
+    </row>
+    <row r="69" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="10"/>
+      <c r="B69" s="11"/>
+      <c r="C69" s="12"/>
+      <c r="D69" s="13"/>
+    </row>
+    <row r="70" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="10"/>
+      <c r="B70" s="11"/>
+      <c r="C70" s="12"/>
+      <c r="D70" s="13"/>
+    </row>
+    <row r="71" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="10"/>
+      <c r="B71" s="11"/>
+      <c r="C71" s="12"/>
+      <c r="D71" s="13"/>
+    </row>
+    <row r="72" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="10"/>
+      <c r="B72" s="11"/>
+      <c r="C72" s="12"/>
+      <c r="D72" s="13"/>
+    </row>
+    <row r="73" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="10"/>
+      <c r="B73" s="11"/>
+      <c r="C73" s="12"/>
+      <c r="D73" s="13"/>
+    </row>
+    <row r="74" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="10"/>
+      <c r="B74" s="11"/>
+      <c r="C74" s="12"/>
+      <c r="D74" s="13"/>
+    </row>
+    <row r="75" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="10"/>
+      <c r="B75" s="11"/>
+      <c r="C75" s="12"/>
+      <c r="D75" s="13"/>
+    </row>
+    <row r="76" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="10"/>
+      <c r="B76" s="11"/>
+      <c r="C76" s="12"/>
+      <c r="D76" s="13"/>
+    </row>
+    <row r="77" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="10"/>
+      <c r="B77" s="11"/>
+      <c r="C77" s="12"/>
+      <c r="D77" s="13"/>
+    </row>
+    <row r="78" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="10"/>
+      <c r="B78" s="11"/>
+      <c r="C78" s="12"/>
+      <c r="D78" s="13"/>
+    </row>
+    <row r="79" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="10"/>
+      <c r="B79" s="11"/>
+      <c r="C79" s="12"/>
+      <c r="D79" s="13"/>
+    </row>
+    <row r="80" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="10"/>
+      <c r="B80" s="11"/>
+      <c r="C80" s="12"/>
+      <c r="D80" s="13"/>
+    </row>
+    <row r="81" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="10"/>
+      <c r="B81" s="11"/>
+      <c r="C81" s="12"/>
+      <c r="D81" s="13"/>
+    </row>
+    <row r="82" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="10"/>
+      <c r="B82" s="11"/>
+      <c r="C82" s="12"/>
+      <c r="D82" s="13"/>
+    </row>
+    <row r="83" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="10"/>
+      <c r="B83" s="11"/>
+      <c r="C83" s="12"/>
+      <c r="D83" s="13"/>
+    </row>
+    <row r="84" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="10"/>
+      <c r="B84" s="11"/>
+      <c r="C84" s="12"/>
+      <c r="D84" s="13"/>
+    </row>
+    <row r="85" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="10"/>
+      <c r="B85" s="11"/>
+      <c r="C85" s="12"/>
+      <c r="D85" s="13"/>
+    </row>
+    <row r="86" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="10"/>
+      <c r="B86" s="11"/>
+      <c r="C86" s="12"/>
+      <c r="D86" s="13"/>
+    </row>
+    <row r="87" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="10"/>
+      <c r="B87" s="11"/>
+      <c r="C87" s="12"/>
+      <c r="D87" s="13"/>
+    </row>
+    <row r="88" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="10"/>
+      <c r="B88" s="11"/>
+      <c r="C88" s="12"/>
+      <c r="D88" s="13"/>
+    </row>
+    <row r="89" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="10"/>
+      <c r="B89" s="11"/>
+      <c r="C89" s="12"/>
+      <c r="D89" s="13"/>
+    </row>
+    <row r="90" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="10"/>
+      <c r="B90" s="11"/>
+      <c r="C90" s="12"/>
+      <c r="D90" s="13"/>
+    </row>
+    <row r="91" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="10"/>
+      <c r="B91" s="11"/>
+      <c r="C91" s="12"/>
+      <c r="D91" s="13"/>
+    </row>
+    <row r="92" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="10"/>
+      <c r="B92" s="11"/>
+      <c r="C92" s="12"/>
+      <c r="D92" s="13"/>
+    </row>
+    <row r="93" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="10"/>
+      <c r="B93" s="11"/>
+      <c r="C93" s="12"/>
+      <c r="D93" s="13"/>
+    </row>
+    <row r="94" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="10"/>
+      <c r="B94" s="11"/>
+      <c r="C94" s="12"/>
+      <c r="D94" s="13"/>
+    </row>
+    <row r="95" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="10"/>
+      <c r="B95" s="11"/>
+      <c r="C95" s="12"/>
+      <c r="D95" s="13"/>
+    </row>
+    <row r="96" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="10"/>
+      <c r="B96" s="11"/>
+      <c r="C96" s="12"/>
+      <c r="D96" s="13"/>
+    </row>
+    <row r="97" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="10"/>
+      <c r="B97" s="11"/>
+      <c r="C97" s="12"/>
+      <c r="D97" s="13"/>
+    </row>
+    <row r="98" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="10"/>
+      <c r="B98" s="11"/>
+      <c r="C98" s="12"/>
+      <c r="D98" s="13"/>
+    </row>
+    <row r="99" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="10"/>
+      <c r="B99" s="11"/>
+      <c r="C99" s="12"/>
+      <c r="D99" s="13"/>
+    </row>
+    <row r="100" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="10"/>
+      <c r="B100" s="11"/>
+      <c r="C100" s="12"/>
+      <c r="D100" s="13"/>
+    </row>
+    <row r="101" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="10"/>
+      <c r="B101" s="11"/>
+      <c r="C101" s="12"/>
+      <c r="D101" s="13"/>
+    </row>
+    <row r="102" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="10"/>
+      <c r="B102" s="11"/>
+      <c r="C102" s="12"/>
+      <c r="D102" s="13"/>
+    </row>
+    <row r="103" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="10"/>
+      <c r="B103" s="11"/>
+      <c r="C103" s="12"/>
+      <c r="D103" s="13"/>
+    </row>
+    <row r="104" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="10"/>
+      <c r="B104" s="11"/>
+      <c r="C104" s="12"/>
+      <c r="D104" s="13"/>
+    </row>
+    <row r="105" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="10"/>
+      <c r="B105" s="11"/>
+      <c r="C105" s="12"/>
+      <c r="D105" s="13"/>
+    </row>
+    <row r="106" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="10"/>
+      <c r="B106" s="11"/>
+      <c r="C106" s="12"/>
+      <c r="D106" s="13"/>
+    </row>
+    <row r="107" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="10"/>
+      <c r="B107" s="11"/>
+      <c r="C107" s="12"/>
+      <c r="D107" s="13"/>
+    </row>
+    <row r="108" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="10"/>
+      <c r="B108" s="11"/>
+      <c r="C108" s="12"/>
+      <c r="D108" s="13"/>
+    </row>
+    <row r="109" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="10"/>
+      <c r="B109" s="11"/>
+      <c r="C109" s="12"/>
+      <c r="D109" s="13"/>
+    </row>
+    <row r="110" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="10"/>
+      <c r="B110" s="11"/>
+      <c r="C110" s="12"/>
+      <c r="D110" s="13"/>
+    </row>
+    <row r="111" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="10"/>
+      <c r="B111" s="11"/>
+      <c r="C111" s="12"/>
+      <c r="D111" s="13"/>
+    </row>
+    <row r="112" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="10"/>
+      <c r="B112" s="11"/>
+      <c r="C112" s="12"/>
+      <c r="D112" s="13"/>
+    </row>
+    <row r="113" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A113" s="10"/>
+      <c r="B113" s="11"/>
+      <c r="C113" s="12"/>
+      <c r="D113" s="13"/>
+    </row>
+    <row r="114" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A114" s="10"/>
+      <c r="B114" s="11"/>
+      <c r="C114" s="12"/>
+      <c r="D114" s="13"/>
+    </row>
+    <row r="115" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A115" s="10"/>
+      <c r="B115" s="11"/>
+      <c r="C115" s="12"/>
+      <c r="D115" s="13"/>
+    </row>
+    <row r="116" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A116" s="10"/>
+      <c r="B116" s="11"/>
+      <c r="C116" s="12"/>
+      <c r="D116" s="13"/>
+    </row>
+    <row r="117" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A117" s="10"/>
+      <c r="B117" s="11"/>
+      <c r="C117" s="12"/>
+      <c r="D117" s="13"/>
+    </row>
+    <row r="118" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A118" s="10"/>
+      <c r="B118" s="11"/>
+      <c r="C118" s="12"/>
+      <c r="D118" s="13"/>
+    </row>
+    <row r="119" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A119" s="10"/>
+      <c r="B119" s="11"/>
+      <c r="C119" s="12"/>
+      <c r="D119" s="13"/>
+    </row>
+    <row r="120" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A120" s="10"/>
+      <c r="B120" s="11"/>
+      <c r="C120" s="12"/>
+      <c r="D120" s="13"/>
+    </row>
+    <row r="121" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A121" s="10"/>
+      <c r="B121" s="11"/>
+      <c r="C121" s="12"/>
+      <c r="D121" s="13"/>
+    </row>
+    <row r="122" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A122" s="10"/>
+      <c r="B122" s="11"/>
+      <c r="C122" s="12"/>
+      <c r="D122" s="13"/>
+    </row>
+    <row r="123" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A123" s="10"/>
+      <c r="B123" s="11"/>
+      <c r="C123" s="12"/>
+      <c r="D123" s="13"/>
+    </row>
+    <row r="124" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A124" s="10"/>
+      <c r="B124" s="11"/>
+      <c r="C124" s="12"/>
+      <c r="D124" s="13"/>
+    </row>
+    <row r="125" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A125" s="10"/>
+      <c r="B125" s="11"/>
+      <c r="C125" s="12"/>
+      <c r="D125" s="13"/>
+    </row>
+    <row r="126" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A126" s="10"/>
+      <c r="B126" s="11"/>
+      <c r="C126" s="12"/>
+      <c r="D126" s="13"/>
+    </row>
+    <row r="127" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A127" s="10"/>
+      <c r="B127" s="11"/>
+      <c r="C127" s="12"/>
+      <c r="D127" s="13"/>
+    </row>
+    <row r="128" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A128" s="10"/>
+      <c r="B128" s="11"/>
+      <c r="C128" s="12"/>
+      <c r="D128" s="13"/>
+    </row>
+    <row r="129" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A129" s="10"/>
+      <c r="B129" s="11"/>
+      <c r="C129" s="12"/>
+      <c r="D129" s="13"/>
+    </row>
+    <row r="130" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A130" s="10"/>
+      <c r="B130" s="11"/>
+      <c r="C130" s="12"/>
+      <c r="D130" s="13"/>
+    </row>
+    <row r="131" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A131" s="10"/>
+      <c r="B131" s="11"/>
+      <c r="C131" s="12"/>
+      <c r="D131" s="13"/>
+    </row>
+    <row r="132" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A132" s="10"/>
+      <c r="B132" s="11"/>
+      <c r="C132" s="12"/>
+      <c r="D132" s="13"/>
+    </row>
+    <row r="133" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A133" s="10"/>
+      <c r="B133" s="11"/>
+      <c r="C133" s="12"/>
+      <c r="D133" s="13"/>
+    </row>
+    <row r="134" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A134" s="10"/>
+      <c r="B134" s="11"/>
+      <c r="C134" s="12"/>
+      <c r="D134" s="13"/>
+    </row>
+    <row r="135" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A135" s="10"/>
+      <c r="B135" s="11"/>
+      <c r="C135" s="12"/>
+      <c r="D135" s="13"/>
+    </row>
+    <row r="136" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A136" s="10"/>
+      <c r="B136" s="11"/>
+      <c r="C136" s="12"/>
+      <c r="D136" s="13"/>
+    </row>
+    <row r="137" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A137" s="10"/>
+      <c r="B137" s="11"/>
+      <c r="C137" s="12"/>
+      <c r="D137" s="13"/>
+    </row>
+    <row r="138" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A138" s="10"/>
+      <c r="B138" s="11"/>
+      <c r="C138" s="12"/>
+      <c r="D138" s="13"/>
+    </row>
+    <row r="139" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A139" s="10"/>
+      <c r="B139" s="11"/>
+      <c r="C139" s="12"/>
+      <c r="D139" s="13"/>
+    </row>
+    <row r="140" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A140" s="10"/>
+      <c r="B140" s="11"/>
+      <c r="C140" s="12"/>
+      <c r="D140" s="13"/>
+    </row>
+    <row r="141" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A141" s="10"/>
+      <c r="B141" s="11"/>
+      <c r="C141" s="12"/>
+      <c r="D141" s="13"/>
+    </row>
+    <row r="142" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A142" s="10"/>
+      <c r="B142" s="11"/>
+      <c r="C142" s="12"/>
+      <c r="D142" s="13"/>
+    </row>
+    <row r="143" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A143" s="10"/>
+      <c r="B143" s="11"/>
+      <c r="C143" s="12"/>
+      <c r="D143" s="13"/>
+    </row>
+    <row r="144" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A144" s="10"/>
+      <c r="B144" s="11"/>
+      <c r="C144" s="12"/>
+      <c r="D144" s="13"/>
+    </row>
+    <row r="145" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A145" s="10"/>
+      <c r="B145" s="11"/>
+      <c r="C145" s="12"/>
+      <c r="D145" s="13"/>
+    </row>
+    <row r="146" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A146" s="10"/>
+      <c r="B146" s="11"/>
+      <c r="C146" s="12"/>
+      <c r="D146" s="13"/>
+    </row>
+    <row r="147" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A147" s="10"/>
+      <c r="B147" s="11"/>
+      <c r="C147" s="12"/>
+      <c r="D147" s="13"/>
+    </row>
+    <row r="148" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A148" s="10"/>
+      <c r="B148" s="11"/>
+      <c r="C148" s="12"/>
+      <c r="D148" s="13"/>
+    </row>
+    <row r="149" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A149" s="10"/>
+      <c r="B149" s="11"/>
+      <c r="C149" s="12"/>
+      <c r="D149" s="13"/>
+    </row>
+    <row r="150" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A150" s="10"/>
+      <c r="B150" s="11"/>
+      <c r="C150" s="12"/>
+      <c r="D150" s="13"/>
+    </row>
+    <row r="151" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A151" s="10"/>
+      <c r="B151" s="11"/>
+      <c r="C151" s="12"/>
+      <c r="D151" s="13"/>
+    </row>
+    <row r="152" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A152" s="10"/>
+      <c r="B152" s="11"/>
+      <c r="C152" s="12"/>
+      <c r="D152" s="13"/>
+    </row>
+    <row r="153" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A153" s="10"/>
+      <c r="B153" s="11"/>
+      <c r="C153" s="12"/>
+      <c r="D153" s="13"/>
+    </row>
+    <row r="154" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A154" s="10"/>
+      <c r="B154" s="11"/>
+      <c r="C154" s="12"/>
+      <c r="D154" s="13"/>
+    </row>
+    <row r="155" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A155" s="10"/>
+      <c r="B155" s="11"/>
+      <c r="C155" s="12"/>
+      <c r="D155" s="13"/>
+    </row>
+    <row r="156" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A156" s="10"/>
+      <c r="B156" s="11"/>
+      <c r="C156" s="12"/>
+      <c r="D156" s="13"/>
+    </row>
+    <row r="157" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A157" s="10"/>
+      <c r="B157" s="11"/>
+      <c r="C157" s="12"/>
+      <c r="D157" s="13"/>
+    </row>
+    <row r="158" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A158" s="10"/>
+      <c r="B158" s="11"/>
+      <c r="C158" s="12"/>
+      <c r="D158" s="13"/>
+    </row>
+    <row r="159" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A159" s="10"/>
+      <c r="B159" s="11"/>
+      <c r="C159" s="12"/>
+      <c r="D159" s="13"/>
+    </row>
+    <row r="160" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A160" s="10"/>
+      <c r="B160" s="11"/>
+      <c r="C160" s="12"/>
+      <c r="D160" s="13"/>
+    </row>
+    <row r="161" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A161" s="10"/>
+      <c r="B161" s="11"/>
+      <c r="C161" s="12"/>
+      <c r="D161" s="13"/>
+    </row>
+    <row r="162" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A162" s="10"/>
+      <c r="B162" s="11"/>
+      <c r="C162" s="12"/>
+      <c r="D162" s="13"/>
+    </row>
+    <row r="163" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A163" s="10"/>
+      <c r="B163" s="11"/>
+      <c r="C163" s="12"/>
+      <c r="D163" s="13"/>
+    </row>
+    <row r="164" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A164" s="10"/>
+      <c r="B164" s="11"/>
+      <c r="C164" s="12"/>
+      <c r="D164" s="13"/>
+    </row>
+    <row r="165" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A165" s="10"/>
+      <c r="B165" s="11"/>
+      <c r="C165" s="12"/>
+      <c r="D165" s="13"/>
+    </row>
+    <row r="166" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A166" s="10"/>
+      <c r="B166" s="11"/>
+      <c r="C166" s="12"/>
+      <c r="D166" s="13"/>
+    </row>
+    <row r="167" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A167" s="10"/>
+      <c r="B167" s="11"/>
+      <c r="C167" s="12"/>
+      <c r="D167" s="13"/>
+    </row>
+    <row r="168" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A168" s="10"/>
+      <c r="B168" s="11"/>
+      <c r="C168" s="12"/>
+      <c r="D168" s="13"/>
+    </row>
+    <row r="169" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A169" s="10"/>
+      <c r="B169" s="11"/>
+      <c r="C169" s="12"/>
+      <c r="D169" s="13"/>
+    </row>
+    <row r="170" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A170" s="10"/>
+      <c r="B170" s="11"/>
+      <c r="C170" s="12"/>
+      <c r="D170" s="13"/>
+    </row>
+    <row r="171" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A171" s="10"/>
+      <c r="B171" s="11"/>
+      <c r="C171" s="12"/>
+      <c r="D171" s="13"/>
+    </row>
+    <row r="172" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A172" s="10"/>
+      <c r="B172" s="11"/>
+      <c r="C172" s="12"/>
+      <c r="D172" s="13"/>
+    </row>
+    <row r="173" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A173" s="10"/>
+      <c r="B173" s="11"/>
+      <c r="C173" s="12"/>
+      <c r="D173" s="13"/>
+    </row>
+    <row r="174" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A174" s="10"/>
+      <c r="B174" s="11"/>
+      <c r="C174" s="12"/>
+      <c r="D174" s="13"/>
+    </row>
+    <row r="175" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A175" s="10"/>
+      <c r="B175" s="11"/>
+      <c r="C175" s="12"/>
+      <c r="D175" s="13"/>
+    </row>
+    <row r="176" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A176" s="10"/>
+      <c r="B176" s="11"/>
+      <c r="C176" s="12"/>
+      <c r="D176" s="13"/>
+    </row>
+    <row r="177" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A177" s="10"/>
+      <c r="B177" s="11"/>
+      <c r="C177" s="12"/>
+      <c r="D177" s="13"/>
+    </row>
+    <row r="178" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A178" s="10"/>
+      <c r="B178" s="11"/>
+      <c r="C178" s="12"/>
+      <c r="D178" s="13"/>
+    </row>
+    <row r="179" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A179" s="10"/>
+      <c r="B179" s="11"/>
+      <c r="C179" s="12"/>
+      <c r="D179" s="13"/>
+    </row>
+    <row r="180" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A180" s="10"/>
+      <c r="B180" s="11"/>
+      <c r="C180" s="12"/>
+      <c r="D180" s="13"/>
+    </row>
+    <row r="181" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A181" s="10"/>
+      <c r="B181" s="11"/>
+      <c r="C181" s="12"/>
+      <c r="D181" s="13"/>
+    </row>
+    <row r="182" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A182" s="10"/>
+      <c r="B182" s="11"/>
+      <c r="C182" s="12"/>
+      <c r="D182" s="13"/>
+    </row>
+    <row r="183" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A183" s="10"/>
+      <c r="B183" s="11"/>
+      <c r="C183" s="12"/>
+      <c r="D183" s="13"/>
+    </row>
+    <row r="184" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A184" s="10"/>
+      <c r="B184" s="11"/>
+      <c r="C184" s="12"/>
+      <c r="D184" s="13"/>
+    </row>
+    <row r="185" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A185" s="10"/>
+      <c r="B185" s="11"/>
+      <c r="C185" s="12"/>
+      <c r="D185" s="13"/>
+    </row>
+    <row r="186" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A186" s="10"/>
+      <c r="B186" s="11"/>
+      <c r="C186" s="12"/>
+      <c r="D186" s="13"/>
+    </row>
+    <row r="187" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A187" s="10"/>
+      <c r="B187" s="11"/>
+      <c r="C187" s="12"/>
+      <c r="D187" s="13"/>
+    </row>
+    <row r="188" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A188" s="10"/>
+      <c r="B188" s="11"/>
+      <c r="C188" s="12"/>
+      <c r="D188" s="13"/>
+    </row>
+    <row r="189" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A189" s="10"/>
+      <c r="B189" s="11"/>
+      <c r="C189" s="12"/>
+      <c r="D189" s="13"/>
+    </row>
+    <row r="190" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A190" s="10"/>
+      <c r="B190" s="11"/>
+      <c r="C190" s="12"/>
+      <c r="D190" s="13"/>
+    </row>
+    <row r="191" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A191" s="10"/>
+      <c r="B191" s="11"/>
+      <c r="C191" s="12"/>
+      <c r="D191" s="13"/>
+    </row>
+    <row r="192" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A192" s="10"/>
+      <c r="B192" s="11"/>
+      <c r="C192" s="12"/>
+      <c r="D192" s="13"/>
+    </row>
+    <row r="193" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A193" s="10"/>
+      <c r="B193" s="11"/>
+      <c r="C193" s="12"/>
+      <c r="D193" s="13"/>
+    </row>
+    <row r="194" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A194" s="10"/>
+      <c r="B194" s="11"/>
+      <c r="C194" s="12"/>
+      <c r="D194" s="13"/>
+    </row>
+    <row r="195" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A195" s="10"/>
+      <c r="B195" s="11"/>
+      <c r="C195" s="12"/>
+      <c r="D195" s="13"/>
+    </row>
+    <row r="196" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A196" s="10"/>
+      <c r="B196" s="11"/>
+      <c r="C196" s="12"/>
+      <c r="D196" s="13"/>
+    </row>
+    <row r="197" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A197" s="10"/>
+      <c r="B197" s="11"/>
+      <c r="C197" s="12"/>
+      <c r="D197" s="13"/>
+    </row>
+    <row r="198" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A198" s="10"/>
+      <c r="B198" s="11"/>
+      <c r="C198" s="12"/>
+      <c r="D198" s="13"/>
+    </row>
+    <row r="199" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A199" s="10"/>
+      <c r="B199" s="11"/>
+      <c r="C199" s="12"/>
+      <c r="D199" s="13"/>
+    </row>
+    <row r="200" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A200" s="10"/>
+      <c r="B200" s="11"/>
+      <c r="C200" s="12"/>
+      <c r="D200" s="13"/>
+    </row>
+    <row r="201" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A201" s="10"/>
+      <c r="B201" s="11"/>
+      <c r="C201" s="12"/>
+      <c r="D201" s="13"/>
+    </row>
+    <row r="202" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A202" s="10"/>
+      <c r="B202" s="11"/>
+      <c r="C202" s="12"/>
+      <c r="D202" s="13"/>
+    </row>
+    <row r="203" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A203" s="10"/>
+      <c r="B203" s="11"/>
+      <c r="C203" s="12"/>
+      <c r="D203" s="13"/>
+    </row>
+    <row r="204" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A204" s="10"/>
+      <c r="B204" s="11"/>
+      <c r="C204" s="12"/>
+      <c r="D204" s="13"/>
+    </row>
+    <row r="205" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A205" s="10"/>
+      <c r="B205" s="11"/>
+      <c r="C205" s="12"/>
+      <c r="D205" s="13"/>
+    </row>
+    <row r="206" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A206" s="10"/>
+      <c r="B206" s="11"/>
+      <c r="C206" s="12"/>
+      <c r="D206" s="13"/>
+    </row>
+    <row r="207" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A207" s="10"/>
+      <c r="B207" s="11"/>
+      <c r="C207" s="12"/>
+      <c r="D207" s="13"/>
+    </row>
+    <row r="208" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A208" s="10"/>
+      <c r="B208" s="11"/>
+      <c r="C208" s="12"/>
+      <c r="D208" s="13"/>
+    </row>
+    <row r="209" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A209" s="10"/>
+      <c r="B209" s="11"/>
+      <c r="C209" s="12"/>
+      <c r="D209" s="13"/>
+    </row>
+    <row r="210" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A210" s="10"/>
+      <c r="B210" s="11"/>
+      <c r="C210" s="12"/>
+      <c r="D210" s="13"/>
+    </row>
+    <row r="211" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A211" s="10"/>
+      <c r="B211" s="11"/>
+      <c r="C211" s="12"/>
+      <c r="D211" s="13"/>
+    </row>
+    <row r="212" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A212" s="10"/>
+      <c r="B212" s="11"/>
+      <c r="C212" s="12"/>
+      <c r="D212" s="13"/>
+    </row>
+    <row r="213" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A213" s="10"/>
+      <c r="B213" s="11"/>
+      <c r="C213" s="12"/>
+      <c r="D213" s="13"/>
+    </row>
+    <row r="214" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A214" s="10"/>
+      <c r="B214" s="11"/>
+      <c r="C214" s="12"/>
+      <c r="D214" s="13"/>
+    </row>
+    <row r="215" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A215" s="10"/>
+      <c r="B215" s="11"/>
+      <c r="C215" s="12"/>
+      <c r="D215" s="13"/>
+    </row>
+    <row r="216" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A216" s="10"/>
+      <c r="B216" s="11"/>
+      <c r="C216" s="12"/>
+      <c r="D216" s="13"/>
+    </row>
+    <row r="217" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A217" s="10"/>
+      <c r="B217" s="11"/>
+      <c r="C217" s="12"/>
+      <c r="D217" s="13"/>
+    </row>
+    <row r="218" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A218" s="10"/>
+      <c r="B218" s="11"/>
+      <c r="C218" s="12"/>
+      <c r="D218" s="13"/>
+    </row>
+    <row r="219" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A219" s="10"/>
+      <c r="B219" s="11"/>
+      <c r="C219" s="12"/>
+      <c r="D219" s="13"/>
+    </row>
+    <row r="220" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A220" s="10"/>
+      <c r="B220" s="11"/>
+      <c r="C220" s="12"/>
+      <c r="D220" s="13"/>
+    </row>
+    <row r="221" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A221" s="10"/>
+      <c r="B221" s="11"/>
+      <c r="C221" s="12"/>
+      <c r="D221" s="13"/>
+    </row>
+    <row r="222" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A222" s="10"/>
+      <c r="B222" s="11"/>
+      <c r="C222" s="12"/>
+      <c r="D222" s="13"/>
+    </row>
+    <row r="223" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A223" s="10"/>
+      <c r="B223" s="11"/>
+      <c r="C223" s="12"/>
+      <c r="D223" s="13"/>
+    </row>
+    <row r="224" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A224" s="10"/>
+      <c r="B224" s="11"/>
+      <c r="C224" s="12"/>
+      <c r="D224" s="13"/>
+    </row>
+    <row r="225" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A225" s="10"/>
+      <c r="B225" s="11"/>
+      <c r="C225" s="12"/>
+      <c r="D225" s="13"/>
+    </row>
+    <row r="226" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A226" s="10"/>
+      <c r="B226" s="11"/>
+      <c r="C226" s="12"/>
+      <c r="D226" s="13"/>
+    </row>
+    <row r="227" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A227" s="10"/>
+      <c r="B227" s="11"/>
+      <c r="C227" s="12"/>
+      <c r="D227" s="13"/>
+    </row>
+    <row r="228" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A228" s="10"/>
+      <c r="B228" s="11"/>
+      <c r="C228" s="12"/>
+      <c r="D228" s="13"/>
+    </row>
+    <row r="229" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A229" s="10"/>
+      <c r="B229" s="11"/>
+      <c r="C229" s="12"/>
+      <c r="D229" s="13"/>
+    </row>
+    <row r="230" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A230" s="10"/>
+      <c r="B230" s="11"/>
+      <c r="C230" s="12"/>
+      <c r="D230" s="13"/>
+    </row>
+    <row r="231" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A231" s="10"/>
+      <c r="B231" s="11"/>
+      <c r="C231" s="12"/>
+      <c r="D231" s="13"/>
+    </row>
+    <row r="232" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A232" s="10"/>
+      <c r="B232" s="11"/>
+      <c r="C232" s="12"/>
+      <c r="D232" s="13"/>
+    </row>
+    <row r="233" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A233" s="10"/>
+      <c r="B233" s="11"/>
+      <c r="C233" s="12"/>
+      <c r="D233" s="13"/>
+    </row>
+    <row r="234" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A234" s="10"/>
+      <c r="B234" s="11"/>
+      <c r="C234" s="12"/>
+      <c r="D234" s="13"/>
+    </row>
+    <row r="235" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A235" s="10"/>
+      <c r="B235" s="11"/>
+      <c r="C235" s="12"/>
+      <c r="D235" s="13"/>
+    </row>
+    <row r="236" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A236" s="10"/>
+      <c r="B236" s="11"/>
+      <c r="C236" s="12"/>
+      <c r="D236" s="13"/>
+    </row>
+    <row r="237" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A237" s="10"/>
+      <c r="B237" s="11"/>
+      <c r="C237" s="12"/>
+      <c r="D237" s="13"/>
+    </row>
+    <row r="238" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A238" s="10"/>
+      <c r="B238" s="11"/>
+      <c r="C238" s="12"/>
+      <c r="D238" s="13"/>
+    </row>
+    <row r="239" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A239" s="10"/>
+      <c r="B239" s="11"/>
+      <c r="C239" s="12"/>
+      <c r="D239" s="13"/>
+    </row>
+    <row r="240" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A240" s="10"/>
+      <c r="B240" s="11"/>
+      <c r="C240" s="12"/>
+      <c r="D240" s="13"/>
+    </row>
+    <row r="241" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A241" s="10"/>
+      <c r="B241" s="11"/>
+      <c r="C241" s="12"/>
+      <c r="D241" s="13"/>
+    </row>
+    <row r="242" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A242" s="10"/>
+      <c r="B242" s="11"/>
+      <c r="C242" s="12"/>
+      <c r="D242" s="13"/>
+    </row>
+    <row r="243" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A243" s="10"/>
+      <c r="B243" s="11"/>
+      <c r="C243" s="12"/>
+      <c r="D243" s="13"/>
+    </row>
+    <row r="244" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A244" s="10"/>
+      <c r="B244" s="11"/>
+      <c r="C244" s="12"/>
+      <c r="D244" s="13"/>
+    </row>
+    <row r="245" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A245" s="10"/>
+      <c r="B245" s="11"/>
+      <c r="C245" s="12"/>
+      <c r="D245" s="13"/>
+    </row>
+    <row r="246" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A246" s="10"/>
+      <c r="B246" s="11"/>
+      <c r="C246" s="12"/>
+      <c r="D246" s="13"/>
+    </row>
+    <row r="247" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A247" s="10"/>
+      <c r="B247" s="11"/>
+      <c r="C247" s="12"/>
+      <c r="D247" s="13"/>
+    </row>
+    <row r="248" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A248" s="10"/>
+      <c r="B248" s="11"/>
+      <c r="C248" s="12"/>
+      <c r="D248" s="13"/>
+    </row>
+    <row r="249" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A249" s="10"/>
+      <c r="B249" s="11"/>
+      <c r="C249" s="12"/>
+      <c r="D249" s="13"/>
+    </row>
+    <row r="250" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A250" s="10"/>
+      <c r="B250" s="11"/>
+      <c r="C250" s="12"/>
+      <c r="D250" s="13"/>
+    </row>
+    <row r="251" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A251" s="10"/>
+      <c r="B251" s="11"/>
+      <c r="C251" s="12"/>
+      <c r="D251" s="13"/>
+    </row>
+    <row r="252" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A252" s="10"/>
+      <c r="B252" s="11"/>
+      <c r="C252" s="12"/>
+      <c r="D252" s="13"/>
+    </row>
+    <row r="253" spans="1:4" ht="409.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A253" s="10"/>
+      <c r="B253" s="11"/>
+      <c r="C253" s="12"/>
+      <c r="D253" s="13"/>
+    </row>
+    <row r="351" ht="218.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="352" ht="409.6" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Commit on 24.01.2019. Added code and answer explanations to questions up to 44th. Currently on the 45th.
</commit_message>
<xml_diff>
--- a/Exam Preparation/resources/70-480 Practice Exam Answers and Explanations.xlsx
+++ b/Exam Preparation/resources/70-480 Practice Exam Answers and Explanations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22264" windowHeight="12647"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="149">
   <si>
     <t>Question</t>
   </si>
@@ -455,6 +455,138 @@
   </si>
   <si>
     <t>My answer is correct.Answer explanation: According to the CSS box model each box has a content area and optional surrounding margin, border and padding areas.The content area is the innermost followed by padding border and margin areas.</t>
+  </si>
+  <si>
+    <t>35.You need to set the transperancy of the element to 80% and its background-color to red.</t>
+  </si>
+  <si>
+    <t>1. background-color: #FF0000; opacity: 0.2; 2. background: rgba(255, 0, 0, .2);</t>
+  </si>
+  <si>
+    <t>My answers were correct.Answers explanation: The first rule sets the background property by using the rgba function.This function allows you to specify the integer values for the red, green and blue components of the color as well as the alpha component that represents transparency.The red, green and blue component values can be a number between 0 and 255.The alpha component can be a number between 0 and 1 with the number 0 representing no opacity or full transperancy.The value 0.2 represents 20% opacity and or 80% transparency.The second rule sets the background-color property to a hexadecimal representation of the color.It also sets the opacity property to 0.2 representing 20% opacity or 80% transparency.The opacity property can be set to a number between 0 and 1 with the number 0 representing no opacity or full transparency.</t>
+  </si>
+  <si>
+    <t>36.You are using a div element to layout content.The layout of the div element must meet these requirements: *The total width must not exceed 250px; *A gray border must be displayed around the element; *The width and height of the border must be 5px; *The space between the border and its surrounding elements must be 10px;</t>
+  </si>
+  <si>
+    <t>div {
+    width: 220px;
+    border: solid 5px gray;
+    margin: 10px;
+}</t>
+  </si>
+  <si>
+    <t>My answer is correct.Answer explanation: The rule set sets the width property to 220px the border property to 5px and the margin to 10px.The margin is the space between the border of an element and the element's surrounding elements.Because there is a left border and a right border the total width taken up by the border is 10px.Because there is a left margin and a right margin the total width taken up by the margin is 20px.The width property specifies the width of the content area of the element.By setting the width property to 220px you generate a total width of 250px(220px + 10px + 20px).</t>
+  </si>
+  <si>
+    <t>37.You are using a div element to layout content.The layout of the div element must meet these requirements: *The total width of the div element must not exceed 300px; *A gray border must be displayed arround the element; *The width and height of the border must be 5px; *The space between the border and its surrounding elements must be 20px; *The space between the border and its content must be 10px;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+div {
+    width: 230px;
+    border: solid 5px gray;
+    margin: 20px;
+    padding: 10px;
+}</t>
+  </si>
+  <si>
+    <t>My answer is correct.Answer explanation: This rule set sets the the width property 230px the border property to 5px the margin to 20px and the padding to 10px.The margin is the space between the border of an element and the element's surrounding elements.The padding represents the space between the border of an element and the element's content.Because there is a left and right border the total width taken up by the border is 10pxBecause there is a left and right margin the total width taken up by the margin is 40px.Because there is a left and right padding the total width taken up by the padding is 20px.By setting the width property to 230px you generate a total width of 300px(230px + 10px + 40px + 20px).</t>
+  </si>
+  <si>
+    <t>38.There are three div elements in the web page.You want to programmatically hide the second div element.The position of the other two elements should not change as a consequence of hiding the second element.</t>
+  </si>
+  <si>
+    <t>1. div.style.opacity = 0; 2. div.style.visibility = "hidden";</t>
+  </si>
+  <si>
+    <t>My answers are correct.Answer explanation: Hiding an HTML element can be achieved using CSS properties: display, visibility and opacity.To hide an element you can set its visibility property to "hidden".When an element's opacity is set to 0 it is fully transparent and therefore also hidden.Both options will keep the space taken up by the element.By setting the display property to "none" the element will be hidden as well and it will no longer take up any space on the web page.</t>
+  </si>
+  <si>
+    <t>39.You are styling a button element on a web page.The element should be initially not visible and it should not take up any space on the page.</t>
+  </si>
+  <si>
+    <t>&lt;button style="display: none;" /&gt;</t>
+  </si>
+  <si>
+    <t>&lt;button style="visibility: hidden;" /&gt;</t>
+  </si>
+  <si>
+    <t>My answer is incorrect.Answer explanation: By setting the display style attribute to none you hide the button element and cause it to take up no space.</t>
+  </si>
+  <si>
+    <t>40.You are styling a button element on a web page.The element should be initially not visible but space should be reversed for the element in case it is dynamically shown.</t>
+  </si>
+  <si>
+    <t>&lt;button style="visibility:hidden;" /&gt;</t>
+  </si>
+  <si>
+    <t>My answer is incorrect. Answer explanation: This markup sets the visibility style attribute to hidden.This hides the element.Because the default display style attribute is set to inline the element takes up space even though it is hidden,.</t>
+  </si>
+  <si>
+    <t>41.You need to ensure that the Submit button is placed 50px to the right of the Cancel button regardless of where on the page the Cancel button exists.</t>
+  </si>
+  <si>
+    <t>Modify the Submit button as follows:                                                                                                                         &lt;button style="position: relative; left: 50px;"&gt;Submit&lt;/button&gt;</t>
+  </si>
+  <si>
+    <t>Modify the Submit button as follows:                                                                                                                         &lt;button style="position: absolute; left: 50px;"&gt;Submit&lt;/button&gt;</t>
+  </si>
+  <si>
+    <t>My answer is incorrect.Answer explanation:This markup positions the Submit button 50px to the right of the preceeding element which in this scenario is the Cancel button.By setting the position style attribute to relative you position the element relative to its preceeding element.By setting the left style attribute to 50px you specify that the left edge of the element should begin at 50px from the preceding element.</t>
+  </si>
+  <si>
+    <t>42.You need to programmatically ensure that the Finish button is placed 50px to the right of the Next button regardless of where on the page the Next button exists.</t>
+  </si>
+  <si>
+    <t>$("#finish").css({"position": "relative", "left": "50px"});</t>
+  </si>
+  <si>
+    <t>$("#finish").css({"position": "absolute", "left": "50px"});</t>
+  </si>
+  <si>
+    <t>My answer is incorrect. Answer explanation: This code positions the Finish button 50px to the right of the preceding element which in this scenario is the Next button.It uses the jQuery css function to accomplish this.By setting the position style attribute to relative you position the element relative to its preceding element.By setting the left style attribute to 50px you specify that the left edge of the element should begin at 50px from the preceding element.</t>
+  </si>
+  <si>
+    <t>43.You need to programmatically remove the button so that it does not take up any space on the page.</t>
+  </si>
+  <si>
+    <t>$("button").hide();</t>
+  </si>
+  <si>
+    <t>My answer is correct.Answer explanation: This code hides the element by setting its CSS display attribute to none.This ensures that the element becomes invisible and takes up no space.</t>
+  </si>
+  <si>
+    <t>44.You want to use jQuery to make an AJAX request to the web service so it does not block the code execution of other requests on the website.You need to ensure that the weather being displayed is always the latest information obtained from the web service.</t>
+  </si>
+  <si>
+    <t>$.ajax({
+    url: "Weather.asmx/GetWeather",
+    type: "POST",
+    async: true,
+    cache: false,
+    data: {"ZipCode": zipCode},
+    dataType: "html",
+    success: function (result) {
+        showWeather(result);
+    }
+});</t>
+  </si>
+  <si>
+    <t>$.ajax({
+   url: "Weather.asmx/GetWeather",
+   type: "POST",
+   async: true,
+   cache: true,
+   data: {"ZipCode": zipCode},
+   dataType: "html",
+   success: function (result) {
+       showWeather(result);
+   } 
+});</t>
+  </si>
+  <si>
+    <t>My answer is incorrect. Answer explanation: To ensure that the request does not block the execution of other requests it should be executed asynchronously so async should be set to "true".The value of cache should be set to "false" to prevent the browser from caching the result because you want to always display the latest weather information.You should also set the dataType to "html" because the web service provides information in this format.</t>
   </si>
 </sst>
 </file>
@@ -881,19 +1013,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D352"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="23.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="147.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="147.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="151" style="5" customWidth="1"/>
-    <col min="3" max="3" width="149.88671875" style="7" customWidth="1"/>
-    <col min="4" max="4" width="147" style="9" customWidth="1"/>
+    <col min="3" max="3" width="149.85546875" style="7" customWidth="1"/>
+    <col min="4" max="4" width="213.42578125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" ht="30.7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -907,7 +1039,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>3</v>
       </c>
@@ -915,7 +1047,7 @@
       <c r="C2" s="12"/>
       <c r="D2" s="13"/>
     </row>
-    <row r="3" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>4</v>
       </c>
@@ -927,7 +1059,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>7</v>
       </c>
@@ -939,7 +1071,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>11</v>
       </c>
@@ -951,7 +1083,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>14</v>
       </c>
@@ -959,7 +1091,7 @@
       <c r="C6" s="12"/>
       <c r="D6" s="13"/>
     </row>
-    <row r="7" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>15</v>
       </c>
@@ -971,7 +1103,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>18</v>
       </c>
@@ -983,7 +1115,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>20</v>
       </c>
@@ -995,7 +1127,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>22</v>
       </c>
@@ -1009,7 +1141,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>26</v>
       </c>
@@ -1023,7 +1155,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>30</v>
       </c>
@@ -1037,7 +1169,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>34</v>
       </c>
@@ -1049,7 +1181,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>37</v>
       </c>
@@ -1063,7 +1195,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>41</v>
       </c>
@@ -1075,7 +1207,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>44</v>
       </c>
@@ -1087,7 +1219,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>47</v>
       </c>
@@ -1101,7 +1233,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>51</v>
       </c>
@@ -1115,7 +1247,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>55</v>
       </c>
@@ -1127,7 +1259,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>58</v>
       </c>
@@ -1141,7 +1273,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>62</v>
       </c>
@@ -1155,7 +1287,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>66</v>
       </c>
@@ -1167,7 +1299,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>69</v>
       </c>
@@ -1179,7 +1311,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>72</v>
       </c>
@@ -1193,7 +1325,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>76</v>
       </c>
@@ -1205,7 +1337,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>79</v>
       </c>
@@ -1219,7 +1351,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
         <v>83</v>
       </c>
@@ -1231,7 +1363,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>86</v>
       </c>
@@ -1243,7 +1375,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
         <v>89</v>
       </c>
@@ -1253,7 +1385,7 @@
       <c r="C29" s="12"/>
       <c r="D29" s="13"/>
     </row>
-    <row r="30" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>91</v>
       </c>
@@ -1265,7 +1397,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
         <v>94</v>
       </c>
@@ -1277,7 +1409,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
         <v>97</v>
       </c>
@@ -1289,7 +1421,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
         <v>100</v>
       </c>
@@ -1301,7 +1433,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
         <v>103</v>
       </c>
@@ -1313,7 +1445,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
         <v>106</v>
       </c>
@@ -1325,7 +1457,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
         <v>109</v>
       </c>
@@ -1337,7 +1469,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
         <v>112</v>
       </c>
@@ -1349,1304 +1481,1374 @@
         <v>114</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="10"/>
-      <c r="B38" s="11"/>
+    <row r="38" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>116</v>
+      </c>
       <c r="C38" s="12"/>
-      <c r="D38" s="13"/>
-    </row>
-    <row r="39" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="10"/>
-      <c r="B39" s="11"/>
+      <c r="D38" s="13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>119</v>
+      </c>
       <c r="C39" s="12"/>
-      <c r="D39" s="13"/>
-    </row>
-    <row r="40" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="10"/>
-      <c r="B40" s="11"/>
+      <c r="D39" s="13" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>122</v>
+      </c>
       <c r="C40" s="12"/>
-      <c r="D40" s="13"/>
-    </row>
-    <row r="41" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="10"/>
-      <c r="B41" s="11"/>
+      <c r="D40" s="13" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>125</v>
+      </c>
       <c r="C41" s="12"/>
-      <c r="D41" s="13"/>
-    </row>
-    <row r="42" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="10"/>
-      <c r="B42" s="11"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="13"/>
-    </row>
-    <row r="43" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="10"/>
-      <c r="B43" s="11"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="13"/>
-    </row>
-    <row r="44" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="10"/>
-      <c r="B44" s="11"/>
-      <c r="C44" s="12"/>
-      <c r="D44" s="13"/>
-    </row>
-    <row r="45" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="10"/>
-      <c r="B45" s="11"/>
-      <c r="C45" s="12"/>
-      <c r="D45" s="13"/>
-    </row>
-    <row r="46" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="10"/>
-      <c r="B46" s="11"/>
+      <c r="D41" s="13" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="D42" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="D43" s="13" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="B44" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="D44" s="13" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="D45" s="13" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="B46" s="11" t="s">
+        <v>143</v>
+      </c>
       <c r="C46" s="12"/>
-      <c r="D46" s="13"/>
-    </row>
-    <row r="47" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="10"/>
-      <c r="B47" s="11"/>
-      <c r="C47" s="12"/>
-      <c r="D47" s="13"/>
-    </row>
-    <row r="48" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D46" s="13" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="D47" s="13" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="10"/>
       <c r="B48" s="11"/>
       <c r="C48" s="12"/>
       <c r="D48" s="13"/>
     </row>
-    <row r="49" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="10"/>
       <c r="B49" s="11"/>
       <c r="C49" s="12"/>
       <c r="D49" s="13"/>
     </row>
-    <row r="50" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="10"/>
       <c r="B50" s="11"/>
       <c r="C50" s="12"/>
       <c r="D50" s="13"/>
     </row>
-    <row r="51" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="10"/>
       <c r="B51" s="11"/>
       <c r="C51" s="12"/>
       <c r="D51" s="13"/>
     </row>
-    <row r="52" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="10"/>
       <c r="B52" s="11"/>
       <c r="C52" s="12"/>
       <c r="D52" s="13"/>
     </row>
-    <row r="53" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="10"/>
       <c r="B53" s="11"/>
       <c r="C53" s="12"/>
       <c r="D53" s="13"/>
     </row>
-    <row r="54" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="10"/>
       <c r="B54" s="11"/>
       <c r="C54" s="12"/>
       <c r="D54" s="13"/>
     </row>
-    <row r="55" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="10"/>
       <c r="B55" s="11"/>
       <c r="C55" s="12"/>
       <c r="D55" s="13"/>
     </row>
-    <row r="56" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="10"/>
       <c r="B56" s="11"/>
       <c r="C56" s="12"/>
       <c r="D56" s="13"/>
     </row>
-    <row r="57" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="10"/>
       <c r="B57" s="11"/>
       <c r="C57" s="12"/>
       <c r="D57" s="13"/>
     </row>
-    <row r="58" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="10"/>
       <c r="B58" s="11"/>
       <c r="C58" s="12"/>
       <c r="D58" s="13"/>
     </row>
-    <row r="59" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="10"/>
       <c r="B59" s="11"/>
       <c r="C59" s="12"/>
       <c r="D59" s="13"/>
     </row>
-    <row r="60" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="10"/>
       <c r="B60" s="11"/>
       <c r="C60" s="12"/>
       <c r="D60" s="13"/>
     </row>
-    <row r="61" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="10"/>
       <c r="B61" s="11"/>
       <c r="C61" s="12"/>
       <c r="D61" s="13"/>
     </row>
-    <row r="62" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="10"/>
       <c r="B62" s="11"/>
       <c r="C62" s="12"/>
       <c r="D62" s="13"/>
     </row>
-    <row r="63" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="10"/>
       <c r="B63" s="11"/>
       <c r="C63" s="12"/>
       <c r="D63" s="13"/>
     </row>
-    <row r="64" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="10"/>
       <c r="B64" s="11"/>
       <c r="C64" s="12"/>
       <c r="D64" s="13"/>
     </row>
-    <row r="65" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="10"/>
       <c r="B65" s="11"/>
       <c r="C65" s="12"/>
       <c r="D65" s="13"/>
     </row>
-    <row r="66" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="10"/>
       <c r="B66" s="11"/>
       <c r="C66" s="12"/>
       <c r="D66" s="13"/>
     </row>
-    <row r="67" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="10"/>
       <c r="B67" s="11"/>
       <c r="C67" s="12"/>
       <c r="D67" s="13"/>
     </row>
-    <row r="68" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="10"/>
       <c r="B68" s="11"/>
       <c r="C68" s="12"/>
       <c r="D68" s="13"/>
     </row>
-    <row r="69" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="10"/>
       <c r="B69" s="11"/>
       <c r="C69" s="12"/>
       <c r="D69" s="13"/>
     </row>
-    <row r="70" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="10"/>
       <c r="B70" s="11"/>
       <c r="C70" s="12"/>
       <c r="D70" s="13"/>
     </row>
-    <row r="71" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="10"/>
       <c r="B71" s="11"/>
       <c r="C71" s="12"/>
       <c r="D71" s="13"/>
     </row>
-    <row r="72" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="10"/>
       <c r="B72" s="11"/>
       <c r="C72" s="12"/>
       <c r="D72" s="13"/>
     </row>
-    <row r="73" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="10"/>
       <c r="B73" s="11"/>
       <c r="C73" s="12"/>
       <c r="D73" s="13"/>
     </row>
-    <row r="74" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="10"/>
       <c r="B74" s="11"/>
       <c r="C74" s="12"/>
       <c r="D74" s="13"/>
     </row>
-    <row r="75" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="10"/>
       <c r="B75" s="11"/>
       <c r="C75" s="12"/>
       <c r="D75" s="13"/>
     </row>
-    <row r="76" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="10"/>
       <c r="B76" s="11"/>
       <c r="C76" s="12"/>
       <c r="D76" s="13"/>
     </row>
-    <row r="77" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="10"/>
       <c r="B77" s="11"/>
       <c r="C77" s="12"/>
       <c r="D77" s="13"/>
     </row>
-    <row r="78" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="10"/>
       <c r="B78" s="11"/>
       <c r="C78" s="12"/>
       <c r="D78" s="13"/>
     </row>
-    <row r="79" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="10"/>
       <c r="B79" s="11"/>
       <c r="C79" s="12"/>
       <c r="D79" s="13"/>
     </row>
-    <row r="80" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="10"/>
       <c r="B80" s="11"/>
       <c r="C80" s="12"/>
       <c r="D80" s="13"/>
     </row>
-    <row r="81" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="10"/>
       <c r="B81" s="11"/>
       <c r="C81" s="12"/>
       <c r="D81" s="13"/>
     </row>
-    <row r="82" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="10"/>
       <c r="B82" s="11"/>
       <c r="C82" s="12"/>
       <c r="D82" s="13"/>
     </row>
-    <row r="83" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="10"/>
       <c r="B83" s="11"/>
       <c r="C83" s="12"/>
       <c r="D83" s="13"/>
     </row>
-    <row r="84" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="10"/>
       <c r="B84" s="11"/>
       <c r="C84" s="12"/>
       <c r="D84" s="13"/>
     </row>
-    <row r="85" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="10"/>
       <c r="B85" s="11"/>
       <c r="C85" s="12"/>
       <c r="D85" s="13"/>
     </row>
-    <row r="86" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="10"/>
       <c r="B86" s="11"/>
       <c r="C86" s="12"/>
       <c r="D86" s="13"/>
     </row>
-    <row r="87" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="10"/>
       <c r="B87" s="11"/>
       <c r="C87" s="12"/>
       <c r="D87" s="13"/>
     </row>
-    <row r="88" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="10"/>
       <c r="B88" s="11"/>
       <c r="C88" s="12"/>
       <c r="D88" s="13"/>
     </row>
-    <row r="89" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="10"/>
       <c r="B89" s="11"/>
       <c r="C89" s="12"/>
       <c r="D89" s="13"/>
     </row>
-    <row r="90" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="10"/>
       <c r="B90" s="11"/>
       <c r="C90" s="12"/>
       <c r="D90" s="13"/>
     </row>
-    <row r="91" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="10"/>
       <c r="B91" s="11"/>
       <c r="C91" s="12"/>
       <c r="D91" s="13"/>
     </row>
-    <row r="92" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="10"/>
       <c r="B92" s="11"/>
       <c r="C92" s="12"/>
       <c r="D92" s="13"/>
     </row>
-    <row r="93" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="10"/>
       <c r="B93" s="11"/>
       <c r="C93" s="12"/>
       <c r="D93" s="13"/>
     </row>
-    <row r="94" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="10"/>
       <c r="B94" s="11"/>
       <c r="C94" s="12"/>
       <c r="D94" s="13"/>
     </row>
-    <row r="95" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="10"/>
       <c r="B95" s="11"/>
       <c r="C95" s="12"/>
       <c r="D95" s="13"/>
     </row>
-    <row r="96" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="10"/>
       <c r="B96" s="11"/>
       <c r="C96" s="12"/>
       <c r="D96" s="13"/>
     </row>
-    <row r="97" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="10"/>
       <c r="B97" s="11"/>
       <c r="C97" s="12"/>
       <c r="D97" s="13"/>
     </row>
-    <row r="98" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="10"/>
       <c r="B98" s="11"/>
       <c r="C98" s="12"/>
       <c r="D98" s="13"/>
     </row>
-    <row r="99" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="10"/>
       <c r="B99" s="11"/>
       <c r="C99" s="12"/>
       <c r="D99" s="13"/>
     </row>
-    <row r="100" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="10"/>
       <c r="B100" s="11"/>
       <c r="C100" s="12"/>
       <c r="D100" s="13"/>
     </row>
-    <row r="101" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="10"/>
       <c r="B101" s="11"/>
       <c r="C101" s="12"/>
       <c r="D101" s="13"/>
     </row>
-    <row r="102" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="10"/>
       <c r="B102" s="11"/>
       <c r="C102" s="12"/>
       <c r="D102" s="13"/>
     </row>
-    <row r="103" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="10"/>
       <c r="B103" s="11"/>
       <c r="C103" s="12"/>
       <c r="D103" s="13"/>
     </row>
-    <row r="104" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="10"/>
       <c r="B104" s="11"/>
       <c r="C104" s="12"/>
       <c r="D104" s="13"/>
     </row>
-    <row r="105" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="10"/>
       <c r="B105" s="11"/>
       <c r="C105" s="12"/>
       <c r="D105" s="13"/>
     </row>
-    <row r="106" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="10"/>
       <c r="B106" s="11"/>
       <c r="C106" s="12"/>
       <c r="D106" s="13"/>
     </row>
-    <row r="107" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="10"/>
       <c r="B107" s="11"/>
       <c r="C107" s="12"/>
       <c r="D107" s="13"/>
     </row>
-    <row r="108" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="10"/>
       <c r="B108" s="11"/>
       <c r="C108" s="12"/>
       <c r="D108" s="13"/>
     </row>
-    <row r="109" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="10"/>
       <c r="B109" s="11"/>
       <c r="C109" s="12"/>
       <c r="D109" s="13"/>
     </row>
-    <row r="110" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="10"/>
       <c r="B110" s="11"/>
       <c r="C110" s="12"/>
       <c r="D110" s="13"/>
     </row>
-    <row r="111" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="10"/>
       <c r="B111" s="11"/>
       <c r="C111" s="12"/>
       <c r="D111" s="13"/>
     </row>
-    <row r="112" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="10"/>
       <c r="B112" s="11"/>
       <c r="C112" s="12"/>
       <c r="D112" s="13"/>
     </row>
-    <row r="113" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="10"/>
       <c r="B113" s="11"/>
       <c r="C113" s="12"/>
       <c r="D113" s="13"/>
     </row>
-    <row r="114" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="10"/>
       <c r="B114" s="11"/>
       <c r="C114" s="12"/>
       <c r="D114" s="13"/>
     </row>
-    <row r="115" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="10"/>
       <c r="B115" s="11"/>
       <c r="C115" s="12"/>
       <c r="D115" s="13"/>
     </row>
-    <row r="116" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="10"/>
       <c r="B116" s="11"/>
       <c r="C116" s="12"/>
       <c r="D116" s="13"/>
     </row>
-    <row r="117" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="10"/>
       <c r="B117" s="11"/>
       <c r="C117" s="12"/>
       <c r="D117" s="13"/>
     </row>
-    <row r="118" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="10"/>
       <c r="B118" s="11"/>
       <c r="C118" s="12"/>
       <c r="D118" s="13"/>
     </row>
-    <row r="119" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="10"/>
       <c r="B119" s="11"/>
       <c r="C119" s="12"/>
       <c r="D119" s="13"/>
     </row>
-    <row r="120" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="10"/>
       <c r="B120" s="11"/>
       <c r="C120" s="12"/>
       <c r="D120" s="13"/>
     </row>
-    <row r="121" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="10"/>
       <c r="B121" s="11"/>
       <c r="C121" s="12"/>
       <c r="D121" s="13"/>
     </row>
-    <row r="122" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="10"/>
       <c r="B122" s="11"/>
       <c r="C122" s="12"/>
       <c r="D122" s="13"/>
     </row>
-    <row r="123" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="10"/>
       <c r="B123" s="11"/>
       <c r="C123" s="12"/>
       <c r="D123" s="13"/>
     </row>
-    <row r="124" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="10"/>
       <c r="B124" s="11"/>
       <c r="C124" s="12"/>
       <c r="D124" s="13"/>
     </row>
-    <row r="125" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="10"/>
       <c r="B125" s="11"/>
       <c r="C125" s="12"/>
       <c r="D125" s="13"/>
     </row>
-    <row r="126" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="10"/>
       <c r="B126" s="11"/>
       <c r="C126" s="12"/>
       <c r="D126" s="13"/>
     </row>
-    <row r="127" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="10"/>
       <c r="B127" s="11"/>
       <c r="C127" s="12"/>
       <c r="D127" s="13"/>
     </row>
-    <row r="128" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="10"/>
       <c r="B128" s="11"/>
       <c r="C128" s="12"/>
       <c r="D128" s="13"/>
     </row>
-    <row r="129" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="10"/>
       <c r="B129" s="11"/>
       <c r="C129" s="12"/>
       <c r="D129" s="13"/>
     </row>
-    <row r="130" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="10"/>
       <c r="B130" s="11"/>
       <c r="C130" s="12"/>
       <c r="D130" s="13"/>
     </row>
-    <row r="131" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="10"/>
       <c r="B131" s="11"/>
       <c r="C131" s="12"/>
       <c r="D131" s="13"/>
     </row>
-    <row r="132" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="10"/>
       <c r="B132" s="11"/>
       <c r="C132" s="12"/>
       <c r="D132" s="13"/>
     </row>
-    <row r="133" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="10"/>
       <c r="B133" s="11"/>
       <c r="C133" s="12"/>
       <c r="D133" s="13"/>
     </row>
-    <row r="134" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="10"/>
       <c r="B134" s="11"/>
       <c r="C134" s="12"/>
       <c r="D134" s="13"/>
     </row>
-    <row r="135" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="10"/>
       <c r="B135" s="11"/>
       <c r="C135" s="12"/>
       <c r="D135" s="13"/>
     </row>
-    <row r="136" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="10"/>
       <c r="B136" s="11"/>
       <c r="C136" s="12"/>
       <c r="D136" s="13"/>
     </row>
-    <row r="137" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="10"/>
       <c r="B137" s="11"/>
       <c r="C137" s="12"/>
       <c r="D137" s="13"/>
     </row>
-    <row r="138" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="10"/>
       <c r="B138" s="11"/>
       <c r="C138" s="12"/>
       <c r="D138" s="13"/>
     </row>
-    <row r="139" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="10"/>
       <c r="B139" s="11"/>
       <c r="C139" s="12"/>
       <c r="D139" s="13"/>
     </row>
-    <row r="140" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="10"/>
       <c r="B140" s="11"/>
       <c r="C140" s="12"/>
       <c r="D140" s="13"/>
     </row>
-    <row r="141" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="10"/>
       <c r="B141" s="11"/>
       <c r="C141" s="12"/>
       <c r="D141" s="13"/>
     </row>
-    <row r="142" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="10"/>
       <c r="B142" s="11"/>
       <c r="C142" s="12"/>
       <c r="D142" s="13"/>
     </row>
-    <row r="143" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="10"/>
       <c r="B143" s="11"/>
       <c r="C143" s="12"/>
       <c r="D143" s="13"/>
     </row>
-    <row r="144" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="10"/>
       <c r="B144" s="11"/>
       <c r="C144" s="12"/>
       <c r="D144" s="13"/>
     </row>
-    <row r="145" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="10"/>
       <c r="B145" s="11"/>
       <c r="C145" s="12"/>
       <c r="D145" s="13"/>
     </row>
-    <row r="146" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="10"/>
       <c r="B146" s="11"/>
       <c r="C146" s="12"/>
       <c r="D146" s="13"/>
     </row>
-    <row r="147" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="10"/>
       <c r="B147" s="11"/>
       <c r="C147" s="12"/>
       <c r="D147" s="13"/>
     </row>
-    <row r="148" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="10"/>
       <c r="B148" s="11"/>
       <c r="C148" s="12"/>
       <c r="D148" s="13"/>
     </row>
-    <row r="149" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="10"/>
       <c r="B149" s="11"/>
       <c r="C149" s="12"/>
       <c r="D149" s="13"/>
     </row>
-    <row r="150" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="10"/>
       <c r="B150" s="11"/>
       <c r="C150" s="12"/>
       <c r="D150" s="13"/>
     </row>
-    <row r="151" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="10"/>
       <c r="B151" s="11"/>
       <c r="C151" s="12"/>
       <c r="D151" s="13"/>
     </row>
-    <row r="152" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="10"/>
       <c r="B152" s="11"/>
       <c r="C152" s="12"/>
       <c r="D152" s="13"/>
     </row>
-    <row r="153" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="10"/>
       <c r="B153" s="11"/>
       <c r="C153" s="12"/>
       <c r="D153" s="13"/>
     </row>
-    <row r="154" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="10"/>
       <c r="B154" s="11"/>
       <c r="C154" s="12"/>
       <c r="D154" s="13"/>
     </row>
-    <row r="155" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="10"/>
       <c r="B155" s="11"/>
       <c r="C155" s="12"/>
       <c r="D155" s="13"/>
     </row>
-    <row r="156" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="10"/>
       <c r="B156" s="11"/>
       <c r="C156" s="12"/>
       <c r="D156" s="13"/>
     </row>
-    <row r="157" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="10"/>
       <c r="B157" s="11"/>
       <c r="C157" s="12"/>
       <c r="D157" s="13"/>
     </row>
-    <row r="158" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="10"/>
       <c r="B158" s="11"/>
       <c r="C158" s="12"/>
       <c r="D158" s="13"/>
     </row>
-    <row r="159" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="10"/>
       <c r="B159" s="11"/>
       <c r="C159" s="12"/>
       <c r="D159" s="13"/>
     </row>
-    <row r="160" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="10"/>
       <c r="B160" s="11"/>
       <c r="C160" s="12"/>
       <c r="D160" s="13"/>
     </row>
-    <row r="161" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="10"/>
       <c r="B161" s="11"/>
       <c r="C161" s="12"/>
       <c r="D161" s="13"/>
     </row>
-    <row r="162" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="10"/>
       <c r="B162" s="11"/>
       <c r="C162" s="12"/>
       <c r="D162" s="13"/>
     </row>
-    <row r="163" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="10"/>
       <c r="B163" s="11"/>
       <c r="C163" s="12"/>
       <c r="D163" s="13"/>
     </row>
-    <row r="164" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="10"/>
       <c r="B164" s="11"/>
       <c r="C164" s="12"/>
       <c r="D164" s="13"/>
     </row>
-    <row r="165" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="10"/>
       <c r="B165" s="11"/>
       <c r="C165" s="12"/>
       <c r="D165" s="13"/>
     </row>
-    <row r="166" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="10"/>
       <c r="B166" s="11"/>
       <c r="C166" s="12"/>
       <c r="D166" s="13"/>
     </row>
-    <row r="167" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="10"/>
       <c r="B167" s="11"/>
       <c r="C167" s="12"/>
       <c r="D167" s="13"/>
     </row>
-    <row r="168" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="10"/>
       <c r="B168" s="11"/>
       <c r="C168" s="12"/>
       <c r="D168" s="13"/>
     </row>
-    <row r="169" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="10"/>
       <c r="B169" s="11"/>
       <c r="C169" s="12"/>
       <c r="D169" s="13"/>
     </row>
-    <row r="170" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="10"/>
       <c r="B170" s="11"/>
       <c r="C170" s="12"/>
       <c r="D170" s="13"/>
     </row>
-    <row r="171" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="10"/>
       <c r="B171" s="11"/>
       <c r="C171" s="12"/>
       <c r="D171" s="13"/>
     </row>
-    <row r="172" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="10"/>
       <c r="B172" s="11"/>
       <c r="C172" s="12"/>
       <c r="D172" s="13"/>
     </row>
-    <row r="173" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="10"/>
       <c r="B173" s="11"/>
       <c r="C173" s="12"/>
       <c r="D173" s="13"/>
     </row>
-    <row r="174" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="10"/>
       <c r="B174" s="11"/>
       <c r="C174" s="12"/>
       <c r="D174" s="13"/>
     </row>
-    <row r="175" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="10"/>
       <c r="B175" s="11"/>
       <c r="C175" s="12"/>
       <c r="D175" s="13"/>
     </row>
-    <row r="176" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="10"/>
       <c r="B176" s="11"/>
       <c r="C176" s="12"/>
       <c r="D176" s="13"/>
     </row>
-    <row r="177" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="10"/>
       <c r="B177" s="11"/>
       <c r="C177" s="12"/>
       <c r="D177" s="13"/>
     </row>
-    <row r="178" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="10"/>
       <c r="B178" s="11"/>
       <c r="C178" s="12"/>
       <c r="D178" s="13"/>
     </row>
-    <row r="179" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="10"/>
       <c r="B179" s="11"/>
       <c r="C179" s="12"/>
       <c r="D179" s="13"/>
     </row>
-    <row r="180" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="10"/>
       <c r="B180" s="11"/>
       <c r="C180" s="12"/>
       <c r="D180" s="13"/>
     </row>
-    <row r="181" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="10"/>
       <c r="B181" s="11"/>
       <c r="C181" s="12"/>
       <c r="D181" s="13"/>
     </row>
-    <row r="182" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="10"/>
       <c r="B182" s="11"/>
       <c r="C182" s="12"/>
       <c r="D182" s="13"/>
     </row>
-    <row r="183" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="10"/>
       <c r="B183" s="11"/>
       <c r="C183" s="12"/>
       <c r="D183" s="13"/>
     </row>
-    <row r="184" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="10"/>
       <c r="B184" s="11"/>
       <c r="C184" s="12"/>
       <c r="D184" s="13"/>
     </row>
-    <row r="185" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="10"/>
       <c r="B185" s="11"/>
       <c r="C185" s="12"/>
       <c r="D185" s="13"/>
     </row>
-    <row r="186" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="10"/>
       <c r="B186" s="11"/>
       <c r="C186" s="12"/>
       <c r="D186" s="13"/>
     </row>
-    <row r="187" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="10"/>
       <c r="B187" s="11"/>
       <c r="C187" s="12"/>
       <c r="D187" s="13"/>
     </row>
-    <row r="188" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="10"/>
       <c r="B188" s="11"/>
       <c r="C188" s="12"/>
       <c r="D188" s="13"/>
     </row>
-    <row r="189" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="10"/>
       <c r="B189" s="11"/>
       <c r="C189" s="12"/>
       <c r="D189" s="13"/>
     </row>
-    <row r="190" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="10"/>
       <c r="B190" s="11"/>
       <c r="C190" s="12"/>
       <c r="D190" s="13"/>
     </row>
-    <row r="191" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="10"/>
       <c r="B191" s="11"/>
       <c r="C191" s="12"/>
       <c r="D191" s="13"/>
     </row>
-    <row r="192" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="10"/>
       <c r="B192" s="11"/>
       <c r="C192" s="12"/>
       <c r="D192" s="13"/>
     </row>
-    <row r="193" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="10"/>
       <c r="B193" s="11"/>
       <c r="C193" s="12"/>
       <c r="D193" s="13"/>
     </row>
-    <row r="194" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="10"/>
       <c r="B194" s="11"/>
       <c r="C194" s="12"/>
       <c r="D194" s="13"/>
     </row>
-    <row r="195" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="10"/>
       <c r="B195" s="11"/>
       <c r="C195" s="12"/>
       <c r="D195" s="13"/>
     </row>
-    <row r="196" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="10"/>
       <c r="B196" s="11"/>
       <c r="C196" s="12"/>
       <c r="D196" s="13"/>
     </row>
-    <row r="197" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="10"/>
       <c r="B197" s="11"/>
       <c r="C197" s="12"/>
       <c r="D197" s="13"/>
     </row>
-    <row r="198" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="10"/>
       <c r="B198" s="11"/>
       <c r="C198" s="12"/>
       <c r="D198" s="13"/>
     </row>
-    <row r="199" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="10"/>
       <c r="B199" s="11"/>
       <c r="C199" s="12"/>
       <c r="D199" s="13"/>
     </row>
-    <row r="200" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" s="10"/>
       <c r="B200" s="11"/>
       <c r="C200" s="12"/>
       <c r="D200" s="13"/>
     </row>
-    <row r="201" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" s="10"/>
       <c r="B201" s="11"/>
       <c r="C201" s="12"/>
       <c r="D201" s="13"/>
     </row>
-    <row r="202" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="10"/>
       <c r="B202" s="11"/>
       <c r="C202" s="12"/>
       <c r="D202" s="13"/>
     </row>
-    <row r="203" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" s="10"/>
       <c r="B203" s="11"/>
       <c r="C203" s="12"/>
       <c r="D203" s="13"/>
     </row>
-    <row r="204" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="10"/>
       <c r="B204" s="11"/>
       <c r="C204" s="12"/>
       <c r="D204" s="13"/>
     </row>
-    <row r="205" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="10"/>
       <c r="B205" s="11"/>
       <c r="C205" s="12"/>
       <c r="D205" s="13"/>
     </row>
-    <row r="206" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="10"/>
       <c r="B206" s="11"/>
       <c r="C206" s="12"/>
       <c r="D206" s="13"/>
     </row>
-    <row r="207" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A207" s="10"/>
       <c r="B207" s="11"/>
       <c r="C207" s="12"/>
       <c r="D207" s="13"/>
     </row>
-    <row r="208" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A208" s="10"/>
       <c r="B208" s="11"/>
       <c r="C208" s="12"/>
       <c r="D208" s="13"/>
     </row>
-    <row r="209" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A209" s="10"/>
       <c r="B209" s="11"/>
       <c r="C209" s="12"/>
       <c r="D209" s="13"/>
     </row>
-    <row r="210" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="10"/>
       <c r="B210" s="11"/>
       <c r="C210" s="12"/>
       <c r="D210" s="13"/>
     </row>
-    <row r="211" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="10"/>
       <c r="B211" s="11"/>
       <c r="C211" s="12"/>
       <c r="D211" s="13"/>
     </row>
-    <row r="212" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="10"/>
       <c r="B212" s="11"/>
       <c r="C212" s="12"/>
       <c r="D212" s="13"/>
     </row>
-    <row r="213" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="10"/>
       <c r="B213" s="11"/>
       <c r="C213" s="12"/>
       <c r="D213" s="13"/>
     </row>
-    <row r="214" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A214" s="10"/>
       <c r="B214" s="11"/>
       <c r="C214" s="12"/>
       <c r="D214" s="13"/>
     </row>
-    <row r="215" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A215" s="10"/>
       <c r="B215" s="11"/>
       <c r="C215" s="12"/>
       <c r="D215" s="13"/>
     </row>
-    <row r="216" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A216" s="10"/>
       <c r="B216" s="11"/>
       <c r="C216" s="12"/>
       <c r="D216" s="13"/>
     </row>
-    <row r="217" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A217" s="10"/>
       <c r="B217" s="11"/>
       <c r="C217" s="12"/>
       <c r="D217" s="13"/>
     </row>
-    <row r="218" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" s="10"/>
       <c r="B218" s="11"/>
       <c r="C218" s="12"/>
       <c r="D218" s="13"/>
     </row>
-    <row r="219" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A219" s="10"/>
       <c r="B219" s="11"/>
       <c r="C219" s="12"/>
       <c r="D219" s="13"/>
     </row>
-    <row r="220" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A220" s="10"/>
       <c r="B220" s="11"/>
       <c r="C220" s="12"/>
       <c r="D220" s="13"/>
     </row>
-    <row r="221" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A221" s="10"/>
       <c r="B221" s="11"/>
       <c r="C221" s="12"/>
       <c r="D221" s="13"/>
     </row>
-    <row r="222" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="10"/>
       <c r="B222" s="11"/>
       <c r="C222" s="12"/>
       <c r="D222" s="13"/>
     </row>
-    <row r="223" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="10"/>
       <c r="B223" s="11"/>
       <c r="C223" s="12"/>
       <c r="D223" s="13"/>
     </row>
-    <row r="224" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="10"/>
       <c r="B224" s="11"/>
       <c r="C224" s="12"/>
       <c r="D224" s="13"/>
     </row>
-    <row r="225" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A225" s="10"/>
       <c r="B225" s="11"/>
       <c r="C225" s="12"/>
       <c r="D225" s="13"/>
     </row>
-    <row r="226" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="10"/>
       <c r="B226" s="11"/>
       <c r="C226" s="12"/>
       <c r="D226" s="13"/>
     </row>
-    <row r="227" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A227" s="10"/>
       <c r="B227" s="11"/>
       <c r="C227" s="12"/>
       <c r="D227" s="13"/>
     </row>
-    <row r="228" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A228" s="10"/>
       <c r="B228" s="11"/>
       <c r="C228" s="12"/>
       <c r="D228" s="13"/>
     </row>
-    <row r="229" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A229" s="10"/>
       <c r="B229" s="11"/>
       <c r="C229" s="12"/>
       <c r="D229" s="13"/>
     </row>
-    <row r="230" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230" s="10"/>
       <c r="B230" s="11"/>
       <c r="C230" s="12"/>
       <c r="D230" s="13"/>
     </row>
-    <row r="231" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A231" s="10"/>
       <c r="B231" s="11"/>
       <c r="C231" s="12"/>
       <c r="D231" s="13"/>
     </row>
-    <row r="232" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A232" s="10"/>
       <c r="B232" s="11"/>
       <c r="C232" s="12"/>
       <c r="D232" s="13"/>
     </row>
-    <row r="233" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A233" s="10"/>
       <c r="B233" s="11"/>
       <c r="C233" s="12"/>
       <c r="D233" s="13"/>
     </row>
-    <row r="234" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A234" s="10"/>
       <c r="B234" s="11"/>
       <c r="C234" s="12"/>
       <c r="D234" s="13"/>
     </row>
-    <row r="235" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A235" s="10"/>
       <c r="B235" s="11"/>
       <c r="C235" s="12"/>
       <c r="D235" s="13"/>
     </row>
-    <row r="236" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A236" s="10"/>
       <c r="B236" s="11"/>
       <c r="C236" s="12"/>
       <c r="D236" s="13"/>
     </row>
-    <row r="237" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A237" s="10"/>
       <c r="B237" s="11"/>
       <c r="C237" s="12"/>
       <c r="D237" s="13"/>
     </row>
-    <row r="238" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A238" s="10"/>
       <c r="B238" s="11"/>
       <c r="C238" s="12"/>
       <c r="D238" s="13"/>
     </row>
-    <row r="239" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A239" s="10"/>
       <c r="B239" s="11"/>
       <c r="C239" s="12"/>
       <c r="D239" s="13"/>
     </row>
-    <row r="240" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A240" s="10"/>
       <c r="B240" s="11"/>
       <c r="C240" s="12"/>
       <c r="D240" s="13"/>
     </row>
-    <row r="241" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A241" s="10"/>
       <c r="B241" s="11"/>
       <c r="C241" s="12"/>
       <c r="D241" s="13"/>
     </row>
-    <row r="242" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A242" s="10"/>
       <c r="B242" s="11"/>
       <c r="C242" s="12"/>
       <c r="D242" s="13"/>
     </row>
-    <row r="243" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A243" s="10"/>
       <c r="B243" s="11"/>
       <c r="C243" s="12"/>
       <c r="D243" s="13"/>
     </row>
-    <row r="244" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A244" s="10"/>
       <c r="B244" s="11"/>
       <c r="C244" s="12"/>
       <c r="D244" s="13"/>
     </row>
-    <row r="245" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A245" s="10"/>
       <c r="B245" s="11"/>
       <c r="C245" s="12"/>
       <c r="D245" s="13"/>
     </row>
-    <row r="246" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A246" s="10"/>
       <c r="B246" s="11"/>
       <c r="C246" s="12"/>
       <c r="D246" s="13"/>
     </row>
-    <row r="247" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A247" s="10"/>
       <c r="B247" s="11"/>
       <c r="C247" s="12"/>
       <c r="D247" s="13"/>
     </row>
-    <row r="248" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A248" s="10"/>
       <c r="B248" s="11"/>
       <c r="C248" s="12"/>
       <c r="D248" s="13"/>
     </row>
-    <row r="249" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A249" s="10"/>
       <c r="B249" s="11"/>
       <c r="C249" s="12"/>
       <c r="D249" s="13"/>
     </row>
-    <row r="250" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A250" s="10"/>
       <c r="B250" s="11"/>
       <c r="C250" s="12"/>
       <c r="D250" s="13"/>
     </row>
-    <row r="251" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A251" s="10"/>
       <c r="B251" s="11"/>
       <c r="C251" s="12"/>
       <c r="D251" s="13"/>
     </row>
-    <row r="252" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A252" s="10"/>
       <c r="B252" s="11"/>
       <c r="C252" s="12"/>
       <c r="D252" s="13"/>
     </row>
-    <row r="253" spans="1:4" ht="409.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:4" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A253" s="10"/>
       <c r="B253" s="11"/>
       <c r="C253" s="12"/>
       <c r="D253" s="13"/>
     </row>
-    <row r="351" ht="218.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="352" ht="409.6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="351" ht="218.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="352" ht="409.6" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Commit on 24.01.2019. Added code and answer explanations to questions up to 50th. Currently on the 51th.
</commit_message>
<xml_diff>
--- a/Exam Preparation/resources/70-480 Practice Exam Answers and Explanations.xlsx
+++ b/Exam Preparation/resources/70-480 Practice Exam Answers and Explanations.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="170">
   <si>
     <t>Question</t>
   </si>
@@ -587,6 +587,95 @@
   </si>
   <si>
     <t>My answer is incorrect. Answer explanation: To ensure that the request does not block the execution of other requests it should be executed asynchronously so async should be set to "true".The value of cache should be set to "false" to prevent the browser from caching the result because you want to always display the latest weather information.You should also set the dataType to "html" because the web service provides information in this format.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">45.You are creating an online chat room using HTML WebSocket API.You want to receive WebSocket messages.Which event type should you listen to? </t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>My answer is correct. Answer explanation: You should use the message event.Event message occurs when  the client receives data from the web socket.</t>
+  </si>
+  <si>
+    <t>46.You need to use jQuery ajax function to invoke the web service for exam number 70-480 and display the price as an alert message.</t>
+  </si>
+  <si>
+    <t>$.ajax({
+    url: "http://services.measureup.com/Exam",
+    type: "GET",
+    data: {examNumber: "70-480"},
+    contentType: "application/json; charset=utf-8",
+    dataType: "json",
+    success: function (result) {
+        window.alert(result.price);
+    }
+});</t>
+  </si>
+  <si>
+    <t>My answer is correct. Answer explanation: The ajax function accepts a set of key-value pairs that specify the settings for an Asynchronous JavaScript and XML(AJAX) request.The dataType setting specifies the type of data returned from the web service.In this scenario the data type returned is JavaScript Object Notation(JSON).The success setting specifies a callback function to execute if the request is successful.The first parameter of the callback function is an object that represents the data returned.The object is formatted according to the type specified by the dataType setting.</t>
+  </si>
+  <si>
+    <t>var socket = new WebSocket("wss://ChatService");
+socket.onmessage = function (event) {
+    document.writeln(event.data);
+};</t>
+  </si>
+  <si>
+    <t>var socket = new WebSocket("wss://ChatService");
+socket.send("{document.writeln(socket.bufferedAmount)}");</t>
+  </si>
+  <si>
+    <t>47.You need to implement a callback to write a message to the browser when it is received from the server.</t>
+  </si>
+  <si>
+    <t>My answer is incorrect. Answer explanation: This code uses an anonymous function as a callback to handle the onmessage event of the WebSocket object.This event is raised when a message is received.The callback function accepts an event object as a parameter.The data property of the event object represents the message that is received.</t>
+  </si>
+  <si>
+    <t>48.You need to call the GetCurrentLocation and implement callbacks to display the position if the position is found or to display the error message if the position is not found.</t>
+  </si>
+  <si>
+    <t>GetCurrentLocation(
+    function (position) {
+        alert(position);
+    },
+    function (error) {
+        alert(error);
+    }
+);</t>
+  </si>
+  <si>
+    <t>function onSuccess(position) {
+    alert(position);
+}
+function onError(error) {
+    alert(error);
+}
+GetCurrentLocation(onSuccess(), onError());</t>
+  </si>
+  <si>
+    <t>My answer is incorrect.Answer explanation: The GetCurrentLocation function accepts two parameters.The first is a reference to a callback function that is called if a position is successfully obtained.The second is a reference to a callback function that is called if a position is not obtained.The signature of each function takes one parameter as indicated in the body of the GetCurrentLocation function.This code uses anonymous functions as the callback functions.</t>
+  </si>
+  <si>
+    <t>49.You need to modify the markup so that the alert message correctly displays the value of the speed variable.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Replace the line 11 with this code:  window.alert(newSpeed);   2. Add this code between lines 08 and 09: var newSpeed = this.speed;                                                                                  </t>
+  </si>
+  <si>
+    <t>Add this code between lines 01 and 02: var newSpeed = 0;</t>
+  </si>
+  <si>
+    <t>My answer is incorrect.Answer explanation: 1.This code defines a new local variable named newSpeed that is equal to the speed variable associated with the function. 2. This code uses the newSpeed variable to display the message.This is necessary because the previous code uses the "this" keyword to refer to the speed variable.However the speed variable is not available in the context of the anonymous function because it was declared in a different scope.To make a variable available to an anonymous function you should create a new local variable.</t>
+  </si>
+  <si>
+    <t>50.You need to call the Hide function to an object named button and display a message box after the object is hidden.</t>
+  </si>
+  <si>
+    <t>Hide(button, function() {alert("Hidden");});</t>
+  </si>
+  <si>
+    <t>My answer is correct.Answer explanation: The Hide function accepts two parameters.The first parameter is an object reference of the element to be hidden.The second parameter is the callback.If you examine the signature of the callback it is called with no parameters.Therefore you should pass an annonymous function with zero parameters as the second parameter to the Hide function.</t>
   </si>
 </sst>
 </file>
@@ -1013,8 +1102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D352"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.25"/>
@@ -1612,43 +1701,87 @@
       </c>
     </row>
     <row r="48" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="10"/>
-      <c r="B48" s="11"/>
+      <c r="A48" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="B48" s="11" t="s">
+        <v>150</v>
+      </c>
       <c r="C48" s="12"/>
-      <c r="D48" s="13"/>
+      <c r="D48" s="13" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="49" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="10"/>
-      <c r="B49" s="11"/>
+      <c r="A49" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="B49" s="11" t="s">
+        <v>153</v>
+      </c>
       <c r="C49" s="12"/>
-      <c r="D49" s="13"/>
+      <c r="D49" s="13" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="50" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="10"/>
-      <c r="B50" s="11"/>
-      <c r="C50" s="12"/>
-      <c r="D50" s="13"/>
+      <c r="A50" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="B50" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="C50" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="D50" s="13" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="51" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="10"/>
-      <c r="B51" s="11"/>
-      <c r="C51" s="12"/>
-      <c r="D51" s="13"/>
+      <c r="A51" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="B51" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="C51" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="D51" s="13" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="52" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="10"/>
-      <c r="B52" s="11"/>
-      <c r="C52" s="12"/>
-      <c r="D52" s="13"/>
+      <c r="A52" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="B52" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="C52" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="D52" s="13" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="53" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="10"/>
-      <c r="B53" s="11"/>
+      <c r="A53" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="B53" s="11" t="s">
+        <v>168</v>
+      </c>
       <c r="C53" s="12"/>
-      <c r="D53" s="13"/>
+      <c r="D53" s="13" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="54" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="10"/>
+      <c r="A54" s="10">
+        <v>51</v>
+      </c>
       <c r="B54" s="11"/>
       <c r="C54" s="12"/>
       <c r="D54" s="13"/>

</xml_diff>

<commit_message>
Commit on 25.01.2019. Added code and answer explanations to questions up to 65th. Currently on the 66th.
</commit_message>
<xml_diff>
--- a/Exam Preparation/resources/70-480 Practice Exam Answers and Explanations.xlsx
+++ b/Exam Preparation/resources/70-480 Practice Exam Answers and Explanations.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="220">
   <si>
     <t>Question</t>
   </si>
@@ -676,6 +676,220 @@
   </si>
   <si>
     <t>My answer is correct.Answer explanation: The Hide function accepts two parameters.The first parameter is an object reference of the element to be hidden.The second parameter is the callback.If you examine the signature of the callback it is called with no parameters.Therefore you should pass an annonymous function with zero parameters as the second parameter to the Hide function.</t>
+  </si>
+  <si>
+    <t>51.You use the HTML5 API to determine the current location of the user.</t>
+  </si>
+  <si>
+    <t>if (navigator.geolocation) {
+    navigator.geolocation.getCurrentPosition(function (position) {
+        var latitude = position.coords.latitude;
+        var longitude = position.coords.longitude;
+        // query database to find the nearest petrol station.
+    });
+}</t>
+  </si>
+  <si>
+    <t>My answer is correct.Answer explanation:The HTML Geolocation API introduced the geolocation property of the navigator object.To check if the browser is compaitable with the Geolocation API you can use if(navigator.geolocation) {}.The window.location object refers to the current page address (URL) instead of the geographical location of the user/device.To get the current position you should call the navigator.geolocation.getCurrentPosition() method and a position object is returned in the callback.The coords attribute contains the geographical coordinates which include the latitude, longitude, altitude, speed, etc.</t>
+  </si>
+  <si>
+    <t>52.You are using the Geolocation application programming interface (API) to determine a user's location.You need to retrieve the latitude and longitude coordinates.</t>
+  </si>
+  <si>
+    <t>window.navigator.geolocation.getCurrentPosition(function (position) {
+    var latitude = position.coords.latitude;
+    var longitude = position.coords.longitude;
+});</t>
+  </si>
+  <si>
+    <t>My answer is correct.Answer explanation: The Geolocation API starts with the geolocation object.You can reference this object by accessing the geolocation property of the navigator object which represents the client as a browser.The getCurrentPosition function of the geolocation object accepts a callback function as its first parameter.This function is called if the geographic position is successfully obtained.The signature of the callback function must contain one parameter that represents a position object.The coords property of the position object returns a reference to a coordinates object that specifies the geographic information about the position.The coordinates object contains two properties named latitude and longitude that represent the position's latitude and langitude respectively.</t>
+  </si>
+  <si>
+    <t>53.A web page needs to store data for its users.The storage mechanism must meet these requirements: *It must allow data storage of up to 1MB. *The data must be retrievable after the user closes and reopens the browser. *The data must not be transmited to the Web server.</t>
+  </si>
+  <si>
+    <t>Local Storage</t>
+  </si>
+  <si>
+    <t>My answer is correct. Answer explanation: You should use the local storage.Local storage allows you to store up to 10MB of data on the client.The data is not automatically transmitted to the Web server with each browser request.When you close and reopen the browser the data is still retrievable.You access local storage through the localStorage property of the window object.</t>
+  </si>
+  <si>
+    <t>53.You are creating web site that uses the Application Cache API.You must ensure that resources named Main.js and Main.css are cached.You must ensure that Functions.js is never cached.</t>
+  </si>
+  <si>
+    <t>CACHE MANIFEST
+CACHE:
+Main.js
+Main.css
+FALLBACK:
+Functions.js</t>
+  </si>
+  <si>
+    <t>CACHE MANIFEST
+Main.js
+Main.css
+NETWORK:
+Functions.js</t>
+  </si>
+  <si>
+    <t>My answer is incorrect. Answer explanation: The first line in a cache manifest file should specify the words CACHE MANIFEST.Cache manifest files are then divided into one or more of the following sections: CACHE, FALLBACK and NETWORK.Each section name must be placed on a single line and end with a colon.The CACHE section specifies the resources that should be cached.The FALLBACK section covers section specifies the resources that should be used if resources cannot be downloaded to be cached.The NETWORK section specifies resoures that should never be cached.If you do not specify a section name by default the CACHE section is assumed.In this scenario the Main.js and Main.css resources appear without a section header.Therefore they are associated with the CACHE section indicating that they should be cached.The Functions.js resource is specified in the NETWORK section indicating that it should never be cached.</t>
+  </si>
+  <si>
+    <t>54.А web page needs to save the value of an &lt;input&gt; element.The storage mechanism must meet these requirements: *It must allow data storage of up to 1MB *The data must be retrievable after the user closes and reopens the browser. *The data must not be transmitted to the Web server.</t>
+  </si>
+  <si>
+    <t>localStorage.userdata = $("#userData").val();</t>
+  </si>
+  <si>
+    <t>My answer is correct.Answer explanation: This code uses local storage.Local storage allows you to store up to 10MB of data on the client.The data is not automatically transmitted to the web server with each browser request.When you close and reopen the browser the data is still retrievable.You access local storage through the localStorage property of the window object.</t>
+  </si>
+  <si>
+    <t>55.You create a web site that uses AppCache.You want to always cache resources named App.js and App.css locally.You must ensure that Test.js is never cached.</t>
+  </si>
+  <si>
+    <t>CACHE MANIFEST:
+CACHE:
+App.js
+App.css
+NETWORK:
+Test.js</t>
+  </si>
+  <si>
+    <t>My answer is correct.Answer explanation:In this scenario you should place the App.js and App.css resources within the CACHE section indicating that they should be cached.You should place the Test.js resource in the NETWORK section indicating that it should NEVER BE CACHED.</t>
+  </si>
+  <si>
+    <t>57.You received a JSON string from a web service.To consume the data you to convert the JSON string to JS object.</t>
+  </si>
+  <si>
+    <t>1. JSON.parse 2. jQuery.parseJSON</t>
+  </si>
+  <si>
+    <t>JSON.stringify</t>
+  </si>
+  <si>
+    <t>My answers are incorrect.Answers explanation:1. JSON.parse is a correct option because it deserializes JSON text to a JS object. 2. jQuery.parseJSON is also a correct option because it converts JSON text to a JS object.</t>
+  </si>
+  <si>
+    <t>58.You want to asynchronously load a plain text file using XMLHttpRequest.Which are the correct steps?</t>
+  </si>
+  <si>
+    <t>1. Assign a new instance of XMLHttpRequest to xhr 2. Register a handler for event onreadystatechange 3. Invoke xhr.open("GET", url, true) 4. Invoke xhr.send()</t>
+  </si>
+  <si>
+    <t>My answers are correct. Answers explanation: 1.To use the XMLHttpRequest object you must first create a new instance of it. 2.You should register an event handler to its onreadystatechange event in order to process the response data. 3.The open method should be called next.It accepts three parameters: HTTP method, URL and isAsync.You should use "GET" method to load a plain text file.The isAsync parameter should be set to true for asynchronous requests. 4.The send method should be called last to initiate the request.</t>
+  </si>
+  <si>
+    <t>59.You write the following code to retrive the title of exam 70-480:                                                                       var request = new XMLHttpRequest();
+request.open("GET", "http://service.measureup.com/Exams", false);
+request.send();
+var attribute = doc.selectSingleNode("//Exam[@ID='70-480']/@Title");
+var title = attribute.value;                                                                                                   You need to add a code line at the empty space.</t>
+  </si>
+  <si>
+    <t>var doc = request.responseXML;</t>
+  </si>
+  <si>
+    <t>My answer is correct. Answer explanation: The responseXML property returns an IXMLDOMDocument object that represents the loaded XML data.This object contains a selectSingleNode method that allows you to search for an element, attribute or text node.</t>
+  </si>
+  <si>
+    <t>60.You write the following code to retrieve the title of the first exam:                                                                                     var request = new XMLHttpRequest();
+request.open("GET", "http://service.measureup.com/Exams", false);
+request.send();
+var title = doc.Exams[0].Title;                                                                                                                               You need to add code line at the empty space.</t>
+  </si>
+  <si>
+    <t>var doc = JSON.parse(request.responseText);</t>
+  </si>
+  <si>
+    <t>My answer is correct.Answer explanation: The responseText property returns a string that represents the data retrieved.In this scenario the data is a JSON-encoded string.This code uses the parse function of the JSON object to convert the string data to an object.</t>
+  </si>
+  <si>
+    <t>61.You need to use the IXMLDOMDocument object to determine the total cost of a sandwich and lemonade.</t>
+  </si>
+  <si>
+    <t>var totalPrice = 0;
+var prices = doc.selectNodes("//Item[@Name='Sandwich' or @Name='Lemonade']/@Price");
+for (var index = 0; index &lt; prices.length; index++){
+    totalPrice += prices[index].value;
+}</t>
+  </si>
+  <si>
+    <t>var totalPrice = 0;
+var prices = doc.selectNodes("//Item[Name='Sandwich' or Name='Lemonade']/Price");
+for (var index = 0; index &lt; prices.length; index++){
+    totalPrice += prices[index].value;
+}</t>
+  </si>
+  <si>
+    <t>My answer is incorrect. Answer explanation: This code calls the selectNode method passing to it an XPATH expression that returns all Price attributes where the Name attribute is equal to Sandwich or Lemonade.It then iterates throgh the returned attributes and adds their values.</t>
+  </si>
+  <si>
+    <t>63.The following JS code retrieves data from a web service:                                                                                      var request = new XMLHttpRequest();
+request.open("GET", "GetData", true);
+request.send();
+var data = request.responseText;                                                                                                              After this code runs the data variable is empty.However if you add the following code alert("Testing") the data variable contains the correct value.</t>
+  </si>
+  <si>
+    <t>1. Add the following code between lines 01 and 02:                                                                                                 var data = null;
+request.onreadystatechange = function () {
+    if (request.readyState == 4 &amp;&amp; request.status == 200) {
+        data = request.responseText;
+    }  
+};                                                                                                                                                 2. Remove line 04</t>
+  </si>
+  <si>
+    <t>My answers are correct.Answers exolanation: 1. The problem in this scenario is that the web service is accessed asynchronously as indicated by the third parameter of the open function of the XMLHttpRequest object.When this parameter is set to true you must handle the onreadystatechange event which is raised after the data is available. 2. You should also remove line 04 because you must access the data in the event handler of the onreadystatechange event.</t>
+  </si>
+  <si>
+    <t>63.You retrieve the data as string named menu.You need to convert the string to an object and remove the Calories and Type properties so that they do not exist as part of the object.</t>
+  </si>
+  <si>
+    <t>var newMenu = JSON.parse(menu, function (key, value) {
+    var newValue =  value;
+    switch (key) {
+        case "Calories":
+        case "Type":
+            newValue = undefined;
+            break;
+    }
+    return newValue;
+});</t>
+  </si>
+  <si>
+    <t>var newMenu = JSON.stringify(menu, function (key, value) {
+    var newValue =  value;
+    switch (key) {
+        case "Calories":
+        case "Type":
+            newValue = undefined;
+            break;
+    }
+    return newValue;
+});</t>
+  </si>
+  <si>
+    <t>My answer is incorrect.Answer explanation: In this scenario the data retrieved is a JSON-encoded string.The parse function of the JSON object converts a JSON-encoded string to an object.The second parameter of the parse function is an optional callback that allows you to change the values of properties or remove properties altogheter.The callback accepts the property name as the first parameter and the property value as the second parameter.The return value of the callback represents the new value of the associated property.If you return undefined for a property the property is removed from the resulting object.</t>
+  </si>
+  <si>
+    <t>64.You retrieve the data as a string named data.You need to to convert the string to an object and remove the Responsibility and UNLOC properties so that they do not exist as part of the object.</t>
+  </si>
+  <si>
+    <t>1. JSON.parse 2. undefined</t>
+  </si>
+  <si>
+    <t>2. null</t>
+  </si>
+  <si>
+    <t>My answer is incorrect.Answer explanation:In this scenario the data retrieved is a JSON-encoded string.The parse function of the JSON onject converts a JSON-encoded string to an object.The second parameter of the parse function is an optional callback that allows you to change the values of properties or remove properties altogether.The callback accepts the property name as the first parameter and the property value as the second parameter.The return value of the callback represents the new value of the associated property.If you then return undefined for a property the property is removed from the resulting object.</t>
+  </si>
+  <si>
+    <t>65.You want to use an HTML5 input field to capture user's email address.You need to ensure that an email address is always supplied as part of the subscription request.</t>
+  </si>
+  <si>
+    <t>&lt;input type="email" name="email" required /&gt;</t>
+  </si>
+  <si>
+    <t>My answers are correct.Answers explanation: The most appropriate HTML5 input type for email address is "email".Standarts complaint browsers will validate if the entered value is in valid email format.The "required" attribute ensures that no submission is made until a value is given.</t>
   </si>
 </sst>
 </file>
@@ -1102,8 +1316,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D352"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.25"/>
@@ -1779,96 +1993,194 @@
       </c>
     </row>
     <row r="54" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="10">
-        <v>51</v>
-      </c>
-      <c r="B54" s="11"/>
+      <c r="A54" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="B54" s="11" t="s">
+        <v>171</v>
+      </c>
       <c r="C54" s="12"/>
-      <c r="D54" s="13"/>
+      <c r="D54" s="13" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="55" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="10"/>
-      <c r="B55" s="11"/>
+      <c r="A55" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="B55" s="11" t="s">
+        <v>174</v>
+      </c>
       <c r="C55" s="12"/>
-      <c r="D55" s="13"/>
+      <c r="D55" s="13" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="56" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="10"/>
-      <c r="B56" s="11"/>
+      <c r="A56" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="B56" s="11" t="s">
+        <v>177</v>
+      </c>
       <c r="C56" s="12"/>
-      <c r="D56" s="13"/>
+      <c r="D56" s="13" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="57" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="10"/>
-      <c r="B57" s="11"/>
-      <c r="C57" s="12"/>
-      <c r="D57" s="13"/>
+      <c r="A57" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="B57" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="C57" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="D57" s="13" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="58" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="10"/>
-      <c r="B58" s="11"/>
+      <c r="A58" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="B58" s="11" t="s">
+        <v>184</v>
+      </c>
       <c r="C58" s="12"/>
-      <c r="D58" s="13"/>
+      <c r="D58" s="13" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="59" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="10"/>
-      <c r="B59" s="11"/>
+      <c r="A59" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="B59" s="11" t="s">
+        <v>187</v>
+      </c>
       <c r="C59" s="12"/>
-      <c r="D59" s="13"/>
+      <c r="D59" s="13" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="60" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="10"/>
-      <c r="B60" s="11"/>
-      <c r="C60" s="12"/>
-      <c r="D60" s="13"/>
+      <c r="A60" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="B60" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="C60" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="D60" s="13" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="61" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="10"/>
-      <c r="B61" s="11"/>
+      <c r="A61" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="B61" s="11" t="s">
+        <v>194</v>
+      </c>
       <c r="C61" s="12"/>
-      <c r="D61" s="13"/>
+      <c r="D61" s="13" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="62" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="10"/>
-      <c r="B62" s="11"/>
+      <c r="A62" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="B62" s="11" t="s">
+        <v>197</v>
+      </c>
       <c r="C62" s="12"/>
-      <c r="D62" s="13"/>
+      <c r="D62" s="13" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="63" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="10"/>
-      <c r="B63" s="11"/>
+      <c r="A63" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="B63" s="11" t="s">
+        <v>200</v>
+      </c>
       <c r="C63" s="12"/>
-      <c r="D63" s="13"/>
+      <c r="D63" s="13" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="64" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="10"/>
-      <c r="B64" s="11"/>
-      <c r="C64" s="12"/>
-      <c r="D64" s="13"/>
+      <c r="A64" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="B64" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="C64" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="D64" s="13" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="65" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="10"/>
-      <c r="B65" s="11"/>
+      <c r="A65" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="B65" s="11" t="s">
+        <v>207</v>
+      </c>
       <c r="C65" s="12"/>
-      <c r="D65" s="13"/>
+      <c r="D65" s="13" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="66" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="10"/>
-      <c r="B66" s="11"/>
-      <c r="C66" s="12"/>
-      <c r="D66" s="13"/>
+      <c r="A66" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="B66" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="C66" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="D66" s="13" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="67" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="10"/>
-      <c r="B67" s="11"/>
-      <c r="C67" s="12"/>
-      <c r="D67" s="13"/>
+      <c r="A67" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="B67" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="C67" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="D67" s="13" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="68" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="10"/>
-      <c r="B68" s="11"/>
+      <c r="A68" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="B68" s="11" t="s">
+        <v>218</v>
+      </c>
       <c r="C68" s="12"/>
-      <c r="D68" s="13"/>
+      <c r="D68" s="13" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="69" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="10"/>

</xml_diff>

<commit_message>
Commit on 27.01.2019. Added the answers with the explanations to all of the questions.
</commit_message>
<xml_diff>
--- a/Exam Preparation/resources/70-480 Practice Exam Answers and Explanations.xlsx
+++ b/Exam Preparation/resources/70-480 Practice Exam Answers and Explanations.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="485">
   <si>
     <t>Question</t>
   </si>
@@ -1249,6 +1249,667 @@
   </si>
   <si>
     <t>My answer is incorrect. Answer explanation: This code uses the addEventListener function to register the onclick event of the button element with the event handler represented by the handler variable.When you use the addEventListener function you should remove the "on" prefix.Therefore the first parameter to the function is click instead of onclick.The second parameter specifies the object or callback function that represents the event handler.</t>
+  </si>
+  <si>
+    <t>97.When the left mouse button is pressed but not released you want to capture the location of the mouse pointer and save the location in the  x and y variables.When the mouse moves you want to fill a rectangle from the location where the mouse button was pressed to the current location of the mouse.When the mouse button is released you want to stop filling the rectangle.</t>
+  </si>
+  <si>
+    <t>canvas.onmousedown = function (event) {
+    if (event.button == 0) {
+        x = event.x;
+        y = event.y;
+        isMouseDown = true;
+    }
+ };
+ canvas.onmousemove = function (event) {
+    if(isMouseDown) {
+ context.clearRect(x, y, width, height);} width = event.x - x;  height = event.y - y; context.fillRect(x, y, width, height);}};
+ canvas.onmouseup = function () {isMouseDown = false;};</t>
+  </si>
+  <si>
+    <t>My answer is correct.Answer explanation: This code uses anonymous functions to hadle events.It handles the onmousedown event of the canvas object to initialize the x and y variables when the user presses the left mouse button.The left mopuse button status is determined by the value of the button property of the event object passed as a parameter to the event handler.If the button property returns 0 the left mouse button is pressed.The onmousedown event is raised when the user passes any mouse button on the canvas object.This code handles the onmousemove event of the canvas object to clear a previous rectangle and draw and fill a new one by using the location where the mouse button was pressed and the current location of the mouse pointer but only if the isMouseDown variable is set to true.The onmousemove event is raised whenever the mouse moves over the canvas object.This code handles the onmouseup event to set the isMouseDown variable to false.This prevents subsequent mouse movements from causing rectangles to be drawn until the left mouse button is pressed again.The onmouseup event is raised when a pressed mouse button is released.</t>
+  </si>
+  <si>
+    <t>98.When you click the canvas element two alert messages are displayed.However you want only the alert message "canvas clicked" to be displayed when the canvas element is clicked.</t>
+  </si>
+  <si>
+    <t>Modify lines 07 through 10 as follows: canvas.onclick = function(event) { window.alert("canvas clicked"); event.cancelBubble = true;}</t>
+  </si>
+  <si>
+    <t>My answer is correct.Answer explanation: This code redefines the anonymous function to accept an event object as parameter.The event object contains a cancelBubble property that allows you to specify whether or not an event should bubble up its hierarchy of event handlers.In this scenario both the window object and the canvas objetc have event handlers for the onclick event.When you click the canvas element the onclick event of the canvas object is raised.However this event bubbles up its hierarchy by default.Because the canvas object is placed on the window object, the window object also handles the onclick event.By setting the cancelBubble property to true you prevent that default behavior from occuring.</t>
+  </si>
+  <si>
+    <t>99.You need to add code at line 08 to register each handler with the onchange event.</t>
+  </si>
+  <si>
+    <t>userData.addEventListener("click",  handler);</t>
+  </si>
+  <si>
+    <t>userData.onclick = function() {handler();};</t>
+  </si>
+  <si>
+    <t>My answer is incorrect.Answer explanation:This code uses the addEventListener function to register the onclick event of the button element with the event handler represented by the handler variable.When you use the addEventListener function you should remove the "on" prefix.Therefore the first parameter to the function is click instead of onclick.The second parameter specifies the object or callback function that represents the event handler.</t>
+  </si>
+  <si>
+    <t>100.You noticed that while the paragraph is in green the anchor link is blue.You want to ensure that the link is also green.</t>
+  </si>
+  <si>
+    <t>1. Add the style attribute to the "a" element with the value of "color:green"; 2. Add the style attribute to the "a" element with the value of "color:inherit";</t>
+  </si>
+  <si>
+    <t>Change the style attribute of the "p" element to "color:green!important;"</t>
+  </si>
+  <si>
+    <t>My answer is incorrect.Answer explanation:The color valuie of an anchor link is usually not inherited from its parent element because most users agents apply specific colors to links.To override such behavior you can set the "color" property of the anchor link to be same as its parent element using the keyword "inherit" or just repeat the same value of the parent.Changing the "color" property of the parent element alone would not impact the color of the embedded anchor link.</t>
+  </si>
+  <si>
+    <t>101.The styles of the page elements are cascaded from different origins of CSS declarations. What is the order of precedense of CSS declarations?</t>
+  </si>
+  <si>
+    <t>1.Important author declarations 2.Important user declarations 3. Important user agent declarations 4. Normal author declarations 5. Normal user declarations 6. Normal user agent declarations</t>
+  </si>
+  <si>
+    <t>1. Important user agent declarations 2. Important user declarations 3. Important author declarations 4. Normal author declarations 5. Normal user declarations 6. Normal user agent declarations</t>
+  </si>
+  <si>
+    <t>My answer is incorrect.Answer explanation: According to the CSS3 standard the cascading order of precedense is in descending order: *Transition declarations *Important user agent declarations *Important user declarations *Important override declarations *Important author declarations *Animation declaration *Normal override declarations *Normal author declarations *Normal user declarations *Normal user agent declarations</t>
+  </si>
+  <si>
+    <t>102.The following markup exists on a web page:                                                                                                                                                      
+&lt;style&gt;
+    p {background-color: red;}
+    .light {background-color: pink;}
+    .light p {background-color: yellow;}
+&lt;/style&gt;
+&lt;div class="light" style="background-color: green"&gt;
+    &lt;p&gt;This is some sample text.&lt;/p&gt;
+&lt;/div&gt; You need to determine the background color of the paragraph element.</t>
+  </si>
+  <si>
+    <t>yellow</t>
+  </si>
+  <si>
+    <t>My answer is correct.Answer explanation: The background color that gets rendered is yellow.When multiple CSS rules apply to an element the most specific selector is used to determine the rule that takes precedence.In this scenario the div element has an inline style that sets the background color of it and its contents to green.It also has its class attribute set to light which is defined in the style element to set the background color to pink.A rule is defined for paragraph elements to set their background colors to red.However the following rule is has a more specific CSS selector the paragraph element in this scenario: .light p {  background-color: yellow;} This rule selects paragraph elements that are descendants of any element that has its class attribute set to light.</t>
+  </si>
+  <si>
+    <t>103.The following markup exists on a web page:                                                                                                                                                
+&lt;table&gt;
+    &lt;tr&gt;&lt;td&gt;Name:&lt;/td&gt;&lt;td&gt;&lt;input type="text" id="name"&gt;&lt;/td&gt;&lt;/tr&gt;
+    &lt;tr&gt;&lt;td&gt;Age:&lt;/td&gt;&lt;td&gt;&lt;input type="number" id="age"&gt;&lt;/td&gt;&lt;/tr&gt;
+    &lt;tr&gt;&lt;td&gt;Salary:&lt;/td&gt;&lt;td&gt;&lt;input type="number" id="salary"&gt;&lt;/td&gt;&lt;/tr&gt;
+&lt;/table&gt; You need to define a CSS rule to set the background color of all input elements contained in table cells to yellow.</t>
+  </si>
+  <si>
+    <t>table td&gt;input {background-color: yellow;}</t>
+  </si>
+  <si>
+    <t>My answer is correct.Answer explanation: The CSS selector finds all input elements that are immediate children of td elements which are in turn descendants of table elements.It sets the background color of the input elements to yellow.</t>
+  </si>
+  <si>
+    <t>104.A web page contains several paragraph elements.You want each paragraph element to use the same border style weight and color as the element's parent element.</t>
+  </si>
+  <si>
+    <t>p {border: inherit;}</t>
+  </si>
+  <si>
+    <t>My answer is correct.Answer explanation: This markup sets the border property to inherit.This causes the paragraph element to inherit the value of the border property from its parent element.The border property values in the other answer choices are not valid values for that property.</t>
+  </si>
+  <si>
+    <t>105.The following markup exists on a web page:                                                                                                                                                       
+&lt;style&gt;
+    section article {background-color: red;}
+    article {background-color: green;}
+    .light {background-color: yellow;}
+    .light article {background-color: lightskyblue;}
+&lt;/style&gt;
+&lt;section class="light" style="background-color: darkgrey;"&gt;&lt;article&gt;This is a sample article.&lt;/article&gt;&lt;/section&gt; You need to determine the background color of the article element.</t>
+  </si>
+  <si>
+    <t>lightskyblue</t>
+  </si>
+  <si>
+    <t>My answer is correct.Answer explanation: In this scenario the section element has an inline style that sets the background color of it and its contents to darkgrey.It also has its class attribute set to light which is defined in the style element to set the background color to yellow.A rule is defined for article elements to set their background colors to green.Another rule is defined for article elements that are children of section elements to set their background colors to red.However the following rule is has a more specific CSS selector for the article element in this scenario: .light article {background-color: lightskyblue;} This rule selects article elements that are descendants of any element that has its class attribute set to light.</t>
+  </si>
+  <si>
+    <t>106.A web page contains several section elements.You want each section element to use the same background as the section element's parent element.</t>
+  </si>
+  <si>
+    <t>section {background: inherit}</t>
+  </si>
+  <si>
+    <t>My answer is correct. Answer explanation: This rule sets the background CSS property to inherit.This causes the section element to inherit the value of the background property from its parent element.</t>
+  </si>
+  <si>
+    <t>107.You are implementing a promotional discount feature in JS.Variable promoCode contains the promotion code entered by the user.No discount should be given to if the user does not provide a promotion code.At the moment the only valid promotion code is "BDAY".Additional promotion codes may be added later.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+switch (promoCode) {
+    case "":
+        discount = 0;
+        break;
+    case "BDAY":
+        discount = 0.10;
+        break;
+    default:  alert("Invalid code.");}</t>
+  </si>
+  <si>
+    <t>switch (promoCode) {
+    case "":
+        alert("Invalid code.");
+        break;
+    case "BDAY":
+        discount = 0.10;
+        break;
+    default: discount = 0;}</t>
+  </si>
+  <si>
+    <t>My answer is incorrect.Answer explanation: In a switch statement execution starts from the matching case label and will continue until it encounters a "break" or the end of the switch statement.In this question the logic in each case block is independent and therefore a "break" statement is necessary to terminate each of the case blocks.If the switch expression matched none of the case labels the "default" clause will be executed.In this question you should use "default" clause to alert the user that an invalid promotion code was entered.</t>
+  </si>
+  <si>
+    <t>108.Given that x = 1 and y = '1'.Which expressions are true.</t>
+  </si>
+  <si>
+    <t>1. x !== y 2. x == y</t>
+  </si>
+  <si>
+    <t>My answer are correct. Answers explanation: In JS equality ( == and != ) comparisons, if the types of the two values are different they will be converted to string, number or Boolean.The values are considered equal if their string values equivalent numerical values or Boolean values are identical.Therefore 1 and '1' are considered '==' equal. The identity comparison operators ( === and !== ) do not perform type conversions. Two values must be of the same type to be considered equal ( '===' ). Therefore 1 and '1' are not considered '===' equal.</t>
+  </si>
+  <si>
+    <t>109.You are writing a JS code that determines wheter or not a given year is a leap year .These rules determine whether or not a given year is a leap year: *If the year is divisible by 400 then it is always a leap year; *If the year is divisible by 4 but not by 100 then it is a leap year; *Otherwise the year is not a leap year</t>
+  </si>
+  <si>
+    <t>return year % 400 == 0 || year % 4 == 0 &amp;&amp; year % 100 != 0;</t>
+  </si>
+  <si>
+    <t>My answer is correct.Answer explanation: The modulus operator (%) determines whether or not a number is divisible by another number.If a number is divisible by another number the result is zero.If it is not the result is not zero.The logical OR operator ( || ) returns true if either the expression to its left or to its right returns true.The logical AND ( &amp;&amp; ) returns true of both the expression to its left and the expression to its right are true.However expressions that use the AND operator are evaluated before expressions that use the OR operator.This code first determines whether the year is divisible by 4 and not divisible by 100.If the determination is true then the code returns true.If not then it determines whether the year is divisible by 400.If the determination is true then the code returns true.Otherwise the code returns false.</t>
+  </si>
+  <si>
+    <t>110.You are writing a JS function to calculate the sum of the square sequence of a number.To calculate the square sequence of a number, you square each consecutive number starting with the number 1.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+var count = 1;
+while(count &lt;= maxNumber) {
+    sum += count * count;
+    count += 1;
+}</t>
+  </si>
+  <si>
+    <t>My answer is correct. Answer explanation: This code first checks the while condition to ensure that the value 0 is not passed.If so the loop exists.If not the loop continues until the value of the count variable increments to the value of the maxNumber variable. During each iteration the sum variable adds its previous value to the new square.</t>
+  </si>
+  <si>
+    <t>111.You are examining the following JS function: function IsEvenOrOdd(number) { return number % 2 == 0 ? 'even' : 'odd'; } You need to determine whether or not the function is implemented correctly.</t>
+  </si>
+  <si>
+    <t>The function is implemented correctly.</t>
+  </si>
+  <si>
+    <t>My answer is correct.Answer explanation: You should conclude that the function is implemented correctly.The function uses the modulus operator (%) to determine whether the number is divisible by 2.The conditional ternary operator ( ? : ) specifies a condition and two expressions.The condition is specified to the left of the question mark ( ? ).The expression to return if the condition is true is specified on the left side of the ( : ) and the expression to return if the condition is false is specified on the right  side of the ( : ).If the number is divisible by 2 then the string "even" is returned.If not the string "odd" is returned.</t>
+  </si>
+  <si>
+    <t>112.You discover the following JS code:                                                                                                                                                              var passedExam = false;
+var score = GetExamScore();
+if (score &gt;= 70) {
+    passedExam = true;
+    AddToWaitingList();
+    if (score &gt;= 90) {
+        EmailTeamLead();
+        var yearsOfExperience = GetYearsOfExperience();
+        if (yearsOfExperience &gt;= 10)
+            EmaiHiringManager();}}</t>
+  </si>
+  <si>
+    <t>var passedExam = false;
+while (true) {
+    var score = GetExamScore();
+    if (score &lt; 70) break;
+    passedExam = true;
+    AddToWaitingList();
+    if (score &lt; 90) break;
+    EmailTeamLead();
+    var yearsExperience = GetYearsExperience();
+    if (yearsExperience &lt; 10) break;
+    EmailHiringManager();  break;}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+var passedExam = false;
+var score = GetExamScore();
+if (score &gt;= 70) { passedExam = true; AddToWaitingList(); }
+else if (score &gt;= 90) { EmailTeamLead(); }
+else if (GetYearsExperience() &gt;= 10) { EmailHiringManager(); }</t>
+  </si>
+  <si>
+    <t>My answer is incorrect. Answer explanation: This code uses a while loop to eliminate nested if statements.It performs the opposite of the original conditional checks and then breaks if the conditions return true.For example this code first determines whether the score is below 70.If so then it breaks out the loop.If it is 70 or greater then it sets the passedExam variable to true and calls the AddToWaitingList function similar to the original code.When using a while true loop you must always include a break statement at the end of the loop to ensure that the loop does not iterate indefinitely.</t>
+  </si>
+  <si>
+    <t>113.You are creating a web site for a transportation logistics company.A variable named code represents a numeric transportation code.A variable named description represents the user-friendly description associated with a particular code.</t>
+  </si>
+  <si>
+    <t>switch (code) {
+    case 10:
+        description = 'Ocean';
+        break;
+    case 20:
+        description = 'Rail';
+        break;
+    case 30: description = 'Truck'; break;
+    case 40: description = 'Air';break;
+    default:
+        description = 'Other'; break;}</t>
+  </si>
+  <si>
+    <t>My answer is correct.Answer explanation: This code uses a switch statement to determine which statements to execute.The statements to execute are determined by case statements with each case statement being evaluated from top to bottom.Each case statement is separated by a break statement so that execution leaves the switch statement after a case statement is evaluated.If none of the case statements evaluate to true then the default statement executes.</t>
+  </si>
+  <si>
+    <t>114.You need to rewrite this code by using the inline ternary operator.</t>
+  </si>
+  <si>
+    <t>result = x != 1 ? False : y != 2;</t>
+  </si>
+  <si>
+    <t>result = x == 1 ? True : y == 2;</t>
+  </si>
+  <si>
+    <t>My answer is incorrect. Answer explanation: This code first determines if x is not equal to 1.If it is not then it sets result to false which is the same logic in the existing code.If x is equal to 1 it sets result to true if y is not equal to 2 and false otherwise.</t>
+  </si>
+  <si>
+    <t>115.Your application involves intensive calculations on the client site.You want to ensure that the browser remains responsive while the calculations are being performed.</t>
+  </si>
+  <si>
+    <t>Web Workers</t>
+  </si>
+  <si>
+    <t>My answer is correct. Answer explanation: You should use Web Workers because it is used to run calculation-intensive JS in the background which ensures the responsiveness of the webpage.</t>
+  </si>
+  <si>
+    <t>116.You want to use the HTML5 Web Workers API.Which elements can be accessed within the scope of a web worker?</t>
+  </si>
+  <si>
+    <t>1. postMessage() 2. setTimeout() 3. setInterval() 4. XMLHttpRequest()</t>
+  </si>
+  <si>
+    <t>My answer is correct.Answer explanation: Not all elements accessible in the JS of the main page are also accessible In the scope of a web worker.This is mainly due to the multi-threading nature of web workers.You can access the XMLHttpRequest object, setTimeout(), clearTimeout(), setInterval(), clearInterval(), postMessage() as well as standard JS types (e.g. Date, Array, RegExp, etc.) within a web worker.The DOM is one of the major non-accessible elements within a web worker.Global variables of the main page the window object and the parent object are also not accessible.</t>
+  </si>
+  <si>
+    <t>117.You use the Web Worker API to execute code in a file named Worker.js</t>
+  </si>
+  <si>
+    <t>var worker = new Worker('Worker.js');
+worker.onmessage = function (e) {
+      alert(e.data);
+};
+worker.postMessage("");</t>
+  </si>
+  <si>
+    <t>My answer is correct. Answer explanation: The Web Worker API allows you to execute scripts in a background thread without blocking the user interface thread.You should first instantiate the Worker object by using the "new" keyword and assigning it to a variable.The parameter to the construction is the name of the JS file that represents the background script to execute.The file typically contains one or more long running tasks.The code in that script can signify completion by sending a message to its caller with the postMessage function.You should next associate an event handler with the onmessage event of the Worker object.This allows your main thread to be notified when the background script sends the "Complete" message.You use the following code to handle the event with an anonymous function.The parameter to the anonymous function is an event object.This object contains a data property that specifies the data sent as a parameter to the postMessage function.This property can be either a string or a JSON object.The background script begins by handling the onmessage event by the shared Web Worker object.The addEventListener function allows you ti associate an event handler with an event.</t>
+  </si>
+  <si>
+    <t>118.You need to complete the implementation of this file to ensure that the web page is notified and displays the alert message when address verification is complete.</t>
+  </si>
+  <si>
+    <t>self.onmessage = function (e) {
+    var result = VerifyAddress(e.data);
+    self.postMessage(result);
+};</t>
+  </si>
+  <si>
+    <t>My answer is correct. Answer explanation: This code registers the onmessage event of the current Worker object with an anonymous function that handles the event.All code in a background script is part of the scope of the Worker object created on the page.The Worker object has a property named self that references the scope of the Worker object.Using this property has the same effect as using the "this" keyword.You can also choose not to use the property or the "this" keyword and access properties, events and functions of the Worker object directly.</t>
+  </si>
+  <si>
+    <t>119.You create a Worker object named updater on a web page.You need to stop the background task from the web page.</t>
+  </si>
+  <si>
+    <t>updater.terminate();</t>
+  </si>
+  <si>
+    <t>My answer is correct. Answer explanation: The terminate function immediately terminates the background task.</t>
+  </si>
+  <si>
+    <t>120.You need to write code in the PhoneNumberLookup.js file to retrieve the area code from the sent message.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+onmessage = function (e) {
+    var areaCode = e.data.areaCode;
+};</t>
+  </si>
+  <si>
+    <t>My answer is correct. Answer explanation: This code uses an anonymous function to handle the onmessage event.The parameter to the anonymous function is an event object.This object contains a data property that specifies the data sent as a parameter to the postMessage function.This property can be either a string or a JSON object.In this scenario the data passed to the postMessage function is a JSON object.</t>
+  </si>
+  <si>
+    <t>121.You need to write code in the Search.js file to retrieve the keywords from the sent message.</t>
+  </si>
+  <si>
+    <t>onmessage = function (e) {
+    var keywords = e.data.keywords;
+};</t>
+  </si>
+  <si>
+    <t>122.You want to build a fluid layout that works under different browser window sizes.</t>
+  </si>
+  <si>
+    <t>display: flex;</t>
+  </si>
+  <si>
+    <t>My answer is correct. Answer explanation: To make an element a flexible box container its displays CSS property should be set to "flex".</t>
+  </si>
+  <si>
+    <t>123.You published the winners on a webpage developed using HTML5 and CSS3.You are dividing the list into multiple columns.</t>
+  </si>
+  <si>
+    <t>1. columns 2. column-count</t>
+  </si>
+  <si>
+    <t>My answers are correct.Answers explanation: 1.Property column-count is a correct option because you can specify the number of columns to make the container a multi-column element. 2.Property columns is also a correct option becaise it is shorthand for both column-count and column-width.</t>
+  </si>
+  <si>
+    <t>124.The container class represents the gray container and the item class represents the blue items.When the page is rendered items will be dinamically added to the container.You want to ensure that the items are added from left to right with no more than three items on a row.If the number of items on a row exceeds three the new items must be placed on a new row below the current row.</t>
+  </si>
+  <si>
+    <t>1. Add flex-wrap: wrap to the .container class; 2. Add display:flex to the .container class;</t>
+  </si>
+  <si>
+    <t>1. Add flex-wrap:wrap to the .item class; 2. Add display:flex to the .item class;</t>
+  </si>
+  <si>
+    <t>My answers are incorrect.Answers explanation: You should add display:flex and flex-wrap:wrap to the .container class.This causes the content to wrap within the container.By default the content is laid out horizontally.If the content exceeds the width of the container it is placed on the next row.</t>
+  </si>
+  <si>
+    <t>125.You want to add a function as a method of the String object so all the String objects in your script can use the reverse() method to return their value in the opposite order.</t>
+  </si>
+  <si>
+    <t>String.prototype.reverse = reverse;</t>
+  </si>
+  <si>
+    <t>My answer is correct. Answer explanation: You can add methods and/or properties to a predifined object via its prototype property.</t>
+  </si>
+  <si>
+    <t>126.You need to create a class named Admin that inherits from the User class.The new class must override the isAdmin method of the User class to return true instead of false.</t>
+  </si>
+  <si>
+    <t>1. Admin.prototype = new User(); 2. Admin.prototype.isAdmin = function() { return true; };</t>
+  </si>
+  <si>
+    <t>1. Admin = new User(); 2. Admin.prototype.isAdmin = function() { return true; };</t>
+  </si>
+  <si>
+    <t>My answers are incorrect.Answers explanation: 1. To inherit the User class, a User object must be assigned to the prototype property of the Admin class.You can use new User() to create a new instance of the User type. 2. To override the isAdmin() method in the Admin class.This could be an anonymous function.</t>
+  </si>
+  <si>
+    <t>127.You need to define a JS object that has two properties named firstName and lastName.You need to initialize the firstName property to Jamie and the lastName property to Smith.</t>
+  </si>
+  <si>
+    <t>1. var person = new Object(); person.firstName = "Jamie"; person.lastName = "Smith";                                                                                                                  2. var person = {firstName: "Jamie", lastName: "Smith"};                                                                                                                                     3. function Person() { this.firstName = "Jamie"; this.lastName = "Smith";} var person = new Person();</t>
+  </si>
+  <si>
+    <t>function Person() {}
+var person = new Person();
+person.prototype.firstName = "Jamie";
+person.prototype.lastName = "Smith";</t>
+  </si>
+  <si>
+    <t>My answers are incorrect. Answers explanations:1.The first code statement creates a generic object.The second and third code statements initialize firstName and lastName properties of the created object, respectively. 2.This code uses JSON to create an object and initialize firstName and lastName properties. 3.This code defines a constructor that initializes firstName and lastName properties.It then instantiates an object by calling the constructor.In JS a constructor is simply a function that initializes variables with the "this" keyword.</t>
+  </si>
+  <si>
+    <t>128.You need to extend the Circle definition by adding a function to calculate the area of a circle.</t>
+  </si>
+  <si>
+    <t>Circle.prototype.Area = function () {
+    return Math.PI * this.radius * this.radius;
+};</t>
+  </si>
+  <si>
+    <t>My answer is correct. Answer explanation: This code uses the prototype to add a new function to the existing Circle definition.This allows you to extend objects when you cannot modify their existing definitions correctly.</t>
+  </si>
+  <si>
+    <t>129.You need to create a one-dimensional array with two elements.The first entry should be a string set to the value One Hundred.The second entry should be a number set to 100.</t>
+  </si>
+  <si>
+    <t>1. var array = new Array(2);
+array[0] = 'One Hundred';
+array[1] = 100;                                                                                                                                                                                                             2. var array = ["One Hundred", 100];</t>
+  </si>
+  <si>
+    <t>My answers are correct.Answers explanations:1. This code creates an array by using the built-in Array constructor.The parameter accepts a number that represents the size of the array.In this scenario the size of the array is two  because there are only two elements.The second code statement sets the value for the first element to the string One Hundred.The brackets [] represent an indexer syntax with the number between the brackets specifying the zero-based index of the element.Similarly the third code statement sets the value for the second element to the number 100; 2.This code uses a single statement to initialize an array.Elements are delimited by commas.</t>
+  </si>
+  <si>
+    <t>130.You need to define a JS object that has two properties named modelNumber and serialNumber.You need to initialize the modelNumber property to XKC123 and the serialNumber property to 4114911.</t>
+  </si>
+  <si>
+    <t>1. var device = { modelNumber: "XKC123", serialNumber: "4114911" };                                                                                                       2. function Device() { this.modelNumber = "XKC123"; this.serialNumber = "4114911"; } var device = new Device();                                                                     3. var device = new Object(); device.modelNumber = "XKC123"; device.serialNumber = "4119411";</t>
+  </si>
+  <si>
+    <t xml:space="preserve">function Device() {}
+var device = new Device();
+device.prototype.modelNumber = "XKC123";
+device.prototype.serialNumber = "4119411";
+</t>
+  </si>
+  <si>
+    <t>My answers are incorrect. Answers explanations:1.The first code statement creates a generic object.The second and third code  statements initialize modelNumber and serialNumber properties of the created object respectively. 2.This code uses JSON to create an object and initialize modelNumber and serialNumber properties. 3.This code defines a contstructor that initializes modelNumber and serialNumber properties.It then instantiates an object by calling the constructor.In JS a constructor is simply a function that initializes variables with the "this" keyword.</t>
+  </si>
+  <si>
+    <t>131.You are creating a JS function to validate ZIP Codes using regular expression.A valid ZIP Code could be *5 digits in the format of "nnnnn", e.g. 63130 *5+4 digits in the format of "nnnnn-nnnn", e.g. 63130-0001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+function isValidZipCode(sZipCode) {
+    return /^\d{5}(-\d{4})?$/.test(sZipCode);
+}</t>
+  </si>
+  <si>
+    <t>My answer is correct.Answer explanation: The regular expression ^\d{5}(-\d{4})?$ correctly represented both ZIP Code formats.To create a RegExp object in JS you can use the /pattern/ syntax.The caret (^) matches the position at the start of the string to be tested.The dollar sign (&amp;) matches the position at the end of the string to be tested.The metacharacter \d matches a digit character i.e. 0-9.The metacharacter {n} matches exactly n times.Like in \d{5} matches 5 digits.The round brackets () marks the expression within as a subexpression.The question mark (?) matches the previous character or subexpression 0 or 1 time which is equivalent to {0, 1}.The pipe ( | ) indicates a choice between two or more subexpressions.</t>
+  </si>
+  <si>
+    <t>132.You are creating JS function to validate country code entered by the user in a text box.A valid country code must be in the ISO alpha-2 format i.e. two-letter countyr codes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+function checkCountryCode() {
+    var code = $("#txtCountryCode").val();
+    if (/^[A-Z]{2}$/.test(code)) {
+        return true;
+    }
+    return false;
+}</t>
+  </si>
+  <si>
+    <t>My answer is correct. Answer explanation: The correct method to get the value of an input field is val().The correct regular expression to match the ISO alpha-2 country code is /^[A-Z]{2}$/.</t>
+  </si>
+  <si>
+    <t>133.You need to create the main menu using a semantic tag.</t>
+  </si>
+  <si>
+    <t>nav</t>
+  </si>
+  <si>
+    <t>My answer is correct.Answer explanation: In HTML5 a group of links in a major navigation block should be wrapped in the &lt;nav&gt; tag.Applications (e.g. search engines) and devices (e.g. screen readers) use semantic tags to determine their behaviors.</t>
+  </si>
+  <si>
+    <t>134.You need to replace the markup with semantic HTML5 structural elements.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+&lt;body&gt;
+&lt;header /&gt;
+&lt;nav /&gt;
+&lt;section /&gt;
+&lt;footer /&gt;
+&lt;/body&gt;</t>
+  </si>
+  <si>
+    <t>My answer is correct. Answer explanation: This markup replaces the HTML4 div elements with corresponding semantic HTML5 elements.The header element contains the header content of a site.The nav element contains the navigation menu for a page.The section element defines a section of page content.</t>
+  </si>
+  <si>
+    <t>135.You need to structure the markup by using only section and h1 elements without changing the look and feel of the page.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+&lt;h1&gt;Heading 1&lt;/h1&gt;
+&lt;section&gt;
+    &lt;h1&gt;Heading 2&lt;/h1&gt;
+    &lt;section&gt;
+        &lt;h1&gt;Heading 3&lt;/h1&gt;
+    &lt;/section&gt;
+&lt;/section&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+&lt;section&gt;
+    &lt;h1&gt;Heading 1&lt;/h1&gt;
+&lt;/section&gt;
+&lt;section&gt;
+    &lt;h1&gt;Heading 2&lt;/h1&gt;
+&lt;/section&gt;
+&lt;section&gt;
+    &lt;h1&gt;Heading 3&lt;/h1&gt;
+&lt;/section&gt;</t>
+  </si>
+  <si>
+    <t>My answer is incorrect. Answer explanation: Headings are represented by the elements h1 through h6.The number represents a style and size with sizes decreasing as the number increase.Sizes are automatically reduced when headings are placed within section elements.In this scenario this allows you to use only h1 elements by nesting them within section elements.In this scenario this allows you to use only h1 elements by nesting them within section elements.</t>
+  </si>
+  <si>
+    <t>136.A heading, subheading structure with semantic HTML5 structural elements must be created.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+&lt;h1&gt;Sample Web Site&lt;/h1&gt;
+&lt;section&gt;&lt;h1&gt;About Us&lt;/h1&gt;&lt;/section&gt;
+&lt;section&gt;&lt;h1&gt;Contact Us&lt;/h1&gt;&lt;/section&gt;</t>
+  </si>
+  <si>
+    <t>My answer is correct.Answer explanation: In this scenario, this allows you to use only h1 elements by nesting them within section elements.</t>
+  </si>
+  <si>
+    <t>137.You need to ensure that the following text is displayed as the description of your page when the page is listed in search engine's search results.</t>
+  </si>
+  <si>
+    <t>&lt;meta name="description" content="Learning HTML5"/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;title&gt;Description: Learning HTML5&lt;/title&gt;</t>
+  </si>
+  <si>
+    <t>My answer is incorrect. Answer explanation: The meta element allows you to convey hidden information about a page.By setting the name attribute to description you can provide a description of the page to search engines.You set the description as the value of the content attribute.</t>
+  </si>
+  <si>
+    <t>138.You need to ensure that standards-compliant screen readers interpret the menu correctly.</t>
+  </si>
+  <si>
+    <t>Place the markup within &lt;nav&gt; tags</t>
+  </si>
+  <si>
+    <t>My answer is correct.Answer explanation: You should place the markup within &lt;nav&gt; tags.With HTML5 you should use the &lt;nav&gt; element to specify markup as a navigationm menu.This allows standards-compliant screen readers to interpret the menu correctly and choose whether to omit the initial rendering of the navigation content.</t>
+  </si>
+  <si>
+    <t>139.You want to animate an element.The animation repeats every 5 seconds and transits from a red square to a yellow rectangle.</t>
+  </si>
+  <si>
+    <t>#demo {
+        width: 100px;
+        height: 100px;
+        keyframes: frame 5s repeat; }
+    @animation to {
+        begin {background: red; }
+        end {
+            width: 200px;
+            background: yellow;
+        }
+    }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+    #demo { width: 100px; height: 100px; animation: frames 5s infinite; }
+    @keyframes frames {
+        from { background: red; }
+        to { width: 200px; background: yellow; }
+    }</t>
+  </si>
+  <si>
+    <t>My answer is incorrect.Answer explanation: You can use the "animation" property to apply CSS3 animation to an element.The "animation" property is shorthand for 6 animation properties and starts with the animation name.The animation name is the name defined immediately after the "@keyframes".Using "@keyframes" you can define a list of animation stages.At least two stages must be defined in a "@keyframes" definition.The "from" stage (equivalent to 0%) is the initial stage and the "to" stage (equivalent to 100%) is  the final stage.Additional stages can be defined with values between 0% and 100%.As you can see the initial stage is a 100x100 red square and the final stage is a 200x100 rectangle.Therefore the first stage defined in the "@keyframes frames" should be the "from" stage with the background of red and the second stage shouild be the "to" stage with the background of yellow and width of 200px.</t>
+  </si>
+  <si>
+    <t>140.Your webpage contains two  sidebars for advertisements.You have the following requirements: *The advertisement sidebars should be displayed on full-size desktop browsers. *The advertisement sidebars should be hidden on mobile devices with a maximum width of 480px.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+    @media screen and (max-width: 480px) {
+        .adbar { display: none; }
+    }</t>
+  </si>
+  <si>
+    <t>My answer is correct. Answer explanation: To hide the advertisement sidebars for mobile devices with a maximum width of 480px you can use the CSS media query.Media type "screen" applies to screen devices including mobile devices.You should also specify the "max-width" for the media query because the advertisement sidebars should only be hidden for devices with a maximum width of 480px.</t>
+  </si>
+  <si>
+    <t>141.You need to add a CSS rule to the div element so that it is rotated at a 90 degree angle.</t>
+  </si>
+  <si>
+    <t>transform:rotateY(90deg)</t>
+  </si>
+  <si>
+    <t>1. transform: rotateZ(90deg); 2. transform: rotate(90deg);</t>
+  </si>
+  <si>
+    <t>My answer is incorrect.Answer explanation: The first rule sets the value of the transform property to a rotate function.This function uses two-dimensional rotation to rotate an element clockwise.The second rule sets the value of the transform property to a rotateZ function.This function allows you to rorate an element in a three-dimensional space along the Z axis.This has the same effect as using the rotate function.The Z axis can be visualized as leaving the screen and extending toward you.</t>
+  </si>
+  <si>
+    <t>142.When you move the mouse pointer over the div element its width increases from 100 px to 300 px.When you move the mouse pointer out the div element its width decreases from 300 px to 100 px.You want this increase and decrease in size to occur smoothly over half  second.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+&lt;style&gt;
+    div { width: 100px; height: 100px; background: red; transition: width 500ms; }
+    div:hover { width: 300px; }
+&lt;/style&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+&lt;style&gt;
+    div { width: 100px; height: 100px; background: red; }
+    div:hover { width: 300px; transition: width 500ms; }
+&lt;/style&gt;</t>
+  </si>
+  <si>
+    <t>My answer is incorrect.Answer explanation: This markup sets the transition CSS property to add an effect when the width property is changed.The first argument to the transition property is the name of the property to be changed.The second argument is the duration of the transition.Whenever the width of the div element changes it takes 500 miliseconds or one-half second to complete the change.This provides a smooth transition from one width to the other.</t>
+  </si>
+  <si>
+    <t>143.You are using CSS3 to style a web page.Your page must meet these requirements: *If the orientation of the display is landscape all section elements must have a width of 400px and a height of 200px. *If the orientation of the display is portrait all section elements must have a width of 200px and a height of 400px.</t>
+  </si>
+  <si>
+    <t>"@media all and (orientation: landscape) {
+        section { width: 400px; height: 200px; }
+    }
+   " @media all and (orientation: portrait) {
+        section { width: 400px; height: 200px; }
+    }</t>
+  </si>
+  <si>
+    <t>My answer is correct.Answer explanation: The @media rule allows you to target specific CSS rules to specific media types such as portrait and landscape devices.The @media all rule specifies all media types.The "and" operator specifies a logical AND.The "(orientation:landscape)" property-value pair indicates that the enclosed rules apply to all devices that have their orientation set to landscape mode.The "(orientation:portrait)" property-value pair indicates that the enclosed rules that apply to all devices that have their orientation set to portrait.</t>
+  </si>
+  <si>
+    <t>144.Apply transition property to a div element.</t>
+  </si>
+  <si>
+    <t>Add transition: width 300ms to the div style</t>
+  </si>
+  <si>
+    <t>Add transition: width 300ms to the div:hover style</t>
+  </si>
+  <si>
+    <t>My answer is incorrect.Answer explanation: You should add transtion to the div style.</t>
+  </si>
+  <si>
+    <t>145.Your page must meet these requirements: *If the orientation of the display is landscape all section elements must have a width of 400px and a height of 200px. *If the orientation of the display is portrait all section elements must have a width of 200px and a height of 400px.</t>
+  </si>
+  <si>
+    <t>"@media all and (orientation: landscape) {
+        section { width: 200px; height: 400px; }
+    }
+   " @media all and (orientation: portrait) {
+        section { width: 200px; height: 400px; }
+    }</t>
   </si>
 </sst>
 </file>
@@ -1679,8 +2340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D352"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="A100" sqref="A100"/>
+    <sheetView tabSelected="1" topLeftCell="A143" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="C151" sqref="C151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="36.35" x14ac:dyDescent="0.3"/>
@@ -2876,67 +3537,605 @@
         <v>323</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="101" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="102" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="103" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="104" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="105" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="106" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="107" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="108" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="109" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="110" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="111" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="112" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="113" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="114" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="115" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="116" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="117" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="118" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="119" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="120" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="121" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="122" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="123" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="124" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="125" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="126" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="127" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="128" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="129" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="130" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="131" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="132" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="133" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="134" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="135" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="136" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="137" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="138" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="139" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="140" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="141" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="142" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="143" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="144" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="145" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="146" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="147" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="148" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="149" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="150" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="151" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="152" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="153" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="154" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="155" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="156" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="157" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="158" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="159" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="160" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="100" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="B100" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="B101" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="B102" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="C102" s="5" t="s">
+        <v>332</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="B103" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="C103" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="B104" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="C104" s="5" t="s">
+        <v>339</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="B105" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="B106" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="B107" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="B108" s="4" t="s">
+        <v>352</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="B109" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="D109" s="2" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="B110" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="C110" s="5" t="s">
+        <v>359</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="B111" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="B112" s="4" t="s">
+        <v>365</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A113" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="B113" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A114" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="B114" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="D114" s="2" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A115" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="B115" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="C115" s="5" t="s">
+        <v>375</v>
+      </c>
+      <c r="D115" s="2" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A116" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="B116" s="4" t="s">
+        <v>378</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A117" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="B117" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="C117" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="D117" s="2" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A118" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="B118" s="4" t="s">
+        <v>385</v>
+      </c>
+      <c r="D118" s="2" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A119" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="B119" s="4" t="s">
+        <v>388</v>
+      </c>
+      <c r="D119" s="2" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A120" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="B120" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="D120" s="2" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A121" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="B121" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="D121" s="2" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A122" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="B122" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="D122" s="2" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A123" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="B123" s="4" t="s">
+        <v>400</v>
+      </c>
+      <c r="D123" s="2" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A124" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="B124" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="D124" s="2" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A125" s="3" t="s">
+        <v>404</v>
+      </c>
+      <c r="B125" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="D125" s="2" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A126" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="B126" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="D126" s="2" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A127" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="B127" s="4" t="s">
+        <v>411</v>
+      </c>
+      <c r="C127" s="5" t="s">
+        <v>412</v>
+      </c>
+      <c r="D127" s="2" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A128" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="B128" s="4" t="s">
+        <v>415</v>
+      </c>
+      <c r="D128" s="2" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A129" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="B129" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="C129" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="D129" s="2" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A130" s="3" t="s">
+        <v>421</v>
+      </c>
+      <c r="B130" s="4" t="s">
+        <v>422</v>
+      </c>
+      <c r="C130" s="5" t="s">
+        <v>423</v>
+      </c>
+      <c r="D130" s="2" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A131" s="3" t="s">
+        <v>425</v>
+      </c>
+      <c r="B131" s="4" t="s">
+        <v>426</v>
+      </c>
+      <c r="D131" s="2" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A132" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="B132" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="D132" s="2" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A133" s="3" t="s">
+        <v>431</v>
+      </c>
+      <c r="B133" s="4" t="s">
+        <v>432</v>
+      </c>
+      <c r="C133" s="5" t="s">
+        <v>433</v>
+      </c>
+      <c r="D133" s="2" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A134" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="B134" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="D134" s="2" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A135" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="B135" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="D135" s="2" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A136" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="B136" s="4" t="s">
+        <v>442</v>
+      </c>
+      <c r="D136" s="2" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A137" s="3" t="s">
+        <v>444</v>
+      </c>
+      <c r="B137" s="4" t="s">
+        <v>445</v>
+      </c>
+      <c r="D137" s="2" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A138" s="3" t="s">
+        <v>447</v>
+      </c>
+      <c r="B138" s="4" t="s">
+        <v>448</v>
+      </c>
+      <c r="C138" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="D138" s="2" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A139" s="3" t="s">
+        <v>451</v>
+      </c>
+      <c r="B139" s="4" t="s">
+        <v>452</v>
+      </c>
+      <c r="D139" s="2" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A140" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="B140" s="4" t="s">
+        <v>455</v>
+      </c>
+      <c r="C140" s="5" t="s">
+        <v>456</v>
+      </c>
+      <c r="D140" s="2" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A141" s="3" t="s">
+        <v>458</v>
+      </c>
+      <c r="B141" s="4" t="s">
+        <v>459</v>
+      </c>
+      <c r="D141" s="2" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A142" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="B142" s="4" t="s">
+        <v>463</v>
+      </c>
+      <c r="C142" s="5" t="s">
+        <v>462</v>
+      </c>
+      <c r="D142" s="2" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A143" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="B143" s="4" t="s">
+        <v>466</v>
+      </c>
+      <c r="D143" s="2" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A144" s="3" t="s">
+        <v>468</v>
+      </c>
+      <c r="B144" s="4" t="s">
+        <v>470</v>
+      </c>
+      <c r="C144" s="5" t="s">
+        <v>469</v>
+      </c>
+      <c r="D144" s="2" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A145" s="3" t="s">
+        <v>472</v>
+      </c>
+      <c r="B145" s="4" t="s">
+        <v>473</v>
+      </c>
+      <c r="C145" s="5" t="s">
+        <v>474</v>
+      </c>
+      <c r="D145" s="2" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A146" s="3" t="s">
+        <v>476</v>
+      </c>
+      <c r="B146" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="D146" s="2" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A147" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="B147" s="4" t="s">
+        <v>480</v>
+      </c>
+      <c r="C147" s="5" t="s">
+        <v>481</v>
+      </c>
+      <c r="D147" s="2" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A148" s="3" t="s">
+        <v>483</v>
+      </c>
+      <c r="B148" s="4" t="s">
+        <v>484</v>
+      </c>
+      <c r="D148" s="2" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="150" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="151" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="152" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="153" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="154" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="155" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="156" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="157" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="158" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="159" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="160" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="161" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="162" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="163" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Commit on 28.01.2019. Added code and answer explanations to the missing questions.
</commit_message>
<xml_diff>
--- a/Exam Preparation/resources/70-480 Practice Exam Answers and Explanations.xlsx
+++ b/Exam Preparation/resources/70-480 Practice Exam Answers and Explanations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11996" windowHeight="1703"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12000" windowHeight="1710"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="487">
   <si>
     <t>Question</t>
   </si>
@@ -48,9 +48,6 @@
     <t>1.Destination verified 2.Error calculating shipping costs 3.Cleaning up resources</t>
   </si>
   <si>
-    <t>My answer is full and correct.</t>
-  </si>
-  <si>
     <t>My answer is incomplete and incorrect. I am missing the first statement. Answer Explanations: In this scenario, the VerifyDestinationAddress function runs successfully, so the next code statement writes the message "Destination verified" to the browser. Because the CreatePackages function throws an error, excecution immediately leaves its try block and enters the corresponding catch block.The corresponding catch block writes the message "Error calculating shipping costs" to the browser.Code in a finally block always executes, even if an error is thrown. The code in the corresponding finally block writes the message "Cleaning up resources" to the browser.</t>
   </si>
   <si>
@@ -70,9 +67,6 @@
   </si>
   <si>
     <t>&lt;input id="data" type="number" min="0" max="100" required /&gt;</t>
-  </si>
-  <si>
-    <t>My answer is correct.</t>
   </si>
   <si>
     <t>5.You need to modify the markup of the data input field so that it meets this requirement when the form is submitted: *If a value is specified in the input field, it must be a number between 0 and 100</t>
@@ -1910,6 +1904,18 @@
    " @media all and (orientation: portrait) {
         section { width: 200px; height: 400px; }
     }</t>
+  </si>
+  <si>
+    <t>My answer is correct.Answer explanation: With nested try catch blocks thrown exceptions in inner try blocks are first handled by the corresponding inner catch blocks.If an inner catch block does not exist to catch the thrown exception the exception propagates up the call stack until an outer catch block handles the exception.In this scenario the VerifyDestinationAddress function throws an exception.This means that execution immediately leaves the try block and enters the corresponding catch block.The corresponding catch block writes the message "Error verifying destination address" to the browser.Code in a finally block writes the message "Cleaning up resources" to the browser.</t>
+  </si>
+  <si>
+    <t>My answer is correct.Answer explanation:The type attribute specifies the type of data that is allowed in the field.The value number indicates that only numbers are allowed.Other possible values are color, date, datetime, datetime-local, email, month, range, search, tel, time, url, week and text.The min and max attributes specify the minimum and maximum numbers allowed respectively.The required attribute specifies that data must be entered into the input field.</t>
+  </si>
+  <si>
+    <t>My answer is correct.Answer explanation:The type attribute specifies the type of data that is allowed in the field.The value range indicates that a slider should be displayed to allow a user to select a number.Other possible values are color, date, datetime, datetime-local, email, month, range, search, tel, time, url, week and text.The min and max attributes specify the minimum and maximum numbers allowed respectively</t>
+  </si>
+  <si>
+    <t>My answer is correct. Answer explanation: This code uses the $(":button") syntax to find all elements of type button.This includes &lt;input type="button"/&gt; elements and &lt;button&gt; elements.It then calls the css function to set a solid one-pixel red border.</t>
   </si>
 </sst>
 </file>
@@ -2340,19 +2346,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D352"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A143" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="C151" sqref="C151"/>
+    <sheetView tabSelected="1" topLeftCell="A147" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="A148" sqref="A148"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="36.35" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="36" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="255.44140625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="255.44140625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="255.44140625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="255.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="255.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="255.42578125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="255.42578125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="255.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="62" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="61.5" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2366,12 +2372,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -2379,10 +2385,10 @@
         <v>6</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -2390,1847 +2396,1850 @@
         <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="D5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="2" t="s">
+    </row>
+    <row r="6" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+    <row r="7" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="D7" s="2" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="B8" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+      <c r="D8" s="2" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+      <c r="D9" s="2" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B10" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+      <c r="C10" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="D10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="11" t="s">
+    </row>
+    <row r="11" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="B11" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+      <c r="C11" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="D11" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="5" t="s">
+    </row>
+    <row r="12" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="B12" s="4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
+      <c r="C12" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="D12" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="5" t="s">
+    </row>
+    <row r="13" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="B13" s="4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="4" t="s">
+    </row>
+    <row r="14" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="B14" s="4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
+      <c r="C14" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="D14" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="5" t="s">
+    </row>
+    <row r="15" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="B15" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
+    <row r="16" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B16" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="B69" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="B60" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="B61" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>269</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="C66" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="B67" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="C67" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="B68" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="D68" s="2" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="3" t="s">
+      <c r="D69" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="B69" s="4" t="s">
+    </row>
+    <row r="70" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="D69" s="2" t="s">
+      <c r="B70" s="4" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="3" t="s">
+      <c r="D70" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="B70" s="4" t="s">
+    </row>
+    <row r="71" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="B71" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="D70" s="2" t="s">
+      <c r="D71" s="2" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="3" t="s">
+    <row r="72" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="B72" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="B71" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="3" t="s">
+      <c r="D72" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="B72" s="4" t="s">
+    </row>
+    <row r="73" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="D72" s="2" t="s">
+      <c r="B73" s="4" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="3" t="s">
+      <c r="D73" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="B73" s="4" t="s">
+    </row>
+    <row r="74" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="D73" s="2" t="s">
+      <c r="B74" s="4" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="3" t="s">
+      <c r="D74" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="B74" s="4" t="s">
+    </row>
+    <row r="75" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="D74" s="2" t="s">
+      <c r="B75" s="4" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="3" t="s">
+      <c r="C75" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="B75" s="4" t="s">
+      <c r="D75" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="C75" s="5" t="s">
+    </row>
+    <row r="76" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="D75" s="2" t="s">
+      <c r="B76" s="4" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="3" t="s">
+      <c r="D76" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="B76" s="4" t="s">
+    </row>
+    <row r="77" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
         <v>242</v>
-      </c>
-      <c r="D76" s="2" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="3" t="s">
-        <v>244</v>
       </c>
       <c r="B77" s="4">
         <v>12</v>
       </c>
       <c r="D77" s="2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="B78" s="4" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="3" t="s">
+      <c r="C78" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="B78" s="4" t="s">
+      <c r="D78" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="C78" s="5" t="s">
+    </row>
+    <row r="79" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="3" t="s">
         <v>248</v>
-      </c>
-      <c r="D78" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="3" t="s">
-        <v>250</v>
       </c>
       <c r="B79" s="4">
         <v>105</v>
       </c>
       <c r="D79" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="C80" s="5" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="B80" s="4" t="s">
+      <c r="D80" s="2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="C80" s="5" t="s">
-        <v>253</v>
-      </c>
-      <c r="D80" s="2" t="s">
+      <c r="B81" s="4" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="3" t="s">
+      <c r="C81" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="B81" s="4" t="s">
+      <c r="D81" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="C81" s="5" t="s">
+    </row>
+    <row r="82" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="D81" s="2" t="s">
+      <c r="B82" s="4" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="3" t="s">
+      <c r="D82" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="B82" s="4" t="s">
+    </row>
+    <row r="83" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="D82" s="2" t="s">
+      <c r="B83" s="4" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="3" t="s">
+      <c r="C83" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="B83" s="4" t="s">
+      <c r="D83" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="C83" s="5" t="s">
+    </row>
+    <row r="84" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="D83" s="2" t="s">
+      <c r="B84" s="4" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="B84" s="4" t="s">
+      <c r="C84" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="C84" s="5" t="s">
+      <c r="D84" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="D84" s="2" t="s">
+      <c r="B85" s="4" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="3" t="s">
+      <c r="D85" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="B85" s="4" t="s">
+    </row>
+    <row r="86" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="D85" s="2" t="s">
+      <c r="B86" s="4" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="3" t="s">
+      <c r="C86" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="B86" s="4" t="s">
+      <c r="D86" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="C86" s="5" t="s">
+    </row>
+    <row r="87" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="D86" s="2" t="s">
+      <c r="B87" s="4" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="3" t="s">
+      <c r="C87" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="B87" s="4" t="s">
+      <c r="D87" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="C87" s="5" t="s">
+    </row>
+    <row r="88" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="D87" s="2" t="s">
+      <c r="B88" s="4" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="3" t="s">
+      <c r="C88" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="B88" s="4" t="s">
+      <c r="D88" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="C88" s="5" t="s">
+    </row>
+    <row r="89" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="D88" s="2" t="s">
+      <c r="B89" s="4" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="3" t="s">
+      <c r="D89" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="B89" s="4" t="s">
+    </row>
+    <row r="90" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="D89" s="2" t="s">
+      <c r="B90" s="4" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="3" t="s">
+      <c r="D90" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="B90" s="4" t="s">
+    </row>
+    <row r="91" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="D90" s="2" t="s">
+      <c r="B91" s="4" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="3" t="s">
+      <c r="D91" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="B91" s="4" t="s">
+    </row>
+    <row r="92" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="D91" s="2" t="s">
+      <c r="B92" s="4" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="3" t="s">
+      <c r="C92" s="5" t="s">
         <v>296</v>
       </c>
-      <c r="B92" s="4" t="s">
+      <c r="D92" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="C92" s="5" t="s">
+    </row>
+    <row r="93" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="D92" s="2" t="s">
+      <c r="B93" s="4" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="3" t="s">
+      <c r="C93" s="5" t="s">
         <v>300</v>
       </c>
-      <c r="B93" s="4" t="s">
+      <c r="D93" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="C93" s="5" t="s">
+    </row>
+    <row r="94" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="D93" s="2" t="s">
+      <c r="B94" s="4" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="3" t="s">
+      <c r="D94" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="B94" s="4" t="s">
+    </row>
+    <row r="95" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="D94" s="2" t="s">
+      <c r="B95" s="4" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="3" t="s">
+      <c r="D95" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="B95" s="4" t="s">
+    </row>
+    <row r="96" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="D95" s="2" t="s">
+      <c r="B96" s="4" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="3" t="s">
+      <c r="D96" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="B96" s="4" t="s">
+    </row>
+    <row r="97" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="B97" s="4" t="s">
         <v>311</v>
       </c>
-      <c r="D96" s="2" t="s">
+      <c r="C97" s="5" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="3" t="s">
+      <c r="D97" s="2" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="3" t="s">
         <v>315</v>
       </c>
-      <c r="B97" s="4" t="s">
-        <v>313</v>
-      </c>
-      <c r="C97" s="5" t="s">
-        <v>314</v>
-      </c>
-      <c r="D97" s="2" t="s">
+      <c r="B98" s="4" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="3" t="s">
+      <c r="D98" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="B98" s="4" t="s">
+    </row>
+    <row r="99" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="3" t="s">
         <v>318</v>
       </c>
-      <c r="D98" s="2" t="s">
+      <c r="B99" s="4" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="3" t="s">
+      <c r="C99" s="5" t="s">
         <v>320</v>
       </c>
-      <c r="B99" s="4" t="s">
+      <c r="D99" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="C99" s="5" t="s">
+    </row>
+    <row r="100" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="D99" s="2" t="s">
+      <c r="B100" s="4" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="3" t="s">
+      <c r="D100" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="B100" s="4" t="s">
+    </row>
+    <row r="101" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="3" t="s">
         <v>325</v>
       </c>
-      <c r="D100" s="2" t="s">
+      <c r="B101" s="4" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="3" t="s">
+      <c r="D101" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="B101" s="4" t="s">
+    </row>
+    <row r="102" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="D101" s="2" t="s">
+      <c r="B102" s="4" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="3" t="s">
+      <c r="C102" s="5" t="s">
         <v>330</v>
       </c>
-      <c r="B102" s="4" t="s">
+      <c r="D102" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="C102" s="5" t="s">
+    </row>
+    <row r="103" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="3" t="s">
         <v>332</v>
       </c>
-      <c r="D102" s="2" t="s">
+      <c r="B103" s="4" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="3" t="s">
+      <c r="C103" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="B103" s="4" t="s">
+      <c r="D103" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="C103" s="5" t="s">
+    </row>
+    <row r="104" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="3" t="s">
         <v>336</v>
       </c>
-      <c r="D103" s="2" t="s">
+      <c r="B104" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="C104" s="5" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="3" t="s">
-        <v>338</v>
-      </c>
-      <c r="B104" s="4" t="s">
+      <c r="D104" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="3" t="s">
         <v>340</v>
       </c>
-      <c r="C104" s="5" t="s">
-        <v>339</v>
-      </c>
-      <c r="D104" s="2" t="s">
+      <c r="B105" s="4" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="3" t="s">
+      <c r="D105" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="B105" s="4" t="s">
+    </row>
+    <row r="106" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="D105" s="2" t="s">
+      <c r="B106" s="4" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="3" t="s">
+      <c r="D106" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="B106" s="4" t="s">
+    </row>
+    <row r="107" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="3" t="s">
         <v>346</v>
       </c>
-      <c r="D106" s="2" t="s">
+      <c r="B107" s="4" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="3" t="s">
+      <c r="D107" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="B107" s="4" t="s">
+    </row>
+    <row r="108" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="D107" s="2" t="s">
+      <c r="B108" s="4" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="3" t="s">
+      <c r="D108" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="B108" s="4" t="s">
+    </row>
+    <row r="109" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="D108" s="2" t="s">
+      <c r="B109" s="4" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="3" t="s">
+      <c r="D109" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="B109" s="4" t="s">
+    </row>
+    <row r="110" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="3" t="s">
         <v>355</v>
       </c>
-      <c r="D109" s="2" t="s">
+      <c r="B110" s="4" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="3" t="s">
+      <c r="C110" s="5" t="s">
         <v>357</v>
       </c>
-      <c r="B110" s="4" t="s">
+      <c r="D110" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="C110" s="5" t="s">
+    </row>
+    <row r="111" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="3" t="s">
         <v>359</v>
       </c>
-      <c r="D110" s="2" t="s">
+      <c r="B111" s="4" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="3" t="s">
+      <c r="D111" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="B111" s="4" t="s">
+    </row>
+    <row r="112" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="D111" s="2" t="s">
+      <c r="B112" s="4" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="3" t="s">
+      <c r="D112" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="B112" s="4" t="s">
+    </row>
+    <row r="113" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="3" t="s">
         <v>365</v>
       </c>
-      <c r="D112" s="2" t="s">
+      <c r="B113" s="4" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="3" t="s">
+      <c r="D113" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="B113" s="4" t="s">
+    </row>
+    <row r="114" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="3" t="s">
         <v>368</v>
       </c>
-      <c r="D113" s="2" t="s">
+      <c r="B114" s="4" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="3" t="s">
+      <c r="D114" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="B114" s="4" t="s">
+    </row>
+    <row r="115" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="3" t="s">
         <v>371</v>
       </c>
-      <c r="D114" s="2" t="s">
+      <c r="B115" s="4" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="3" t="s">
+      <c r="C115" s="5" t="s">
         <v>373</v>
       </c>
-      <c r="B115" s="4" t="s">
+      <c r="D115" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="C115" s="5" t="s">
+    </row>
+    <row r="116" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="3" t="s">
         <v>375</v>
       </c>
-      <c r="D115" s="2" t="s">
+      <c r="B116" s="4" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="3" t="s">
+      <c r="D116" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="B116" s="4" t="s">
+    </row>
+    <row r="117" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="3" t="s">
         <v>378</v>
       </c>
-      <c r="D116" s="2" t="s">
+      <c r="B117" s="4" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="3" t="s">
+      <c r="C117" s="5" t="s">
         <v>380</v>
       </c>
-      <c r="B117" s="4" t="s">
+      <c r="D117" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="C117" s="5" t="s">
+    </row>
+    <row r="118" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="3" t="s">
         <v>382</v>
       </c>
-      <c r="D117" s="2" t="s">
+      <c r="B118" s="4" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A118" s="3" t="s">
+      <c r="D118" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="B118" s="4" t="s">
+    </row>
+    <row r="119" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="3" t="s">
         <v>385</v>
       </c>
-      <c r="D118" s="2" t="s">
+      <c r="B119" s="4" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="3" t="s">
+      <c r="D119" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="B119" s="4" t="s">
+    </row>
+    <row r="120" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="3" t="s">
         <v>388</v>
       </c>
-      <c r="D119" s="2" t="s">
+      <c r="B120" s="4" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A120" s="3" t="s">
+      <c r="D120" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="B120" s="4" t="s">
+    </row>
+    <row r="121" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="3" t="s">
         <v>391</v>
       </c>
-      <c r="D120" s="2" t="s">
+      <c r="B121" s="4" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="121" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="3" t="s">
+      <c r="D121" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="B121" s="4" t="s">
+    </row>
+    <row r="122" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="3" t="s">
         <v>394</v>
       </c>
-      <c r="D121" s="2" t="s">
+      <c r="B122" s="4" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="122" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A122" s="3" t="s">
+      <c r="D122" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="B122" s="4" t="s">
+    </row>
+    <row r="123" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="3" t="s">
         <v>397</v>
       </c>
-      <c r="D122" s="2" t="s">
+      <c r="B123" s="4" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="123" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="3" t="s">
+      <c r="D123" s="2" t="s">
         <v>399</v>
       </c>
-      <c r="B123" s="4" t="s">
+    </row>
+    <row r="124" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="3" t="s">
         <v>400</v>
       </c>
-      <c r="D123" s="2" t="s">
+      <c r="B124" s="4" t="s">
         <v>401</v>
       </c>
-    </row>
-    <row r="124" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A124" s="3" t="s">
+      <c r="D124" s="2" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="3" t="s">
         <v>402</v>
       </c>
-      <c r="B124" s="4" t="s">
+      <c r="B125" s="4" t="s">
         <v>403</v>
       </c>
-      <c r="D124" s="2" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A125" s="3" t="s">
+      <c r="D125" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="B125" s="4" t="s">
+    </row>
+    <row r="126" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="D125" s="2" t="s">
+      <c r="B126" s="4" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="126" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A126" s="3" t="s">
+      <c r="D126" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="B126" s="4" t="s">
+    </row>
+    <row r="127" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="3" t="s">
         <v>408</v>
       </c>
-      <c r="D126" s="2" t="s">
+      <c r="B127" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="127" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A127" s="3" t="s">
+      <c r="C127" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="B127" s="4" t="s">
+      <c r="D127" s="2" t="s">
         <v>411</v>
       </c>
-      <c r="C127" s="5" t="s">
+    </row>
+    <row r="128" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="3" t="s">
         <v>412</v>
       </c>
-      <c r="D127" s="2" t="s">
+      <c r="B128" s="4" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="128" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A128" s="3" t="s">
+      <c r="D128" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="B128" s="4" t="s">
+    </row>
+    <row r="129" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="3" t="s">
         <v>415</v>
       </c>
-      <c r="D128" s="2" t="s">
+      <c r="B129" s="4" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="129" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="3" t="s">
+      <c r="C129" s="5" t="s">
         <v>417</v>
       </c>
-      <c r="B129" s="4" t="s">
+      <c r="D129" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="C129" s="5" t="s">
+    </row>
+    <row r="130" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="3" t="s">
         <v>419</v>
       </c>
-      <c r="D129" s="2" t="s">
+      <c r="B130" s="4" t="s">
         <v>420</v>
       </c>
-    </row>
-    <row r="130" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="3" t="s">
+      <c r="C130" s="5" t="s">
         <v>421</v>
       </c>
-      <c r="B130" s="4" t="s">
+      <c r="D130" s="2" t="s">
         <v>422</v>
       </c>
-      <c r="C130" s="5" t="s">
+    </row>
+    <row r="131" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="3" t="s">
         <v>423</v>
       </c>
-      <c r="D130" s="2" t="s">
+      <c r="B131" s="4" t="s">
         <v>424</v>
       </c>
-    </row>
-    <row r="131" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A131" s="3" t="s">
+      <c r="D131" s="2" t="s">
         <v>425</v>
       </c>
-      <c r="B131" s="4" t="s">
+    </row>
+    <row r="132" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="3" t="s">
         <v>426</v>
       </c>
-      <c r="D131" s="2" t="s">
+      <c r="B132" s="4" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="132" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A132" s="3" t="s">
+      <c r="D132" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="B132" s="4" t="s">
+    </row>
+    <row r="133" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="3" t="s">
         <v>429</v>
       </c>
-      <c r="D132" s="2" t="s">
+      <c r="B133" s="4" t="s">
         <v>430</v>
       </c>
-    </row>
-    <row r="133" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="3" t="s">
+      <c r="C133" s="5" t="s">
         <v>431</v>
       </c>
-      <c r="B133" s="4" t="s">
+      <c r="D133" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="C133" s="5" t="s">
+    </row>
+    <row r="134" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="3" t="s">
         <v>433</v>
       </c>
-      <c r="D133" s="2" t="s">
+      <c r="B134" s="4" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="134" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A134" s="3" t="s">
+      <c r="D134" s="2" t="s">
         <v>435</v>
       </c>
-      <c r="B134" s="4" t="s">
+    </row>
+    <row r="135" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="3" t="s">
         <v>436</v>
       </c>
-      <c r="D134" s="2" t="s">
+      <c r="B135" s="4" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="135" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A135" s="3" t="s">
+      <c r="D135" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="B135" s="4" t="s">
+    </row>
+    <row r="136" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="3" t="s">
         <v>439</v>
       </c>
-      <c r="D135" s="2" t="s">
+      <c r="B136" s="4" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="136" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A136" s="3" t="s">
+      <c r="D136" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="B136" s="4" t="s">
+    </row>
+    <row r="137" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="3" t="s">
         <v>442</v>
       </c>
-      <c r="D136" s="2" t="s">
+      <c r="B137" s="4" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="137" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A137" s="3" t="s">
+      <c r="D137" s="2" t="s">
         <v>444</v>
       </c>
-      <c r="B137" s="4" t="s">
+    </row>
+    <row r="138" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="3" t="s">
         <v>445</v>
       </c>
-      <c r="D137" s="2" t="s">
+      <c r="B138" s="4" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="138" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A138" s="3" t="s">
+      <c r="C138" s="5" t="s">
         <v>447</v>
       </c>
-      <c r="B138" s="4" t="s">
+      <c r="D138" s="2" t="s">
         <v>448</v>
       </c>
-      <c r="C138" s="5" t="s">
+    </row>
+    <row r="139" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="3" t="s">
         <v>449</v>
       </c>
-      <c r="D138" s="2" t="s">
+      <c r="B139" s="4" t="s">
         <v>450</v>
       </c>
-    </row>
-    <row r="139" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A139" s="3" t="s">
+      <c r="D139" s="2" t="s">
         <v>451</v>
       </c>
-      <c r="B139" s="4" t="s">
+    </row>
+    <row r="140" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="3" t="s">
         <v>452</v>
       </c>
-      <c r="D139" s="2" t="s">
+      <c r="B140" s="4" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="140" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A140" s="3" t="s">
+      <c r="C140" s="5" t="s">
         <v>454</v>
       </c>
-      <c r="B140" s="4" t="s">
+      <c r="D140" s="2" t="s">
         <v>455</v>
       </c>
-      <c r="C140" s="5" t="s">
+    </row>
+    <row r="141" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="3" t="s">
         <v>456</v>
       </c>
-      <c r="D140" s="2" t="s">
+      <c r="B141" s="4" t="s">
         <v>457</v>
       </c>
-    </row>
-    <row r="141" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A141" s="3" t="s">
+      <c r="D141" s="2" t="s">
         <v>458</v>
       </c>
-      <c r="B141" s="4" t="s">
+    </row>
+    <row r="142" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A142" s="3" t="s">
         <v>459</v>
       </c>
-      <c r="D141" s="2" t="s">
+      <c r="B142" s="4" t="s">
+        <v>461</v>
+      </c>
+      <c r="C142" s="5" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="142" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A142" s="3" t="s">
-        <v>461</v>
-      </c>
-      <c r="B142" s="4" t="s">
+      <c r="D142" s="2" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="3" t="s">
         <v>463</v>
       </c>
-      <c r="C142" s="5" t="s">
-        <v>462</v>
-      </c>
-      <c r="D142" s="2" t="s">
+      <c r="B143" s="4" t="s">
         <v>464</v>
       </c>
-    </row>
-    <row r="143" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A143" s="3" t="s">
+      <c r="D143" s="2" t="s">
         <v>465</v>
       </c>
-      <c r="B143" s="4" t="s">
+    </row>
+    <row r="144" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="3" t="s">
         <v>466</v>
       </c>
-      <c r="D143" s="2" t="s">
+      <c r="B144" s="4" t="s">
+        <v>468</v>
+      </c>
+      <c r="C144" s="5" t="s">
         <v>467</v>
       </c>
-    </row>
-    <row r="144" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A144" s="3" t="s">
-        <v>468</v>
-      </c>
-      <c r="B144" s="4" t="s">
+      <c r="D144" s="2" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="3" t="s">
         <v>470</v>
       </c>
-      <c r="C144" s="5" t="s">
-        <v>469</v>
-      </c>
-      <c r="D144" s="2" t="s">
+      <c r="B145" s="4" t="s">
         <v>471</v>
       </c>
-    </row>
-    <row r="145" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A145" s="3" t="s">
+      <c r="C145" s="5" t="s">
         <v>472</v>
       </c>
-      <c r="B145" s="4" t="s">
+      <c r="D145" s="2" t="s">
         <v>473</v>
       </c>
-      <c r="C145" s="5" t="s">
+    </row>
+    <row r="146" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="3" t="s">
         <v>474</v>
       </c>
-      <c r="D145" s="2" t="s">
+      <c r="B146" s="4" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="146" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A146" s="3" t="s">
+      <c r="D146" s="2" t="s">
         <v>476</v>
       </c>
-      <c r="B146" s="4" t="s">
+    </row>
+    <row r="147" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="3" t="s">
         <v>477</v>
       </c>
-      <c r="D146" s="2" t="s">
+      <c r="B147" s="4" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="147" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A147" s="3" t="s">
+      <c r="C147" s="5" t="s">
         <v>479</v>
       </c>
-      <c r="B147" s="4" t="s">
+      <c r="D147" s="2" t="s">
         <v>480</v>
       </c>
-      <c r="C147" s="5" t="s">
+    </row>
+    <row r="148" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A148" s="3" t="s">
         <v>481</v>
       </c>
-      <c r="D147" s="2" t="s">
+      <c r="B148" s="4" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="148" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A148" s="3" t="s">
-        <v>483</v>
-      </c>
-      <c r="B148" s="4" t="s">
-        <v>484</v>
-      </c>
       <c r="D148" s="2" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="150" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="151" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="152" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="153" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="154" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="155" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="156" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="157" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="158" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="159" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="160" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="161" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="162" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="163" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="164" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="165" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="166" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="167" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="168" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="169" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="170" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="171" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="172" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="173" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="174" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="175" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="176" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="177" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="178" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="179" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="180" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="181" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="182" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="183" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="184" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="185" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="186" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="187" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="188" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="189" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="190" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="191" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="192" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="193" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="194" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="195" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="196" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="197" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="198" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="199" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="200" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="201" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="202" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="203" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="204" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="205" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="206" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="207" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="208" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="209" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="210" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="211" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="212" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="213" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="214" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="215" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="216" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="217" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="218" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="219" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="220" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="221" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="222" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="223" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="224" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="225" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="226" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="227" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="228" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="229" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="230" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="231" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="232" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="233" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="234" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="235" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="236" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="237" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="238" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="239" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="240" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="241" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="242" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="243" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="244" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="245" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="246" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="247" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="248" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="249" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="250" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="251" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="252" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="253" ht="409.6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="351" ht="218.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="352" ht="409.6" customHeight="1" x14ac:dyDescent="0.3"/>
+        <v>476</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="150" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="151" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="152" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="153" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="154" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="155" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="156" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="157" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="158" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="159" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="160" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="161" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="162" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="163" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="164" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="165" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="166" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="167" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="168" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="169" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="170" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="171" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="172" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="173" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="174" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="175" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="176" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="177" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="178" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="179" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="180" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="181" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="182" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="183" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="184" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="185" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="186" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="187" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="188" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="189" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="190" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="191" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="192" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="193" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="194" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="195" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="196" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="197" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="198" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="199" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="200" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="201" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="202" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="203" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="204" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="205" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="206" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="207" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="208" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="209" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="210" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="211" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="212" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="213" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="214" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="215" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="216" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="217" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="218" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="219" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="220" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="221" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="222" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="223" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="224" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="225" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="226" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="227" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="228" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="229" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="230" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="231" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="232" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="233" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="234" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="235" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="236" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="237" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="238" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="239" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="240" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="241" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="242" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="243" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="244" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="245" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="246" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="247" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="248" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="249" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="250" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="251" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="252" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="253" ht="409.6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="351" ht="218.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="352" ht="409.6" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Commit on 28.01.2019. Added navigation menu to all of the html files in the main docs folder.
</commit_message>
<xml_diff>
--- a/Exam Preparation/resources/70-480 Practice Exam Answers and Explanations.xlsx
+++ b/Exam Preparation/resources/70-480 Practice Exam Answers and Explanations.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="489">
   <si>
     <t>Question</t>
   </si>
@@ -63,9 +63,6 @@
     <t>Case Study II:</t>
   </si>
   <si>
-    <t>4.You need to modife the markup of the data input field so that it meets these requirements when the the form is submitted: *The input field cannot be empty. *The value in the input field must be a number between 0 and 100</t>
-  </si>
-  <si>
     <t>&lt;input id="data" type="number" min="0" max="100" required /&gt;</t>
   </si>
   <si>
@@ -79,9 +76,6 @@
   </si>
   <si>
     <t>&lt;input id="data" type="range" min="0" max="100" /&gt;</t>
-  </si>
-  <si>
-    <t>7.The user must select at least one topping.If not, want to display the message "Please select a topping" to the user and prevent the form from being submitted.If the user selects at least one topping, the form should be submitted.</t>
   </si>
   <si>
     <t>1.Modify the button element as follows: &lt;button onclick="return PlaceOrder();"&gt;Place Order&lt;/button&gt; 2.Add the following code at the beginning of the PlaceOrder function: let isValid = false;
@@ -116,9 +110,6 @@
     <t>My both answers were incorrect.Answer explanation: 1.This code modifies the onclick handler to return the return value of the PlaceOrder function.Returning false indicates to an element that ist default behavior should not occur.This way the PlaceOrder function returns false you prevent the button element from submitting the form which is its default behavior. 2. This code iterates all the check boxes to determine if at least one is checked.If so it sets a variable named isValid to true.If not the isValid variable reamains initialized as false.If the isValid variable is false the code displays the message "Please select a topping" to the user.It then returns false from the function.</t>
   </si>
   <si>
-    <t>8.You are using the following regilar expression to validate text in a string variable named data: [^\w\.@-] You need to write JavaScript code to determine wheter the pattern exists in the data variable.</t>
-  </si>
-  <si>
     <t>var regex = /[^\w\.@-]/;
 regex.test(data);</t>
   </si>
@@ -1916,6 +1907,21 @@
   </si>
   <si>
     <t>My answer is correct. Answer explanation: This code uses the $(":button") syntax to find all elements of type button.This includes &lt;input type="button"/&gt; elements and &lt;button&gt; elements.It then calls the css function to set a solid one-pixel red border.</t>
+  </si>
+  <si>
+    <t>Destination Verified</t>
+  </si>
+  <si>
+    <t>Destination Verified; Packages Created</t>
+  </si>
+  <si>
+    <t>4.You need to modify the markup of the data input field so that it meets these requirements when the the form is submitted: *The input field cannot be empty. *The value in the input field must be a number between 0 and 100</t>
+  </si>
+  <si>
+    <t>7.The user must select at least one topping.If not, you want to display the message "Please select a topping" to the user and prevent the form from being submitted.If the user selects at least one topping, the form should be submitted.</t>
+  </si>
+  <si>
+    <t>8.You are using the following regular expression to validate text in a string variable named data: [^\w\.@-] You need to write JavaScript code to determine wheter the pattern exists in the data variable.</t>
   </si>
 </sst>
 </file>
@@ -2346,8 +2352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D352"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A147" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="A148" sqref="A148"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="36" x14ac:dyDescent="0.25"/>
@@ -2385,7 +2391,7 @@
         <v>6</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2395,6 +2401,9 @@
       <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="C4" s="5" t="s">
+        <v>484</v>
+      </c>
       <c r="D4" s="2" t="s">
         <v>9</v>
       </c>
@@ -2406,6 +2415,9 @@
       <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="C5" s="5" t="s">
+        <v>485</v>
+      </c>
       <c r="D5" s="2" t="s">
         <v>12</v>
       </c>
@@ -2417,1720 +2429,1720 @@
     </row>
     <row r="7" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>486</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>15</v>
-      </c>
       <c r="D7" s="2" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="D8" s="2" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>19</v>
-      </c>
       <c r="D9" s="2" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
+        <v>487</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="D10" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
+        <v>488</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="D44" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D45" s="2" t="s">
         <v>135</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="D47" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B50" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="D50" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="D51" s="2" t="s">
         <v>156</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="D52" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="D57" s="2" t="s">
         <v>176</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="D60" s="2" t="s">
         <v>186</v>
-      </c>
-      <c r="B60" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="D64" s="2" t="s">
         <v>199</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="D66" s="2" t="s">
         <v>205</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="C66" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="D67" s="2" t="s">
         <v>209</v>
-      </c>
-      <c r="B67" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="C67" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="D75" s="2" t="s">
         <v>235</v>
-      </c>
-      <c r="B75" s="4" t="s">
-        <v>236</v>
-      </c>
-      <c r="C75" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B77" s="4">
         <v>12</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="C78" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="D78" s="2" t="s">
         <v>244</v>
-      </c>
-      <c r="B78" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="C78" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="D78" s="2" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B79" s="4">
         <v>105</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="D80" s="2" t="s">
         <v>250</v>
-      </c>
-      <c r="B80" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="C80" s="5" t="s">
-        <v>251</v>
-      </c>
-      <c r="D80" s="2" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="D81" s="2" t="s">
         <v>254</v>
-      </c>
-      <c r="B81" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="C81" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="C83" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="D83" s="2" t="s">
         <v>261</v>
-      </c>
-      <c r="B83" s="4" t="s">
-        <v>262</v>
-      </c>
-      <c r="C83" s="5" t="s">
-        <v>263</v>
-      </c>
-      <c r="D83" s="2" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="C84" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="B84" s="4" t="s">
+      <c r="D84" s="2" t="s">
         <v>266</v>
-      </c>
-      <c r="C84" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="D84" s="2" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="C86" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="D86" s="2" t="s">
         <v>273</v>
-      </c>
-      <c r="B86" s="4" t="s">
-        <v>274</v>
-      </c>
-      <c r="C86" s="5" t="s">
-        <v>275</v>
-      </c>
-      <c r="D86" s="2" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="C87" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="D87" s="2" t="s">
         <v>277</v>
-      </c>
-      <c r="B87" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="C87" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="D87" s="2" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="C88" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="D88" s="2" t="s">
         <v>281</v>
-      </c>
-      <c r="B88" s="4" t="s">
-        <v>282</v>
-      </c>
-      <c r="C88" s="5" t="s">
-        <v>283</v>
-      </c>
-      <c r="D88" s="2" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="C92" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="D92" s="2" t="s">
         <v>294</v>
-      </c>
-      <c r="B92" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="C92" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="D92" s="2" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="B93" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="C93" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="D93" s="2" t="s">
         <v>298</v>
-      </c>
-      <c r="B93" s="4" t="s">
-        <v>299</v>
-      </c>
-      <c r="C93" s="5" t="s">
-        <v>300</v>
-      </c>
-      <c r="D93" s="2" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="B97" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="C97" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="D97" s="2" t="s">
         <v>311</v>
-      </c>
-      <c r="C97" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="D97" s="2" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="B99" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="C99" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="D99" s="2" t="s">
         <v>318</v>
-      </c>
-      <c r="B99" s="4" t="s">
-        <v>319</v>
-      </c>
-      <c r="C99" s="5" t="s">
-        <v>320</v>
-      </c>
-      <c r="D99" s="2" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="B102" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="C102" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="D102" s="2" t="s">
         <v>328</v>
-      </c>
-      <c r="B102" s="4" t="s">
-        <v>329</v>
-      </c>
-      <c r="C102" s="5" t="s">
-        <v>330</v>
-      </c>
-      <c r="D102" s="2" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="B103" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="C103" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="D103" s="2" t="s">
         <v>332</v>
-      </c>
-      <c r="B103" s="4" t="s">
-        <v>333</v>
-      </c>
-      <c r="C103" s="5" t="s">
-        <v>334</v>
-      </c>
-      <c r="D103" s="2" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="B104" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="C104" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="D104" s="2" t="s">
         <v>336</v>
-      </c>
-      <c r="B104" s="4" t="s">
-        <v>338</v>
-      </c>
-      <c r="C104" s="5" t="s">
-        <v>337</v>
-      </c>
-      <c r="D104" s="2" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="B110" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="C110" s="5" t="s">
+        <v>354</v>
+      </c>
+      <c r="D110" s="2" t="s">
         <v>355</v>
-      </c>
-      <c r="B110" s="4" t="s">
-        <v>356</v>
-      </c>
-      <c r="C110" s="5" t="s">
-        <v>357</v>
-      </c>
-      <c r="D110" s="2" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="B115" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="C115" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="D115" s="2" t="s">
         <v>371</v>
-      </c>
-      <c r="B115" s="4" t="s">
-        <v>372</v>
-      </c>
-      <c r="C115" s="5" t="s">
-        <v>373</v>
-      </c>
-      <c r="D115" s="2" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="B117" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="C117" s="5" t="s">
+        <v>377</v>
+      </c>
+      <c r="D117" s="2" t="s">
         <v>378</v>
-      </c>
-      <c r="B117" s="4" t="s">
-        <v>379</v>
-      </c>
-      <c r="C117" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="D117" s="2" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="121" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
     <row r="122" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="123" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
     </row>
     <row r="124" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
     </row>
     <row r="125" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="B127" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="C127" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="D127" s="2" t="s">
         <v>408</v>
-      </c>
-      <c r="B127" s="4" t="s">
-        <v>409</v>
-      </c>
-      <c r="C127" s="5" t="s">
-        <v>410</v>
-      </c>
-      <c r="D127" s="2" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
     </row>
     <row r="129" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="B129" s="4" t="s">
+        <v>413</v>
+      </c>
+      <c r="C129" s="5" t="s">
+        <v>414</v>
+      </c>
+      <c r="D129" s="2" t="s">
         <v>415</v>
-      </c>
-      <c r="B129" s="4" t="s">
-        <v>416</v>
-      </c>
-      <c r="C129" s="5" t="s">
-        <v>417</v>
-      </c>
-      <c r="D129" s="2" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="130" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="B130" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C130" s="5" t="s">
+        <v>418</v>
+      </c>
+      <c r="D130" s="2" t="s">
         <v>419</v>
-      </c>
-      <c r="B130" s="4" t="s">
-        <v>420</v>
-      </c>
-      <c r="C130" s="5" t="s">
-        <v>421</v>
-      </c>
-      <c r="D130" s="2" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="131" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
     </row>
     <row r="132" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
     </row>
     <row r="133" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
+        <v>426</v>
+      </c>
+      <c r="B133" s="4" t="s">
+        <v>427</v>
+      </c>
+      <c r="C133" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="D133" s="2" t="s">
         <v>429</v>
-      </c>
-      <c r="B133" s="4" t="s">
-        <v>430</v>
-      </c>
-      <c r="C133" s="5" t="s">
-        <v>431</v>
-      </c>
-      <c r="D133" s="2" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="134" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="B134" s="4" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
     </row>
     <row r="135" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
     </row>
     <row r="136" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="B136" s="4" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="B137" s="4" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="138" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="B138" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="C138" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="D138" s="2" t="s">
         <v>445</v>
-      </c>
-      <c r="B138" s="4" t="s">
-        <v>446</v>
-      </c>
-      <c r="C138" s="5" t="s">
-        <v>447</v>
-      </c>
-      <c r="D138" s="2" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="139" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="B139" s="4" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
     </row>
     <row r="140" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
+        <v>449</v>
+      </c>
+      <c r="B140" s="4" t="s">
+        <v>450</v>
+      </c>
+      <c r="C140" s="5" t="s">
+        <v>451</v>
+      </c>
+      <c r="D140" s="2" t="s">
         <v>452</v>
-      </c>
-      <c r="B140" s="4" t="s">
-        <v>453</v>
-      </c>
-      <c r="C140" s="5" t="s">
-        <v>454</v>
-      </c>
-      <c r="D140" s="2" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="141" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="B141" s="4" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
     </row>
     <row r="142" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
+        <v>456</v>
+      </c>
+      <c r="B142" s="4" t="s">
+        <v>458</v>
+      </c>
+      <c r="C142" s="5" t="s">
+        <v>457</v>
+      </c>
+      <c r="D142" s="2" t="s">
         <v>459</v>
-      </c>
-      <c r="B142" s="4" t="s">
-        <v>461</v>
-      </c>
-      <c r="C142" s="5" t="s">
-        <v>460</v>
-      </c>
-      <c r="D142" s="2" t="s">
-        <v>462</v>
       </c>
     </row>
     <row r="143" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="B143" s="4" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
     </row>
     <row r="144" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
+        <v>463</v>
+      </c>
+      <c r="B144" s="4" t="s">
+        <v>465</v>
+      </c>
+      <c r="C144" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="D144" s="2" t="s">
         <v>466</v>
-      </c>
-      <c r="B144" s="4" t="s">
-        <v>468</v>
-      </c>
-      <c r="C144" s="5" t="s">
-        <v>467</v>
-      </c>
-      <c r="D144" s="2" t="s">
-        <v>469</v>
       </c>
     </row>
     <row r="145" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
+        <v>467</v>
+      </c>
+      <c r="B145" s="4" t="s">
+        <v>468</v>
+      </c>
+      <c r="C145" s="5" t="s">
+        <v>469</v>
+      </c>
+      <c r="D145" s="2" t="s">
         <v>470</v>
-      </c>
-      <c r="B145" s="4" t="s">
-        <v>471</v>
-      </c>
-      <c r="C145" s="5" t="s">
-        <v>472</v>
-      </c>
-      <c r="D145" s="2" t="s">
-        <v>473</v>
       </c>
     </row>
     <row r="146" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="B146" s="4" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
     </row>
     <row r="147" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
+        <v>474</v>
+      </c>
+      <c r="B147" s="4" t="s">
+        <v>475</v>
+      </c>
+      <c r="C147" s="5" t="s">
+        <v>476</v>
+      </c>
+      <c r="D147" s="2" t="s">
         <v>477</v>
-      </c>
-      <c r="B147" s="4" t="s">
-        <v>478</v>
-      </c>
-      <c r="C147" s="5" t="s">
-        <v>479</v>
-      </c>
-      <c r="D147" s="2" t="s">
-        <v>480</v>
       </c>
     </row>
     <row r="148" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="B148" s="4" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
     </row>
     <row r="149" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Commit on 29.01.2019. Minor changes added to the excel file.
</commit_message>
<xml_diff>
--- a/Exam Preparation/resources/70-480 Practice Exam Answers and Explanations.xlsx
+++ b/Exam Preparation/resources/70-480 Practice Exam Answers and Explanations.xlsx
@@ -239,9 +239,6 @@
     <t>Add this code between lines 20 and 21: throw e;</t>
   </si>
   <si>
-    <t>Add this code between lines 20 and 21:                                                                                                                                    finally{ CalculateDefaultShipping(); }</t>
-  </si>
-  <si>
     <t>My answer is incorrect.Answer explanation: The throw statement allows you to re-throw an error that is caught,By default when an error is handled in a catch block it is not propagated up the call stack.By re-throwing the error you allow the catch block higher in the call stack to handle the error.In this scenario the catch block in the call stack executes the CalculateDefaultShipping function.</t>
   </si>
   <si>
@@ -1922,6 +1919,9 @@
   </si>
   <si>
     <t>8.You are using the following regular expression to validate text in a string variable named data: [^\w\.@-] You need to write JavaScript code to determine wheter the pattern exists in the data variable.</t>
+  </si>
+  <si>
+    <t>Add this code between lines 20 and 21:                                                                                                                                                    finally{ CalculateDefaultShipping(); }</t>
   </si>
 </sst>
 </file>
@@ -2352,8 +2352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D352"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="C19" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="36" x14ac:dyDescent="0.25"/>
@@ -2391,7 +2391,7 @@
         <v>6</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2402,7 +2402,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>9</v>
@@ -2416,7 +2416,7 @@
         <v>11</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>12</v>
@@ -2429,13 +2429,13 @@
     </row>
     <row r="7" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2446,7 +2446,7 @@
         <v>16</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2457,12 +2457,12 @@
         <v>18</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>19</v>
@@ -2476,7 +2476,7 @@
     </row>
     <row r="11" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>22</v>
@@ -2532,7 +2532,7 @@
         <v>36</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>37</v>
@@ -2596,1553 +2596,1553 @@
         <v>53</v>
       </c>
       <c r="C20" s="5" t="s">
+        <v>488</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="C21" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="D21" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="D22" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="D23" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="C24" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="D24" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="D25" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="C26" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="D26" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="D27" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="D28" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>84</v>
-      </c>
       <c r="D29" s="2" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B30" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="D30" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="D31" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="D32" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="D33" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B34" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="D34" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B35" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="D35" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B36" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="D36" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B37" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="D37" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B38" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="D38" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B39" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="D39" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B40" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="D40" s="2" t="s">
         <v>116</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B41" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="D41" s="2" t="s">
         <v>119</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B42" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="C42" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="D42" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B43" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="C43" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="D43" s="2" t="s">
         <v>126</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B44" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="C44" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="D44" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B45" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="C45" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="C45" s="5" t="s">
+      <c r="D45" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B46" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="D46" s="2" t="s">
         <v>137</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B47" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="C47" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="C47" s="5" t="s">
+      <c r="D47" s="2" t="s">
         <v>141</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B48" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="D48" s="2" t="s">
         <v>144</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B49" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="D49" s="2" t="s">
         <v>147</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D50" s="2" t="s">
         <v>151</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B51" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="C51" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="C51" s="5" t="s">
+      <c r="D51" s="2" t="s">
         <v>155</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B52" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="C52" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="C52" s="5" t="s">
+      <c r="D52" s="2" t="s">
         <v>159</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B53" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="D53" s="2" t="s">
         <v>162</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B54" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="D54" s="2" t="s">
         <v>165</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B55" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="D55" s="2" t="s">
         <v>168</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B56" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="D56" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="C57" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="D57" s="2" t="s">
         <v>175</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B58" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="D58" s="2" t="s">
         <v>178</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B59" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="D59" s="2" t="s">
         <v>181</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B60" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="C60" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="C60" s="5" t="s">
+      <c r="D60" s="2" t="s">
         <v>185</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B61" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="D61" s="2" t="s">
         <v>188</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B62" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="D62" s="2" t="s">
         <v>191</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B63" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="D63" s="2" t="s">
         <v>194</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B64" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="C64" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="C64" s="5" t="s">
+      <c r="D64" s="2" t="s">
         <v>198</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="D65" s="2" t="s">
         <v>200</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="B66" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="C66" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="C66" s="5" t="s">
+      <c r="D66" s="2" t="s">
         <v>204</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B67" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="C67" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="C67" s="5" t="s">
+      <c r="D67" s="2" t="s">
         <v>208</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B68" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="D68" s="2" t="s">
         <v>211</v>
-      </c>
-      <c r="D68" s="2" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="B69" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="D69" s="2" t="s">
         <v>215</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="B70" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="D70" s="2" t="s">
         <v>218</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B71" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="D71" s="2" t="s">
         <v>220</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="B72" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="D72" s="2" t="s">
         <v>224</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="B73" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="D73" s="2" t="s">
         <v>227</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="B74" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="D74" s="2" t="s">
         <v>230</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="B75" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="B75" s="4" t="s">
+      <c r="C75" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="C75" s="5" t="s">
+      <c r="D75" s="2" t="s">
         <v>234</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="B76" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="B76" s="4" t="s">
+      <c r="D76" s="2" t="s">
         <v>237</v>
-      </c>
-      <c r="D76" s="2" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B77" s="4">
         <v>12</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="B78" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="B78" s="4" t="s">
+      <c r="C78" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="C78" s="5" t="s">
+      <c r="D78" s="2" t="s">
         <v>243</v>
-      </c>
-      <c r="D78" s="2" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B79" s="4">
         <v>105</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="C80" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="B80" s="4" t="s">
+      <c r="D80" s="2" t="s">
         <v>249</v>
-      </c>
-      <c r="C80" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="D80" s="2" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="B81" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="B81" s="4" t="s">
+      <c r="C81" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="C81" s="5" t="s">
+      <c r="D81" s="2" t="s">
         <v>253</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="B82" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="B82" s="4" t="s">
+      <c r="D82" s="2" t="s">
         <v>256</v>
-      </c>
-      <c r="D82" s="2" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="B83" s="4" t="s">
         <v>258</v>
       </c>
-      <c r="B83" s="4" t="s">
+      <c r="C83" s="5" t="s">
         <v>259</v>
       </c>
-      <c r="C83" s="5" t="s">
+      <c r="D83" s="2" t="s">
         <v>260</v>
-      </c>
-      <c r="D83" s="2" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="B84" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="B84" s="4" t="s">
-        <v>263</v>
-      </c>
       <c r="C84" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="D84" s="2" t="s">
         <v>265</v>
-      </c>
-      <c r="D84" s="2" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="B85" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="B85" s="4" t="s">
+      <c r="D85" s="2" t="s">
         <v>268</v>
-      </c>
-      <c r="D85" s="2" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="B86" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="B86" s="4" t="s">
+      <c r="C86" s="5" t="s">
         <v>271</v>
       </c>
-      <c r="C86" s="5" t="s">
+      <c r="D86" s="2" t="s">
         <v>272</v>
-      </c>
-      <c r="D86" s="2" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="B87" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="B87" s="4" t="s">
+      <c r="C87" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="C87" s="5" t="s">
+      <c r="D87" s="2" t="s">
         <v>276</v>
-      </c>
-      <c r="D87" s="2" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="B88" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="B88" s="4" t="s">
+      <c r="C88" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="C88" s="5" t="s">
+      <c r="D88" s="2" t="s">
         <v>280</v>
-      </c>
-      <c r="D88" s="2" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="B89" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="B89" s="4" t="s">
+      <c r="D89" s="2" t="s">
         <v>283</v>
-      </c>
-      <c r="D89" s="2" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="B90" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="B90" s="4" t="s">
+      <c r="D90" s="2" t="s">
         <v>286</v>
-      </c>
-      <c r="D90" s="2" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="B91" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="B91" s="4" t="s">
+      <c r="D91" s="2" t="s">
         <v>289</v>
-      </c>
-      <c r="D91" s="2" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="B92" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="B92" s="4" t="s">
+      <c r="C92" s="5" t="s">
         <v>292</v>
       </c>
-      <c r="C92" s="5" t="s">
+      <c r="D92" s="2" t="s">
         <v>293</v>
-      </c>
-      <c r="D92" s="2" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="B93" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="B93" s="4" t="s">
+      <c r="C93" s="5" t="s">
         <v>296</v>
       </c>
-      <c r="C93" s="5" t="s">
+      <c r="D93" s="2" t="s">
         <v>297</v>
-      </c>
-      <c r="D93" s="2" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="B94" s="4" t="s">
         <v>299</v>
       </c>
-      <c r="B94" s="4" t="s">
+      <c r="D94" s="2" t="s">
         <v>300</v>
-      </c>
-      <c r="D94" s="2" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="B95" s="4" t="s">
         <v>302</v>
       </c>
-      <c r="B95" s="4" t="s">
+      <c r="D95" s="2" t="s">
         <v>303</v>
-      </c>
-      <c r="D95" s="2" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="B96" s="4" t="s">
         <v>305</v>
       </c>
-      <c r="B96" s="4" t="s">
+      <c r="D96" s="2" t="s">
         <v>306</v>
-      </c>
-      <c r="D96" s="2" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="B97" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="C97" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="D97" s="2" t="s">
         <v>310</v>
-      </c>
-      <c r="B97" s="4" t="s">
-        <v>308</v>
-      </c>
-      <c r="C97" s="5" t="s">
-        <v>309</v>
-      </c>
-      <c r="D97" s="2" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="B98" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="B98" s="4" t="s">
+      <c r="D98" s="2" t="s">
         <v>313</v>
-      </c>
-      <c r="D98" s="2" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="B99" s="4" t="s">
         <v>315</v>
       </c>
-      <c r="B99" s="4" t="s">
+      <c r="C99" s="5" t="s">
         <v>316</v>
       </c>
-      <c r="C99" s="5" t="s">
+      <c r="D99" s="2" t="s">
         <v>317</v>
-      </c>
-      <c r="D99" s="2" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="B100" s="4" t="s">
         <v>319</v>
       </c>
-      <c r="B100" s="4" t="s">
+      <c r="D100" s="2" t="s">
         <v>320</v>
-      </c>
-      <c r="D100" s="2" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="B101" s="4" t="s">
         <v>322</v>
       </c>
-      <c r="B101" s="4" t="s">
+      <c r="D101" s="2" t="s">
         <v>323</v>
-      </c>
-      <c r="D101" s="2" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="B102" s="4" t="s">
         <v>325</v>
       </c>
-      <c r="B102" s="4" t="s">
+      <c r="C102" s="5" t="s">
         <v>326</v>
       </c>
-      <c r="C102" s="5" t="s">
+      <c r="D102" s="2" t="s">
         <v>327</v>
-      </c>
-      <c r="D102" s="2" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="B103" s="4" t="s">
         <v>329</v>
       </c>
-      <c r="B103" s="4" t="s">
+      <c r="C103" s="5" t="s">
         <v>330</v>
       </c>
-      <c r="C103" s="5" t="s">
+      <c r="D103" s="2" t="s">
         <v>331</v>
-      </c>
-      <c r="D103" s="2" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="B104" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="C104" s="5" t="s">
         <v>333</v>
       </c>
-      <c r="B104" s="4" t="s">
+      <c r="D104" s="2" t="s">
         <v>335</v>
-      </c>
-      <c r="C104" s="5" t="s">
-        <v>334</v>
-      </c>
-      <c r="D104" s="2" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="B105" s="4" t="s">
         <v>337</v>
       </c>
-      <c r="B105" s="4" t="s">
+      <c r="D105" s="2" t="s">
         <v>338</v>
-      </c>
-      <c r="D105" s="2" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B106" s="4" t="s">
         <v>340</v>
       </c>
-      <c r="B106" s="4" t="s">
+      <c r="D106" s="2" t="s">
         <v>341</v>
-      </c>
-      <c r="D106" s="2" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="B107" s="4" t="s">
         <v>343</v>
       </c>
-      <c r="B107" s="4" t="s">
+      <c r="D107" s="2" t="s">
         <v>344</v>
-      </c>
-      <c r="D107" s="2" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="B108" s="4" t="s">
         <v>346</v>
       </c>
-      <c r="B108" s="4" t="s">
+      <c r="D108" s="2" t="s">
         <v>347</v>
-      </c>
-      <c r="D108" s="2" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="B109" s="4" t="s">
         <v>349</v>
       </c>
-      <c r="B109" s="4" t="s">
+      <c r="D109" s="2" t="s">
         <v>350</v>
-      </c>
-      <c r="D109" s="2" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="B110" s="4" t="s">
         <v>352</v>
       </c>
-      <c r="B110" s="4" t="s">
+      <c r="C110" s="5" t="s">
         <v>353</v>
       </c>
-      <c r="C110" s="5" t="s">
+      <c r="D110" s="2" t="s">
         <v>354</v>
-      </c>
-      <c r="D110" s="2" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="B111" s="4" t="s">
         <v>356</v>
       </c>
-      <c r="B111" s="4" t="s">
+      <c r="D111" s="2" t="s">
         <v>357</v>
-      </c>
-      <c r="D111" s="2" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="B112" s="4" t="s">
         <v>359</v>
       </c>
-      <c r="B112" s="4" t="s">
+      <c r="D112" s="2" t="s">
         <v>360</v>
-      </c>
-      <c r="D112" s="2" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="B113" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="B113" s="4" t="s">
+      <c r="D113" s="2" t="s">
         <v>363</v>
-      </c>
-      <c r="D113" s="2" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="B114" s="4" t="s">
         <v>365</v>
       </c>
-      <c r="B114" s="4" t="s">
+      <c r="D114" s="2" t="s">
         <v>366</v>
-      </c>
-      <c r="D114" s="2" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="B115" s="4" t="s">
         <v>368</v>
       </c>
-      <c r="B115" s="4" t="s">
+      <c r="C115" s="5" t="s">
         <v>369</v>
       </c>
-      <c r="C115" s="5" t="s">
+      <c r="D115" s="2" t="s">
         <v>370</v>
-      </c>
-      <c r="D115" s="2" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="B116" s="4" t="s">
         <v>372</v>
       </c>
-      <c r="B116" s="4" t="s">
+      <c r="D116" s="2" t="s">
         <v>373</v>
-      </c>
-      <c r="D116" s="2" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="B117" s="4" t="s">
         <v>375</v>
       </c>
-      <c r="B117" s="4" t="s">
+      <c r="C117" s="5" t="s">
         <v>376</v>
       </c>
-      <c r="C117" s="5" t="s">
+      <c r="D117" s="2" t="s">
         <v>377</v>
-      </c>
-      <c r="D117" s="2" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="B118" s="4" t="s">
         <v>379</v>
       </c>
-      <c r="B118" s="4" t="s">
+      <c r="D118" s="2" t="s">
         <v>380</v>
-      </c>
-      <c r="D118" s="2" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="B119" s="4" t="s">
         <v>382</v>
       </c>
-      <c r="B119" s="4" t="s">
+      <c r="D119" s="2" t="s">
         <v>383</v>
-      </c>
-      <c r="D119" s="2" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="B120" s="4" t="s">
         <v>385</v>
       </c>
-      <c r="B120" s="4" t="s">
+      <c r="D120" s="2" t="s">
         <v>386</v>
-      </c>
-      <c r="D120" s="2" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="121" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="B121" s="4" t="s">
         <v>388</v>
       </c>
-      <c r="B121" s="4" t="s">
+      <c r="D121" s="2" t="s">
         <v>389</v>
-      </c>
-      <c r="D121" s="2" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="122" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="B122" s="4" t="s">
         <v>391</v>
       </c>
-      <c r="B122" s="4" t="s">
+      <c r="D122" s="2" t="s">
         <v>392</v>
-      </c>
-      <c r="D122" s="2" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="123" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="B123" s="4" t="s">
         <v>394</v>
       </c>
-      <c r="B123" s="4" t="s">
+      <c r="D123" s="2" t="s">
         <v>395</v>
-      </c>
-      <c r="D123" s="2" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="124" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="B124" s="4" t="s">
         <v>397</v>
       </c>
-      <c r="B124" s="4" t="s">
-        <v>398</v>
-      </c>
       <c r="D124" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="125" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="B125" s="4" t="s">
         <v>399</v>
       </c>
-      <c r="B125" s="4" t="s">
+      <c r="D125" s="2" t="s">
         <v>400</v>
-      </c>
-      <c r="D125" s="2" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B126" s="4" t="s">
         <v>402</v>
       </c>
-      <c r="B126" s="4" t="s">
+      <c r="D126" s="2" t="s">
         <v>403</v>
-      </c>
-      <c r="D126" s="2" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
+        <v>404</v>
+      </c>
+      <c r="B127" s="4" t="s">
         <v>405</v>
       </c>
-      <c r="B127" s="4" t="s">
+      <c r="C127" s="5" t="s">
         <v>406</v>
       </c>
-      <c r="C127" s="5" t="s">
+      <c r="D127" s="2" t="s">
         <v>407</v>
-      </c>
-      <c r="D127" s="2" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="B128" s="4" t="s">
         <v>409</v>
       </c>
-      <c r="B128" s="4" t="s">
+      <c r="D128" s="2" t="s">
         <v>410</v>
-      </c>
-      <c r="D128" s="2" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="129" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="B129" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="B129" s="4" t="s">
+      <c r="C129" s="5" t="s">
         <v>413</v>
       </c>
-      <c r="C129" s="5" t="s">
+      <c r="D129" s="2" t="s">
         <v>414</v>
-      </c>
-      <c r="D129" s="2" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="130" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="B130" s="4" t="s">
         <v>416</v>
       </c>
-      <c r="B130" s="4" t="s">
+      <c r="C130" s="5" t="s">
         <v>417</v>
       </c>
-      <c r="C130" s="5" t="s">
+      <c r="D130" s="2" t="s">
         <v>418</v>
-      </c>
-      <c r="D130" s="2" t="s">
-        <v>419</v>
       </c>
     </row>
     <row r="131" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="B131" s="4" t="s">
         <v>420</v>
       </c>
-      <c r="B131" s="4" t="s">
+      <c r="D131" s="2" t="s">
         <v>421</v>
-      </c>
-      <c r="D131" s="2" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="132" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="B132" s="4" t="s">
         <v>423</v>
       </c>
-      <c r="B132" s="4" t="s">
+      <c r="D132" s="2" t="s">
         <v>424</v>
-      </c>
-      <c r="D132" s="2" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="133" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
+        <v>425</v>
+      </c>
+      <c r="B133" s="4" t="s">
         <v>426</v>
       </c>
-      <c r="B133" s="4" t="s">
+      <c r="C133" s="5" t="s">
         <v>427</v>
       </c>
-      <c r="C133" s="5" t="s">
+      <c r="D133" s="2" t="s">
         <v>428</v>
-      </c>
-      <c r="D133" s="2" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="134" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="B134" s="4" t="s">
         <v>430</v>
       </c>
-      <c r="B134" s="4" t="s">
+      <c r="D134" s="2" t="s">
         <v>431</v>
-      </c>
-      <c r="D134" s="2" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="135" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="B135" s="4" t="s">
         <v>433</v>
       </c>
-      <c r="B135" s="4" t="s">
+      <c r="D135" s="2" t="s">
         <v>434</v>
-      </c>
-      <c r="D135" s="2" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="136" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="B136" s="4" t="s">
         <v>436</v>
       </c>
-      <c r="B136" s="4" t="s">
+      <c r="D136" s="2" t="s">
         <v>437</v>
-      </c>
-      <c r="D136" s="2" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="B137" s="4" t="s">
         <v>439</v>
       </c>
-      <c r="B137" s="4" t="s">
+      <c r="D137" s="2" t="s">
         <v>440</v>
-      </c>
-      <c r="D137" s="2" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="138" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="B138" s="4" t="s">
         <v>442</v>
       </c>
-      <c r="B138" s="4" t="s">
+      <c r="C138" s="5" t="s">
         <v>443</v>
       </c>
-      <c r="C138" s="5" t="s">
+      <c r="D138" s="2" t="s">
         <v>444</v>
-      </c>
-      <c r="D138" s="2" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="139" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
+        <v>445</v>
+      </c>
+      <c r="B139" s="4" t="s">
         <v>446</v>
       </c>
-      <c r="B139" s="4" t="s">
+      <c r="D139" s="2" t="s">
         <v>447</v>
-      </c>
-      <c r="D139" s="2" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="140" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="B140" s="4" t="s">
         <v>449</v>
       </c>
-      <c r="B140" s="4" t="s">
+      <c r="C140" s="5" t="s">
         <v>450</v>
       </c>
-      <c r="C140" s="5" t="s">
+      <c r="D140" s="2" t="s">
         <v>451</v>
-      </c>
-      <c r="D140" s="2" t="s">
-        <v>452</v>
       </c>
     </row>
     <row r="141" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="B141" s="4" t="s">
         <v>453</v>
       </c>
-      <c r="B141" s="4" t="s">
+      <c r="D141" s="2" t="s">
         <v>454</v>
-      </c>
-      <c r="D141" s="2" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="142" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
+        <v>455</v>
+      </c>
+      <c r="B142" s="4" t="s">
+        <v>457</v>
+      </c>
+      <c r="C142" s="5" t="s">
         <v>456</v>
       </c>
-      <c r="B142" s="4" t="s">
+      <c r="D142" s="2" t="s">
         <v>458</v>
-      </c>
-      <c r="C142" s="5" t="s">
-        <v>457</v>
-      </c>
-      <c r="D142" s="2" t="s">
-        <v>459</v>
       </c>
     </row>
     <row r="143" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
+        <v>459</v>
+      </c>
+      <c r="B143" s="4" t="s">
         <v>460</v>
       </c>
-      <c r="B143" s="4" t="s">
+      <c r="D143" s="2" t="s">
         <v>461</v>
-      </c>
-      <c r="D143" s="2" t="s">
-        <v>462</v>
       </c>
     </row>
     <row r="144" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
+        <v>462</v>
+      </c>
+      <c r="B144" s="4" t="s">
+        <v>464</v>
+      </c>
+      <c r="C144" s="5" t="s">
         <v>463</v>
       </c>
-      <c r="B144" s="4" t="s">
+      <c r="D144" s="2" t="s">
         <v>465</v>
-      </c>
-      <c r="C144" s="5" t="s">
-        <v>464</v>
-      </c>
-      <c r="D144" s="2" t="s">
-        <v>466</v>
       </c>
     </row>
     <row r="145" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
+        <v>466</v>
+      </c>
+      <c r="B145" s="4" t="s">
         <v>467</v>
       </c>
-      <c r="B145" s="4" t="s">
+      <c r="C145" s="5" t="s">
         <v>468</v>
       </c>
-      <c r="C145" s="5" t="s">
+      <c r="D145" s="2" t="s">
         <v>469</v>
-      </c>
-      <c r="D145" s="2" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="146" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
+        <v>470</v>
+      </c>
+      <c r="B146" s="4" t="s">
         <v>471</v>
       </c>
-      <c r="B146" s="4" t="s">
+      <c r="D146" s="2" t="s">
         <v>472</v>
-      </c>
-      <c r="D146" s="2" t="s">
-        <v>473</v>
       </c>
     </row>
     <row r="147" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
+        <v>473</v>
+      </c>
+      <c r="B147" s="4" t="s">
         <v>474</v>
       </c>
-      <c r="B147" s="4" t="s">
+      <c r="C147" s="5" t="s">
         <v>475</v>
       </c>
-      <c r="C147" s="5" t="s">
+      <c r="D147" s="2" t="s">
         <v>476</v>
-      </c>
-      <c r="D147" s="2" t="s">
-        <v>477</v>
       </c>
     </row>
     <row r="148" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="s">
+        <v>477</v>
+      </c>
+      <c r="B148" s="4" t="s">
         <v>478</v>
       </c>
-      <c r="B148" s="4" t="s">
-        <v>479</v>
-      </c>
       <c r="D148" s="2" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="149" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Commit on 30.01.2019. Minor changes added to the excel file. Also removed the comments.
</commit_message>
<xml_diff>
--- a/Exam Preparation/resources/70-480 Practice Exam Answers and Explanations.xlsx
+++ b/Exam Preparation/resources/70-480 Practice Exam Answers and Explanations.xlsx
@@ -893,9 +893,6 @@
     <t>My answer is correct. Answer explanation: You should set the pattern attribute to a regular expression that allows relativeURLs.By default some browsers do not allow validation to succeed when relative URLs are entered in an input field where the type attribute is set to url.You can override this behavior by setting the pattern attribute.</t>
   </si>
   <si>
-    <t>70.You are using HTML5 to create a web page that allows users to submit data.You want to define an input field that must  meet the following requirements: *If the user enters a value the value must be a number between 0 and 96b. *The number must be divisible by  6</t>
-  </si>
-  <si>
     <t>&lt;input type="number" min="0" max="96" step="6"  /&gt;</t>
   </si>
   <si>
@@ -906,9 +903,6 @@
   </si>
   <si>
     <t>submit(this);</t>
-  </si>
-  <si>
-    <t>My answer is correct. Answer explanation: In a DOM event handler the "this" keyword refers to the DOC element that fired the event.</t>
   </si>
   <si>
     <t>72.The following code contains 4 different scopes:                                                                                                                                                                                                                     
@@ -940,9 +934,6 @@
         this.number = newNumber;
     };
 }</t>
-  </si>
-  <si>
-    <t>My answer is correct. Answer explanation: This code uses the "this" keyword to set the number and previousNumber variables to new values.This is necessary because the variables are initialized by using the "this" keyword.The "this" keyword allows you to scope a variable to the Fibonacci object.</t>
   </si>
   <si>
     <t>74.You need to determine the value of the number variable.</t>
@@ -1919,6 +1910,15 @@
     <t>85.The following markup exists on a web page:                                                                                                                                                 
     &lt;button&gt;Submit&lt;/button&gt;
     &lt;script&gt;$("button").click(function () {var data = $("form").serialize(); }); &lt;/script&gt; You need to determine the value of the data variable when the button is clicked.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>70.You are using HTML5 to create a web page that allows users to submit data.You want to define an input field that must  meet the following requirements: *If the user enters a value the value must be a number between 0 and 96. *The number must be divisible by  6</t>
+  </si>
+  <si>
+    <t>My answer is correct. Answer explanation: In a DOM event handler the "this" keyword refers to the DOM element that fired the event.</t>
   </si>
 </sst>
 </file>
@@ -2333,8 +2333,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D352"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B61" zoomScale="30" zoomScaleNormal="30" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView tabSelected="1" topLeftCell="B73" zoomScale="30" zoomScaleNormal="30" workbookViewId="0">
+      <selection activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="61.5" x14ac:dyDescent="0.25"/>
@@ -2372,7 +2372,7 @@
         <v>6</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2383,7 +2383,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>9</v>
@@ -2397,7 +2397,7 @@
         <v>11</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>12</v>
@@ -2410,13 +2410,13 @@
     </row>
     <row r="7" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2427,7 +2427,7 @@
         <v>16</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2438,12 +2438,12 @@
         <v>18</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>19</v>
@@ -2457,7 +2457,7 @@
     </row>
     <row r="11" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>22</v>
@@ -2577,7 +2577,7 @@
         <v>53</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="D20" s="9" t="s">
         <v>54</v>
@@ -2688,7 +2688,7 @@
         <v>83</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2743,7 +2743,7 @@
         <v>97</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2787,7 +2787,7 @@
         <v>108</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2998,7 +2998,7 @@
         <v>165</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3023,7 +3023,7 @@
         <v>170</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3114,7 +3114,7 @@
         <v>195</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D65" s="9" t="s">
         <v>196</v>
@@ -3205,925 +3205,925 @@
     </row>
     <row r="73" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
+        <v>487</v>
+      </c>
+      <c r="B73" s="7" t="s">
         <v>221</v>
       </c>
-      <c r="B73" s="7" t="s">
+      <c r="D73" s="9" t="s">
         <v>222</v>
-      </c>
-      <c r="D73" s="9" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="B74" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="B74" s="7" t="s">
-        <v>225</v>
-      </c>
       <c r="D74" s="9" t="s">
-        <v>226</v>
+        <v>488</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="C75" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="B75" s="7" t="s">
+      <c r="D75" s="9" t="s">
         <v>228</v>
-      </c>
-      <c r="C75" s="8" t="s">
-        <v>229</v>
-      </c>
-      <c r="D75" s="9" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>233</v>
+        <v>486</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B77" s="7">
         <v>12</v>
       </c>
       <c r="D77" s="9" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="C78" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="D78" s="9" t="s">
         <v>236</v>
-      </c>
-      <c r="B78" s="7" t="s">
-        <v>237</v>
-      </c>
-      <c r="C78" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="D78" s="9" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B79" s="7">
         <v>105</v>
       </c>
       <c r="D79" s="9" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="C80" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="D80" s="9" t="s">
         <v>242</v>
-      </c>
-      <c r="B80" s="7" t="s">
-        <v>244</v>
-      </c>
-      <c r="C80" s="8" t="s">
-        <v>243</v>
-      </c>
-      <c r="D80" s="9" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C81" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="D81" s="9" t="s">
         <v>246</v>
-      </c>
-      <c r="B81" s="7" t="s">
-        <v>247</v>
-      </c>
-      <c r="C81" s="8" t="s">
-        <v>248</v>
-      </c>
-      <c r="D81" s="9" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="D82" s="9" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="C83" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="D83" s="9" t="s">
         <v>253</v>
-      </c>
-      <c r="B83" s="7" t="s">
-        <v>254</v>
-      </c>
-      <c r="C83" s="8" t="s">
-        <v>255</v>
-      </c>
-      <c r="D83" s="9" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="B84" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="C84" s="8" t="s">
         <v>257</v>
       </c>
-      <c r="B84" s="7" t="s">
+      <c r="D84" s="9" t="s">
         <v>258</v>
-      </c>
-      <c r="C84" s="8" t="s">
-        <v>260</v>
-      </c>
-      <c r="D84" s="9" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="6" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="D85" s="9" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="B86" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="C86" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="D86" s="9" t="s">
         <v>265</v>
-      </c>
-      <c r="B86" s="7" t="s">
-        <v>266</v>
-      </c>
-      <c r="C86" s="8" t="s">
-        <v>267</v>
-      </c>
-      <c r="D86" s="9" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="B87" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="C87" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="D87" s="9" t="s">
         <v>269</v>
-      </c>
-      <c r="B87" s="7" t="s">
-        <v>270</v>
-      </c>
-      <c r="C87" s="8" t="s">
-        <v>271</v>
-      </c>
-      <c r="D87" s="9" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C88" s="8" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D88" s="9" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="6" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D89" s="9" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D90" s="9" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="6" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D91" s="9" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="B92" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="C92" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="D92" s="9" t="s">
         <v>285</v>
-      </c>
-      <c r="B92" s="7" t="s">
-        <v>286</v>
-      </c>
-      <c r="C92" s="8" t="s">
-        <v>287</v>
-      </c>
-      <c r="D92" s="9" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="B93" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="C93" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="D93" s="9" t="s">
         <v>289</v>
-      </c>
-      <c r="B93" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="C93" s="8" t="s">
-        <v>291</v>
-      </c>
-      <c r="D93" s="9" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="D94" s="9" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="6" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="D95" s="9" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="6" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="D96" s="9" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="6" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B97" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="C97" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="D97" s="9" t="s">
         <v>302</v>
-      </c>
-      <c r="C97" s="8" t="s">
-        <v>303</v>
-      </c>
-      <c r="D97" s="9" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="6" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D98" s="9" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="B99" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="C99" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="D99" s="9" t="s">
         <v>309</v>
-      </c>
-      <c r="B99" s="7" t="s">
-        <v>310</v>
-      </c>
-      <c r="C99" s="8" t="s">
-        <v>311</v>
-      </c>
-      <c r="D99" s="9" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="6" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="D100" s="9" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="6" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="D101" s="9" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="B102" s="7" t="s">
+        <v>317</v>
+      </c>
+      <c r="C102" s="8" t="s">
+        <v>318</v>
+      </c>
+      <c r="D102" s="9" t="s">
         <v>319</v>
-      </c>
-      <c r="B102" s="7" t="s">
-        <v>320</v>
-      </c>
-      <c r="C102" s="8" t="s">
-        <v>321</v>
-      </c>
-      <c r="D102" s="9" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="B103" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="C103" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="D103" s="9" t="s">
         <v>323</v>
-      </c>
-      <c r="B103" s="7" t="s">
-        <v>324</v>
-      </c>
-      <c r="C103" s="8" t="s">
-        <v>325</v>
-      </c>
-      <c r="D103" s="9" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="B104" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="C104" s="8" t="s">
+        <v>325</v>
+      </c>
+      <c r="D104" s="9" t="s">
         <v>327</v>
-      </c>
-      <c r="B104" s="7" t="s">
-        <v>329</v>
-      </c>
-      <c r="C104" s="8" t="s">
-        <v>328</v>
-      </c>
-      <c r="D104" s="9" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="6" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="D105" s="9" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="6" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="D106" s="9" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="6" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D107" s="9" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="6" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D108" s="9" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="6" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="D109" s="9" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="6" t="s">
+        <v>343</v>
+      </c>
+      <c r="B110" s="7" t="s">
+        <v>344</v>
+      </c>
+      <c r="C110" s="8" t="s">
+        <v>345</v>
+      </c>
+      <c r="D110" s="9" t="s">
         <v>346</v>
-      </c>
-      <c r="B110" s="7" t="s">
-        <v>347</v>
-      </c>
-      <c r="C110" s="8" t="s">
-        <v>348</v>
-      </c>
-      <c r="D110" s="9" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="6" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D111" s="9" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="6" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="B112" s="7" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="D112" s="9" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="6" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="B113" s="7" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="D113" s="9" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="6" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="B114" s="7" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D114" s="9" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="6" t="s">
+        <v>359</v>
+      </c>
+      <c r="B115" s="7" t="s">
+        <v>360</v>
+      </c>
+      <c r="C115" s="8" t="s">
+        <v>361</v>
+      </c>
+      <c r="D115" s="9" t="s">
         <v>362</v>
-      </c>
-      <c r="B115" s="7" t="s">
-        <v>363</v>
-      </c>
-      <c r="C115" s="8" t="s">
-        <v>364</v>
-      </c>
-      <c r="D115" s="9" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="6" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="B116" s="7" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="D116" s="9" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="6" t="s">
+        <v>366</v>
+      </c>
+      <c r="B117" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="C117" s="8" t="s">
+        <v>368</v>
+      </c>
+      <c r="D117" s="9" t="s">
         <v>369</v>
-      </c>
-      <c r="B117" s="7" t="s">
-        <v>370</v>
-      </c>
-      <c r="C117" s="8" t="s">
-        <v>371</v>
-      </c>
-      <c r="D117" s="9" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="6" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="D118" s="9" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="6" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="B119" s="7" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="D119" s="9" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="6" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="B120" s="7" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="D120" s="9" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
     </row>
     <row r="121" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="6" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="D121" s="9" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="122" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="6" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="B122" s="7" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="D122" s="9" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
     </row>
     <row r="123" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="6" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="B123" s="7" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D123" s="9" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="124" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="6" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="B124" s="7" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D124" s="9" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="125" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="6" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="B125" s="7" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="D125" s="9" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="6" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="B126" s="7" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="D126" s="9" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="6" t="s">
+        <v>396</v>
+      </c>
+      <c r="B127" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="C127" s="8" t="s">
+        <v>398</v>
+      </c>
+      <c r="D127" s="9" t="s">
         <v>399</v>
-      </c>
-      <c r="B127" s="7" t="s">
-        <v>400</v>
-      </c>
-      <c r="C127" s="8" t="s">
-        <v>401</v>
-      </c>
-      <c r="D127" s="9" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="6" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="B128" s="7" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="D128" s="9" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
     </row>
     <row r="129" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="6" t="s">
+        <v>403</v>
+      </c>
+      <c r="B129" s="7" t="s">
+        <v>404</v>
+      </c>
+      <c r="C129" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="D129" s="9" t="s">
         <v>406</v>
-      </c>
-      <c r="B129" s="7" t="s">
-        <v>407</v>
-      </c>
-      <c r="C129" s="8" t="s">
-        <v>408</v>
-      </c>
-      <c r="D129" s="9" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="130" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="6" t="s">
+        <v>407</v>
+      </c>
+      <c r="B130" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="C130" s="8" t="s">
+        <v>409</v>
+      </c>
+      <c r="D130" s="9" t="s">
         <v>410</v>
-      </c>
-      <c r="B130" s="7" t="s">
-        <v>411</v>
-      </c>
-      <c r="C130" s="8" t="s">
-        <v>412</v>
-      </c>
-      <c r="D130" s="9" t="s">
-        <v>413</v>
       </c>
     </row>
     <row r="131" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="6" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="B131" s="7" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="D131" s="9" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
     </row>
     <row r="132" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="6" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="B132" s="7" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="D132" s="9" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="133" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="6" t="s">
+        <v>417</v>
+      </c>
+      <c r="B133" s="7" t="s">
+        <v>418</v>
+      </c>
+      <c r="C133" s="8" t="s">
+        <v>419</v>
+      </c>
+      <c r="D133" s="9" t="s">
         <v>420</v>
-      </c>
-      <c r="B133" s="7" t="s">
-        <v>421</v>
-      </c>
-      <c r="C133" s="8" t="s">
-        <v>422</v>
-      </c>
-      <c r="D133" s="9" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="134" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="6" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="B134" s="7" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="D134" s="9" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
     </row>
     <row r="135" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="6" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="B135" s="7" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="D135" s="9" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
     </row>
     <row r="136" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="6" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="B136" s="7" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="D136" s="9" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="6" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="B137" s="7" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="D137" s="9" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
     </row>
     <row r="138" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="B138" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="C138" s="8" t="s">
+        <v>435</v>
+      </c>
+      <c r="D138" s="9" t="s">
         <v>436</v>
-      </c>
-      <c r="B138" s="7" t="s">
-        <v>437</v>
-      </c>
-      <c r="C138" s="8" t="s">
-        <v>438</v>
-      </c>
-      <c r="D138" s="9" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="139" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="6" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="B139" s="7" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="D139" s="9" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
     </row>
     <row r="140" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="6" t="s">
+        <v>440</v>
+      </c>
+      <c r="B140" s="7" t="s">
+        <v>441</v>
+      </c>
+      <c r="C140" s="8" t="s">
+        <v>442</v>
+      </c>
+      <c r="D140" s="9" t="s">
         <v>443</v>
-      </c>
-      <c r="B140" s="7" t="s">
-        <v>444</v>
-      </c>
-      <c r="C140" s="8" t="s">
-        <v>445</v>
-      </c>
-      <c r="D140" s="9" t="s">
-        <v>446</v>
       </c>
     </row>
     <row r="141" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="6" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="B141" s="7" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="D141" s="9" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
     </row>
     <row r="142" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="6" t="s">
+        <v>447</v>
+      </c>
+      <c r="B142" s="7" t="s">
+        <v>449</v>
+      </c>
+      <c r="C142" s="8" t="s">
+        <v>448</v>
+      </c>
+      <c r="D142" s="9" t="s">
         <v>450</v>
-      </c>
-      <c r="B142" s="7" t="s">
-        <v>452</v>
-      </c>
-      <c r="C142" s="8" t="s">
-        <v>451</v>
-      </c>
-      <c r="D142" s="9" t="s">
-        <v>453</v>
       </c>
     </row>
     <row r="143" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="6" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="B143" s="7" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="D143" s="9" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="144" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="6" t="s">
+        <v>454</v>
+      </c>
+      <c r="B144" s="7" t="s">
+        <v>456</v>
+      </c>
+      <c r="C144" s="8" t="s">
+        <v>455</v>
+      </c>
+      <c r="D144" s="9" t="s">
         <v>457</v>
-      </c>
-      <c r="B144" s="7" t="s">
-        <v>459</v>
-      </c>
-      <c r="C144" s="8" t="s">
-        <v>458</v>
-      </c>
-      <c r="D144" s="9" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="145" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="6" t="s">
+        <v>458</v>
+      </c>
+      <c r="B145" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="C145" s="8" t="s">
+        <v>460</v>
+      </c>
+      <c r="D145" s="9" t="s">
         <v>461</v>
-      </c>
-      <c r="B145" s="7" t="s">
-        <v>462</v>
-      </c>
-      <c r="C145" s="8" t="s">
-        <v>463</v>
-      </c>
-      <c r="D145" s="9" t="s">
-        <v>464</v>
       </c>
     </row>
     <row r="146" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="6" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="B146" s="7" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="D146" s="9" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
     </row>
     <row r="147" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="6" t="s">
+        <v>465</v>
+      </c>
+      <c r="B147" s="7" t="s">
+        <v>466</v>
+      </c>
+      <c r="C147" s="8" t="s">
+        <v>467</v>
+      </c>
+      <c r="D147" s="9" t="s">
         <v>468</v>
-      </c>
-      <c r="B147" s="7" t="s">
-        <v>469</v>
-      </c>
-      <c r="C147" s="8" t="s">
-        <v>470</v>
-      </c>
-      <c r="D147" s="9" t="s">
-        <v>471</v>
       </c>
     </row>
     <row r="148" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="6" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="B148" s="7" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="D148" s="9" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
     </row>
     <row r="149" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>